<commit_message>
Arquivos e planilha atualizados.
</commit_message>
<xml_diff>
--- a/arquivos-tradutor.xlsx
+++ b/arquivos-tradutor.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\danger\traducoes\traducao-blue-dragon-xbox360\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Moacyr\Desktop\GITHUB-BD\traducao-blue-dragon-xbox360\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1565" uniqueCount="785">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1631" uniqueCount="787">
   <si>
     <t>Arquivo</t>
   </si>
@@ -2379,6 +2379,12 @@
   </si>
   <si>
     <t>Não</t>
+  </si>
+  <si>
+    <t>UDS</t>
+  </si>
+  <si>
+    <t>SIM</t>
   </si>
 </sst>
 </file>
@@ -2722,7 +2728,7 @@
   <dimension ref="B1:D782"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="C322" sqref="C322"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2748,7 +2754,10 @@
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>785</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
@@ -2756,7 +2765,10 @@
         <v>2</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>785</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
@@ -2764,7 +2776,10 @@
         <v>3</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>785</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
@@ -2772,7 +2787,10 @@
         <v>4</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>785</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
@@ -2780,7 +2798,10 @@
         <v>5</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>785</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
@@ -2788,7 +2809,10 @@
         <v>6</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>785</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.25">
@@ -2796,7 +2820,10 @@
         <v>7</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>785</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.25">
@@ -5167,7 +5194,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="305" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="305" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B305" s="1" t="s">
         <v>304</v>
       </c>
@@ -5175,7 +5202,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="306" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="306" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B306" s="1" t="s">
         <v>305</v>
       </c>
@@ -5183,7 +5210,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="307" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="307" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B307" s="1" t="s">
         <v>306</v>
       </c>
@@ -5191,7 +5218,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="308" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="308" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B308" s="1" t="s">
         <v>307</v>
       </c>
@@ -5199,7 +5226,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="309" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="309" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B309" s="1" t="s">
         <v>308</v>
       </c>
@@ -5207,7 +5234,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="310" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="310" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B310" s="1" t="s">
         <v>309</v>
       </c>
@@ -5215,7 +5242,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="311" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="311" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B311" s="1" t="s">
         <v>310</v>
       </c>
@@ -5223,55 +5250,73 @@
         <v>784</v>
       </c>
     </row>
-    <row r="312" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="312" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B312" s="1" t="s">
         <v>311</v>
       </c>
       <c r="C312" s="1" t="s">
-        <v>784</v>
-      </c>
-    </row>
-    <row r="313" spans="2:3" x14ac:dyDescent="0.25">
+        <v>786</v>
+      </c>
+      <c r="D312" s="1" t="s">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="313" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B313" s="1" t="s">
         <v>312</v>
       </c>
       <c r="C313" s="1" t="s">
-        <v>784</v>
-      </c>
-    </row>
-    <row r="314" spans="2:3" x14ac:dyDescent="0.25">
+        <v>786</v>
+      </c>
+      <c r="D313" s="1" t="s">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="314" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B314" s="1" t="s">
         <v>313</v>
       </c>
       <c r="C314" s="1" t="s">
-        <v>784</v>
-      </c>
-    </row>
-    <row r="315" spans="2:3" x14ac:dyDescent="0.25">
+        <v>786</v>
+      </c>
+      <c r="D314" s="1" t="s">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="315" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B315" s="1" t="s">
         <v>314</v>
       </c>
       <c r="C315" s="1" t="s">
-        <v>784</v>
-      </c>
-    </row>
-    <row r="316" spans="2:3" x14ac:dyDescent="0.25">
+        <v>786</v>
+      </c>
+      <c r="D315" s="1" t="s">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="316" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B316" s="1" t="s">
         <v>315</v>
       </c>
       <c r="C316" s="1" t="s">
-        <v>784</v>
-      </c>
-    </row>
-    <row r="317" spans="2:3" x14ac:dyDescent="0.25">
+        <v>786</v>
+      </c>
+      <c r="D316" s="1" t="s">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="317" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B317" s="1" t="s">
         <v>316</v>
       </c>
       <c r="C317" s="1" t="s">
-        <v>784</v>
-      </c>
-    </row>
-    <row r="318" spans="2:3" x14ac:dyDescent="0.25">
+        <v>786</v>
+      </c>
+      <c r="D317" s="1" t="s">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="318" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B318" s="1" t="s">
         <v>317</v>
       </c>
@@ -5279,15 +5324,18 @@
         <v>784</v>
       </c>
     </row>
-    <row r="319" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="319" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B319" s="1" t="s">
         <v>318</v>
       </c>
       <c r="C319" s="1" t="s">
-        <v>784</v>
-      </c>
-    </row>
-    <row r="320" spans="2:3" x14ac:dyDescent="0.25">
+        <v>786</v>
+      </c>
+      <c r="D319" s="1" t="s">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="320" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B320" s="1" t="s">
         <v>319</v>
       </c>
@@ -5295,7 +5343,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="321" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="321" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B321" s="1" t="s">
         <v>320</v>
       </c>
@@ -5303,7 +5351,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="322" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="322" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B322" s="1" t="s">
         <v>321</v>
       </c>
@@ -5311,7 +5359,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="323" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="323" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B323" s="1" t="s">
         <v>322</v>
       </c>
@@ -5319,7 +5367,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="324" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="324" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B324" s="1" t="s">
         <v>323</v>
       </c>
@@ -5327,15 +5375,18 @@
         <v>784</v>
       </c>
     </row>
-    <row r="325" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="325" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B325" s="1" t="s">
         <v>324</v>
       </c>
       <c r="C325" s="1" t="s">
-        <v>784</v>
-      </c>
-    </row>
-    <row r="326" spans="2:3" x14ac:dyDescent="0.25">
+        <v>786</v>
+      </c>
+      <c r="D325" s="1" t="s">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="326" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B326" s="1" t="s">
         <v>325</v>
       </c>
@@ -5343,7 +5394,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="327" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="327" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B327" s="1" t="s">
         <v>326</v>
       </c>
@@ -5351,7 +5402,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="328" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="328" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B328" s="1" t="s">
         <v>327</v>
       </c>
@@ -5359,7 +5410,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="329" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="329" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B329" s="1" t="s">
         <v>328</v>
       </c>
@@ -5367,7 +5418,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="330" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="330" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B330" s="1" t="s">
         <v>329</v>
       </c>
@@ -5375,7 +5426,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="331" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="331" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B331" s="1" t="s">
         <v>330</v>
       </c>
@@ -5383,7 +5434,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="332" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="332" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B332" s="1" t="s">
         <v>331</v>
       </c>
@@ -5391,7 +5442,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="333" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="333" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B333" s="1" t="s">
         <v>332</v>
       </c>
@@ -5399,7 +5450,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="334" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="334" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B334" s="1" t="s">
         <v>333</v>
       </c>
@@ -5407,7 +5458,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="335" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="335" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B335" s="1" t="s">
         <v>334</v>
       </c>
@@ -5415,15 +5466,18 @@
         <v>784</v>
       </c>
     </row>
-    <row r="336" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="336" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B336" s="1" t="s">
         <v>335</v>
       </c>
       <c r="C336" s="1" t="s">
-        <v>784</v>
-      </c>
-    </row>
-    <row r="337" spans="2:3" x14ac:dyDescent="0.25">
+        <v>786</v>
+      </c>
+      <c r="D336" s="1" t="s">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="337" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B337" s="1" t="s">
         <v>336</v>
       </c>
@@ -5431,15 +5485,18 @@
         <v>784</v>
       </c>
     </row>
-    <row r="338" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="338" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B338" s="1" t="s">
         <v>337</v>
       </c>
       <c r="C338" s="1" t="s">
-        <v>784</v>
-      </c>
-    </row>
-    <row r="339" spans="2:3" x14ac:dyDescent="0.25">
+        <v>786</v>
+      </c>
+      <c r="D338" s="1" t="s">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="339" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B339" s="1" t="s">
         <v>338</v>
       </c>
@@ -5447,7 +5504,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="340" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="340" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B340" s="1" t="s">
         <v>339</v>
       </c>
@@ -5455,7 +5512,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="341" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="341" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B341" s="1" t="s">
         <v>340</v>
       </c>
@@ -5463,7 +5520,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="342" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="342" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B342" s="1" t="s">
         <v>341</v>
       </c>
@@ -5471,7 +5528,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="343" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="343" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B343" s="1" t="s">
         <v>342</v>
       </c>
@@ -5479,15 +5536,18 @@
         <v>784</v>
       </c>
     </row>
-    <row r="344" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="344" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B344" s="1" t="s">
         <v>343</v>
       </c>
       <c r="C344" s="1" t="s">
-        <v>784</v>
-      </c>
-    </row>
-    <row r="345" spans="2:3" x14ac:dyDescent="0.25">
+        <v>786</v>
+      </c>
+      <c r="D344" s="1" t="s">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="345" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B345" s="1" t="s">
         <v>344</v>
       </c>
@@ -5495,7 +5555,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="346" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="346" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B346" s="1" t="s">
         <v>345</v>
       </c>
@@ -5503,7 +5563,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="347" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="347" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B347" s="1" t="s">
         <v>346</v>
       </c>
@@ -5511,7 +5571,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="348" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="348" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B348" s="1" t="s">
         <v>347</v>
       </c>
@@ -5519,7 +5579,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="349" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="349" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B349" s="1" t="s">
         <v>348</v>
       </c>
@@ -5527,7 +5587,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="350" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="350" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B350" s="1" t="s">
         <v>349</v>
       </c>
@@ -5535,15 +5595,18 @@
         <v>784</v>
       </c>
     </row>
-    <row r="351" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="351" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B351" s="1" t="s">
         <v>350</v>
       </c>
       <c r="C351" s="1" t="s">
-        <v>784</v>
-      </c>
-    </row>
-    <row r="352" spans="2:3" x14ac:dyDescent="0.25">
+        <v>786</v>
+      </c>
+      <c r="D351" s="1" t="s">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="352" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B352" s="1" t="s">
         <v>351</v>
       </c>
@@ -5551,7 +5614,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="353" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="353" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B353" s="1" t="s">
         <v>352</v>
       </c>
@@ -5559,7 +5622,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="354" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="354" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B354" s="1" t="s">
         <v>353</v>
       </c>
@@ -5567,15 +5630,18 @@
         <v>784</v>
       </c>
     </row>
-    <row r="355" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="355" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B355" s="1" t="s">
         <v>354</v>
       </c>
       <c r="C355" s="1" t="s">
-        <v>784</v>
-      </c>
-    </row>
-    <row r="356" spans="2:3" x14ac:dyDescent="0.25">
+        <v>786</v>
+      </c>
+      <c r="D355" s="1" t="s">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="356" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B356" s="1" t="s">
         <v>355</v>
       </c>
@@ -5583,7 +5649,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="357" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="357" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B357" s="1" t="s">
         <v>356</v>
       </c>
@@ -5591,15 +5657,18 @@
         <v>784</v>
       </c>
     </row>
-    <row r="358" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="358" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B358" s="1" t="s">
         <v>357</v>
       </c>
       <c r="C358" s="1" t="s">
-        <v>784</v>
-      </c>
-    </row>
-    <row r="359" spans="2:3" x14ac:dyDescent="0.25">
+        <v>786</v>
+      </c>
+      <c r="D358" s="1" t="s">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="359" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B359" s="1" t="s">
         <v>358</v>
       </c>
@@ -5607,7 +5676,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="360" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="360" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B360" s="1" t="s">
         <v>359</v>
       </c>
@@ -5615,7 +5684,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="361" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="361" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B361" s="1" t="s">
         <v>360</v>
       </c>
@@ -5623,7 +5692,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="362" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="362" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B362" s="1" t="s">
         <v>361</v>
       </c>
@@ -5631,7 +5700,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="363" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="363" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B363" s="1" t="s">
         <v>362</v>
       </c>
@@ -5639,7 +5708,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="364" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="364" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B364" s="1" t="s">
         <v>363</v>
       </c>
@@ -5647,7 +5716,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="365" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="365" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B365" s="1" t="s">
         <v>364</v>
       </c>
@@ -5655,7 +5724,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="366" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="366" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B366" s="1" t="s">
         <v>365</v>
       </c>
@@ -5663,7 +5732,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="367" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="367" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B367" s="1" t="s">
         <v>366</v>
       </c>
@@ -5671,7 +5740,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="368" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="368" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B368" s="1" t="s">
         <v>367</v>
       </c>
@@ -5935,7 +6004,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="401" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="401" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B401" s="1" t="s">
         <v>400</v>
       </c>
@@ -5943,15 +6012,18 @@
         <v>784</v>
       </c>
     </row>
-    <row r="402" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="402" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B402" s="1" t="s">
         <v>401</v>
       </c>
       <c r="C402" s="1" t="s">
-        <v>784</v>
-      </c>
-    </row>
-    <row r="403" spans="2:3" x14ac:dyDescent="0.25">
+        <v>786</v>
+      </c>
+      <c r="D402" s="1" t="s">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="403" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B403" s="1" t="s">
         <v>402</v>
       </c>
@@ -5959,7 +6031,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="404" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="404" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B404" s="1" t="s">
         <v>403</v>
       </c>
@@ -5967,7 +6039,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="405" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="405" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B405" s="1" t="s">
         <v>404</v>
       </c>
@@ -5975,7 +6047,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="406" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="406" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B406" s="1" t="s">
         <v>405</v>
       </c>
@@ -5983,7 +6055,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="407" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="407" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B407" s="1" t="s">
         <v>406</v>
       </c>
@@ -5991,7 +6063,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="408" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="408" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B408" s="1" t="s">
         <v>407</v>
       </c>
@@ -5999,7 +6071,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="409" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="409" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B409" s="1" t="s">
         <v>408</v>
       </c>
@@ -6007,7 +6079,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="410" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="410" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B410" s="1" t="s">
         <v>409</v>
       </c>
@@ -6015,7 +6087,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="411" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="411" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B411" s="1" t="s">
         <v>410</v>
       </c>
@@ -6023,7 +6095,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="412" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="412" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B412" s="1" t="s">
         <v>411</v>
       </c>
@@ -6031,7 +6103,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="413" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="413" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B413" s="1" t="s">
         <v>412</v>
       </c>
@@ -6039,7 +6111,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="414" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="414" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B414" s="1" t="s">
         <v>413</v>
       </c>
@@ -6047,31 +6119,40 @@
         <v>784</v>
       </c>
     </row>
-    <row r="415" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="415" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B415" s="1" t="s">
         <v>414</v>
       </c>
       <c r="C415" s="1" t="s">
-        <v>784</v>
-      </c>
-    </row>
-    <row r="416" spans="2:3" x14ac:dyDescent="0.25">
+        <v>786</v>
+      </c>
+      <c r="D415" s="1" t="s">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="416" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B416" s="1" t="s">
         <v>415</v>
       </c>
       <c r="C416" s="1" t="s">
-        <v>784</v>
-      </c>
-    </row>
-    <row r="417" spans="2:3" x14ac:dyDescent="0.25">
+        <v>786</v>
+      </c>
+      <c r="D416" s="1" t="s">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="417" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B417" s="1" t="s">
         <v>416</v>
       </c>
       <c r="C417" s="1" t="s">
-        <v>784</v>
-      </c>
-    </row>
-    <row r="418" spans="2:3" x14ac:dyDescent="0.25">
+        <v>786</v>
+      </c>
+      <c r="D417" s="1" t="s">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="418" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B418" s="1" t="s">
         <v>417</v>
       </c>
@@ -6079,7 +6160,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="419" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="419" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B419" s="1" t="s">
         <v>418</v>
       </c>
@@ -6087,7 +6168,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="420" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="420" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B420" s="1" t="s">
         <v>419</v>
       </c>
@@ -6095,15 +6176,18 @@
         <v>784</v>
       </c>
     </row>
-    <row r="421" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="421" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B421" s="1" t="s">
         <v>420</v>
       </c>
       <c r="C421" s="1" t="s">
-        <v>784</v>
-      </c>
-    </row>
-    <row r="422" spans="2:3" x14ac:dyDescent="0.25">
+        <v>786</v>
+      </c>
+      <c r="D421" s="1" t="s">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="422" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B422" s="1" t="s">
         <v>421</v>
       </c>
@@ -6111,7 +6195,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="423" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="423" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B423" s="1" t="s">
         <v>422</v>
       </c>
@@ -6119,7 +6203,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="424" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="424" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B424" s="1" t="s">
         <v>423</v>
       </c>
@@ -6127,15 +6211,18 @@
         <v>784</v>
       </c>
     </row>
-    <row r="425" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="425" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B425" s="1" t="s">
         <v>424</v>
       </c>
       <c r="C425" s="1" t="s">
-        <v>784</v>
-      </c>
-    </row>
-    <row r="426" spans="2:3" x14ac:dyDescent="0.25">
+        <v>786</v>
+      </c>
+      <c r="D425" s="1" t="s">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="426" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B426" s="1" t="s">
         <v>425</v>
       </c>
@@ -6143,7 +6230,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="427" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="427" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B427" s="1" t="s">
         <v>426</v>
       </c>
@@ -6151,7 +6238,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="428" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="428" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B428" s="1" t="s">
         <v>427</v>
       </c>
@@ -6159,7 +6246,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="429" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="429" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B429" s="1" t="s">
         <v>428</v>
       </c>
@@ -6167,7 +6254,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="430" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="430" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B430" s="1" t="s">
         <v>429</v>
       </c>
@@ -6175,7 +6262,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="431" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="431" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B431" s="1" t="s">
         <v>430</v>
       </c>
@@ -6183,7 +6270,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="432" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="432" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B432" s="1" t="s">
         <v>431</v>
       </c>
@@ -6191,15 +6278,18 @@
         <v>784</v>
       </c>
     </row>
-    <row r="433" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="433" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B433" s="1" t="s">
         <v>432</v>
       </c>
       <c r="C433" s="1" t="s">
-        <v>784</v>
-      </c>
-    </row>
-    <row r="434" spans="2:3" x14ac:dyDescent="0.25">
+        <v>786</v>
+      </c>
+      <c r="D433" s="1" t="s">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="434" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B434" s="1" t="s">
         <v>433</v>
       </c>
@@ -6207,7 +6297,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="435" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="435" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B435" s="1" t="s">
         <v>434</v>
       </c>
@@ -6215,7 +6305,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="436" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="436" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B436" s="1" t="s">
         <v>435</v>
       </c>
@@ -6223,7 +6313,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="437" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="437" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B437" s="1" t="s">
         <v>436</v>
       </c>
@@ -6231,15 +6321,18 @@
         <v>784</v>
       </c>
     </row>
-    <row r="438" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="438" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B438" s="1" t="s">
         <v>437</v>
       </c>
       <c r="C438" s="1" t="s">
-        <v>784</v>
-      </c>
-    </row>
-    <row r="439" spans="2:3" x14ac:dyDescent="0.25">
+        <v>786</v>
+      </c>
+      <c r="D438" s="1" t="s">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="439" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B439" s="1" t="s">
         <v>438</v>
       </c>
@@ -6247,7 +6340,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="440" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="440" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B440" s="1" t="s">
         <v>439</v>
       </c>
@@ -6255,7 +6348,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="441" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="441" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B441" s="1" t="s">
         <v>440</v>
       </c>
@@ -6263,7 +6356,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="442" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="442" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B442" s="1" t="s">
         <v>441</v>
       </c>
@@ -6271,7 +6364,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="443" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="443" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B443" s="1" t="s">
         <v>442</v>
       </c>
@@ -6279,15 +6372,18 @@
         <v>784</v>
       </c>
     </row>
-    <row r="444" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="444" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B444" s="1" t="s">
         <v>443</v>
       </c>
       <c r="C444" s="1" t="s">
-        <v>784</v>
-      </c>
-    </row>
-    <row r="445" spans="2:3" x14ac:dyDescent="0.25">
+        <v>786</v>
+      </c>
+      <c r="D444" s="1" t="s">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="445" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B445" s="1" t="s">
         <v>444</v>
       </c>
@@ -6295,7 +6391,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="446" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="446" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B446" s="1" t="s">
         <v>445</v>
       </c>
@@ -6303,7 +6399,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="447" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="447" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B447" s="1" t="s">
         <v>446</v>
       </c>
@@ -6311,7 +6407,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="448" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="448" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B448" s="1" t="s">
         <v>447</v>
       </c>
@@ -6319,7 +6415,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="449" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="449" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B449" s="1" t="s">
         <v>448</v>
       </c>
@@ -6327,7 +6423,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="450" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="450" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B450" s="1" t="s">
         <v>449</v>
       </c>
@@ -6335,15 +6431,18 @@
         <v>784</v>
       </c>
     </row>
-    <row r="451" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="451" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B451" s="1" t="s">
         <v>450</v>
       </c>
       <c r="C451" s="1" t="s">
-        <v>784</v>
-      </c>
-    </row>
-    <row r="452" spans="2:3" x14ac:dyDescent="0.25">
+        <v>786</v>
+      </c>
+      <c r="D451" s="1" t="s">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="452" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B452" s="1" t="s">
         <v>451</v>
       </c>
@@ -6351,23 +6450,29 @@
         <v>784</v>
       </c>
     </row>
-    <row r="453" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="453" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B453" s="1" t="s">
         <v>452</v>
       </c>
       <c r="C453" s="1" t="s">
-        <v>784</v>
-      </c>
-    </row>
-    <row r="454" spans="2:3" x14ac:dyDescent="0.25">
+        <v>786</v>
+      </c>
+      <c r="D453" s="1" t="s">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="454" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B454" s="1" t="s">
         <v>453</v>
       </c>
       <c r="C454" s="1" t="s">
-        <v>784</v>
-      </c>
-    </row>
-    <row r="455" spans="2:3" x14ac:dyDescent="0.25">
+        <v>786</v>
+      </c>
+      <c r="D454" s="1" t="s">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="455" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B455" s="1" t="s">
         <v>454</v>
       </c>
@@ -6375,7 +6480,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="456" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="456" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B456" s="1" t="s">
         <v>455</v>
       </c>
@@ -6383,15 +6488,18 @@
         <v>784</v>
       </c>
     </row>
-    <row r="457" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="457" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B457" s="1" t="s">
         <v>456</v>
       </c>
       <c r="C457" s="1" t="s">
-        <v>784</v>
-      </c>
-    </row>
-    <row r="458" spans="2:3" x14ac:dyDescent="0.25">
+        <v>786</v>
+      </c>
+      <c r="D457" s="1" t="s">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="458" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B458" s="1" t="s">
         <v>457</v>
       </c>
@@ -6399,7 +6507,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="459" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="459" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B459" s="1" t="s">
         <v>458</v>
       </c>
@@ -6407,7 +6515,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="460" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="460" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B460" s="1" t="s">
         <v>459</v>
       </c>
@@ -6415,7 +6523,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="461" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="461" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B461" s="1" t="s">
         <v>460</v>
       </c>
@@ -6423,7 +6531,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="462" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="462" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B462" s="1" t="s">
         <v>461</v>
       </c>
@@ -6431,7 +6539,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="463" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="463" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B463" s="1" t="s">
         <v>462</v>
       </c>
@@ -6439,7 +6547,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="464" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="464" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B464" s="1" t="s">
         <v>463</v>
       </c>
@@ -6447,7 +6555,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="465" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="465" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B465" s="1" t="s">
         <v>464</v>
       </c>
@@ -6455,7 +6563,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="466" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="466" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B466" s="1" t="s">
         <v>465</v>
       </c>
@@ -6463,7 +6571,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="467" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="467" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B467" s="1" t="s">
         <v>466</v>
       </c>
@@ -6471,7 +6579,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="468" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="468" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B468" s="1" t="s">
         <v>467</v>
       </c>
@@ -6479,7 +6587,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="469" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="469" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B469" s="1" t="s">
         <v>468</v>
       </c>
@@ -6487,7 +6595,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="470" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="470" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B470" s="1" t="s">
         <v>469</v>
       </c>
@@ -6495,7 +6603,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="471" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="471" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B471" s="1" t="s">
         <v>470</v>
       </c>
@@ -6503,7 +6611,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="472" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="472" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B472" s="1" t="s">
         <v>471</v>
       </c>
@@ -6511,7 +6619,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="473" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="473" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B473" s="1" t="s">
         <v>472</v>
       </c>
@@ -6519,7 +6627,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="474" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="474" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B474" s="1" t="s">
         <v>473</v>
       </c>
@@ -6527,7 +6635,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="475" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="475" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B475" s="1" t="s">
         <v>474</v>
       </c>
@@ -6535,7 +6643,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="476" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="476" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B476" s="1" t="s">
         <v>475</v>
       </c>
@@ -6543,7 +6651,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="477" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="477" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B477" s="1" t="s">
         <v>476</v>
       </c>
@@ -6551,15 +6659,18 @@
         <v>784</v>
       </c>
     </row>
-    <row r="478" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="478" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B478" s="1" t="s">
         <v>477</v>
       </c>
       <c r="C478" s="1" t="s">
-        <v>784</v>
-      </c>
-    </row>
-    <row r="479" spans="2:3" x14ac:dyDescent="0.25">
+        <v>786</v>
+      </c>
+      <c r="D478" s="1" t="s">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="479" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B479" s="1" t="s">
         <v>478</v>
       </c>
@@ -6567,7 +6678,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="480" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="480" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B480" s="1" t="s">
         <v>479</v>
       </c>
@@ -6575,7 +6686,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="481" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="481" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B481" s="1" t="s">
         <v>480</v>
       </c>
@@ -6583,7 +6694,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="482" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="482" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B482" s="1" t="s">
         <v>481</v>
       </c>
@@ -6591,7 +6702,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="483" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="483" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B483" s="1" t="s">
         <v>482</v>
       </c>
@@ -6599,7 +6710,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="484" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="484" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B484" s="1" t="s">
         <v>483</v>
       </c>
@@ -6607,15 +6718,18 @@
         <v>784</v>
       </c>
     </row>
-    <row r="485" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="485" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B485" s="1" t="s">
         <v>484</v>
       </c>
       <c r="C485" s="1" t="s">
-        <v>784</v>
-      </c>
-    </row>
-    <row r="486" spans="2:3" x14ac:dyDescent="0.25">
+        <v>786</v>
+      </c>
+      <c r="D485" s="1" t="s">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="486" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B486" s="1" t="s">
         <v>485</v>
       </c>
@@ -6623,7 +6737,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="487" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="487" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B487" s="1" t="s">
         <v>486</v>
       </c>
@@ -6631,7 +6745,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="488" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="488" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B488" s="1" t="s">
         <v>487</v>
       </c>
@@ -6639,7 +6753,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="489" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="489" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B489" s="1" t="s">
         <v>488</v>
       </c>
@@ -6647,7 +6761,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="490" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="490" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B490" s="1" t="s">
         <v>489</v>
       </c>
@@ -6655,7 +6769,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="491" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="491" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B491" s="1" t="s">
         <v>490</v>
       </c>
@@ -6663,7 +6777,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="492" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="492" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B492" s="1" t="s">
         <v>491</v>
       </c>
@@ -6671,7 +6785,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="493" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="493" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B493" s="1" t="s">
         <v>492</v>
       </c>
@@ -6679,7 +6793,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="494" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="494" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B494" s="1" t="s">
         <v>493</v>
       </c>
@@ -6687,7 +6801,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="495" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="495" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B495" s="1" t="s">
         <v>494</v>
       </c>
@@ -6695,7 +6809,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="496" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="496" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B496" s="1" t="s">
         <v>495</v>
       </c>
@@ -6703,7 +6817,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="497" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="497" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B497" s="1" t="s">
         <v>496</v>
       </c>
@@ -6711,7 +6825,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="498" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="498" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B498" s="1" t="s">
         <v>497</v>
       </c>
@@ -6719,7 +6833,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="499" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="499" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B499" s="1" t="s">
         <v>498</v>
       </c>
@@ -6727,7 +6841,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="500" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="500" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B500" s="1" t="s">
         <v>499</v>
       </c>
@@ -6735,15 +6849,18 @@
         <v>784</v>
       </c>
     </row>
-    <row r="501" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="501" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B501" s="1" t="s">
         <v>500</v>
       </c>
       <c r="C501" s="1" t="s">
-        <v>784</v>
-      </c>
-    </row>
-    <row r="502" spans="2:3" x14ac:dyDescent="0.25">
+        <v>786</v>
+      </c>
+      <c r="D501" s="1" t="s">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="502" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B502" s="1" t="s">
         <v>501</v>
       </c>
@@ -6751,7 +6868,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="503" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="503" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B503" s="1" t="s">
         <v>502</v>
       </c>
@@ -6759,15 +6876,18 @@
         <v>784</v>
       </c>
     </row>
-    <row r="504" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="504" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B504" s="1" t="s">
         <v>503</v>
       </c>
       <c r="C504" s="1" t="s">
-        <v>784</v>
-      </c>
-    </row>
-    <row r="505" spans="2:3" x14ac:dyDescent="0.25">
+        <v>786</v>
+      </c>
+      <c r="D504" s="1" t="s">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="505" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B505" s="1" t="s">
         <v>504</v>
       </c>
@@ -6775,7 +6895,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="506" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="506" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B506" s="1" t="s">
         <v>505</v>
       </c>
@@ -6783,7 +6903,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="507" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="507" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B507" s="1" t="s">
         <v>506</v>
       </c>
@@ -6791,7 +6911,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="508" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="508" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B508" s="1" t="s">
         <v>507</v>
       </c>
@@ -6799,7 +6919,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="509" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="509" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B509" s="1" t="s">
         <v>508</v>
       </c>
@@ -6807,7 +6927,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="510" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="510" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B510" s="1" t="s">
         <v>509</v>
       </c>
@@ -6815,7 +6935,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="511" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="511" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B511" s="1" t="s">
         <v>510</v>
       </c>
@@ -6823,7 +6943,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="512" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="512" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B512" s="1" t="s">
         <v>511</v>
       </c>
@@ -6831,7 +6951,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="513" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="513" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B513" s="1" t="s">
         <v>512</v>
       </c>
@@ -6839,7 +6959,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="514" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="514" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B514" s="1" t="s">
         <v>513</v>
       </c>
@@ -6847,7 +6967,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="515" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="515" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B515" s="1" t="s">
         <v>514</v>
       </c>
@@ -6855,7 +6975,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="516" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="516" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B516" s="1" t="s">
         <v>515</v>
       </c>
@@ -6863,7 +6983,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="517" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="517" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B517" s="1" t="s">
         <v>516</v>
       </c>
@@ -6871,7 +6991,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="518" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="518" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B518" s="1" t="s">
         <v>517</v>
       </c>
@@ -6879,7 +6999,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="519" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="519" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B519" s="1" t="s">
         <v>518</v>
       </c>
@@ -6887,7 +7007,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="520" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="520" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B520" s="1" t="s">
         <v>519</v>
       </c>
@@ -6895,7 +7015,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="521" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="521" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B521" s="1" t="s">
         <v>520</v>
       </c>
@@ -6903,7 +7023,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="522" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="522" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B522" s="1" t="s">
         <v>521</v>
       </c>
@@ -6911,15 +7031,18 @@
         <v>784</v>
       </c>
     </row>
-    <row r="523" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="523" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B523" s="1" t="s">
         <v>522</v>
       </c>
       <c r="C523" s="1" t="s">
-        <v>784</v>
-      </c>
-    </row>
-    <row r="524" spans="2:3" x14ac:dyDescent="0.25">
+        <v>786</v>
+      </c>
+      <c r="D523" s="1" t="s">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="524" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B524" s="1" t="s">
         <v>523</v>
       </c>
@@ -6927,7 +7050,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="525" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="525" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B525" s="1" t="s">
         <v>524</v>
       </c>
@@ -6935,7 +7058,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="526" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="526" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B526" s="1" t="s">
         <v>525</v>
       </c>
@@ -6943,7 +7066,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="527" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="527" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B527" s="1" t="s">
         <v>526</v>
       </c>
@@ -6951,7 +7074,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="528" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="528" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B528" s="1" t="s">
         <v>527</v>
       </c>
@@ -6959,7 +7082,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="529" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="529" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B529" s="1" t="s">
         <v>528</v>
       </c>
@@ -6967,7 +7090,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="530" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="530" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B530" s="1" t="s">
         <v>529</v>
       </c>
@@ -6975,7 +7098,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="531" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="531" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B531" s="1" t="s">
         <v>530</v>
       </c>
@@ -6983,7 +7106,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="532" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="532" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B532" s="1" t="s">
         <v>531</v>
       </c>
@@ -6991,7 +7114,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="533" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="533" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B533" s="1" t="s">
         <v>532</v>
       </c>
@@ -6999,7 +7122,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="534" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="534" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B534" s="1" t="s">
         <v>533</v>
       </c>
@@ -7007,7 +7130,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="535" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="535" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B535" s="1" t="s">
         <v>534</v>
       </c>
@@ -7015,15 +7138,18 @@
         <v>784</v>
       </c>
     </row>
-    <row r="536" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="536" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B536" s="1" t="s">
         <v>535</v>
       </c>
       <c r="C536" s="1" t="s">
-        <v>784</v>
-      </c>
-    </row>
-    <row r="537" spans="2:3" x14ac:dyDescent="0.25">
+        <v>786</v>
+      </c>
+      <c r="D536" s="1" t="s">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="537" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B537" s="1" t="s">
         <v>536</v>
       </c>
@@ -7031,7 +7157,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="538" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="538" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B538" s="1" t="s">
         <v>537</v>
       </c>
@@ -7039,7 +7165,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="539" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="539" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B539" s="1" t="s">
         <v>538</v>
       </c>
@@ -7047,7 +7173,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="540" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="540" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B540" s="1" t="s">
         <v>539</v>
       </c>
@@ -7055,7 +7181,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="541" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="541" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B541" s="1" t="s">
         <v>540</v>
       </c>
@@ -7063,7 +7189,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="542" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="542" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B542" s="1" t="s">
         <v>541</v>
       </c>
@@ -7071,7 +7197,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="543" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="543" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B543" s="1" t="s">
         <v>542</v>
       </c>
@@ -7079,7 +7205,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="544" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="544" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B544" s="1" t="s">
         <v>543</v>
       </c>
@@ -7087,7 +7213,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="545" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="545" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B545" s="1" t="s">
         <v>544</v>
       </c>
@@ -7095,7 +7221,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="546" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="546" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B546" s="1" t="s">
         <v>545</v>
       </c>
@@ -7103,7 +7229,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="547" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="547" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B547" s="1" t="s">
         <v>546</v>
       </c>
@@ -7111,7 +7237,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="548" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="548" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B548" s="1" t="s">
         <v>547</v>
       </c>
@@ -7119,7 +7245,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="549" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="549" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B549" s="1" t="s">
         <v>548</v>
       </c>
@@ -7127,7 +7253,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="550" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="550" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B550" s="1" t="s">
         <v>549</v>
       </c>
@@ -7135,7 +7261,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="551" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="551" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B551" s="1" t="s">
         <v>550</v>
       </c>
@@ -7143,7 +7269,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="552" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="552" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B552" s="1" t="s">
         <v>551</v>
       </c>
@@ -7151,7 +7277,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="553" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="553" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B553" s="1" t="s">
         <v>552</v>
       </c>
@@ -7159,7 +7285,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="554" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="554" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B554" s="1" t="s">
         <v>553</v>
       </c>
@@ -7167,7 +7293,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="555" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="555" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B555" s="1" t="s">
         <v>554</v>
       </c>
@@ -7175,7 +7301,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="556" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="556" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B556" s="1" t="s">
         <v>555</v>
       </c>
@@ -7183,7 +7309,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="557" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="557" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B557" s="1" t="s">
         <v>556</v>
       </c>
@@ -7191,28 +7317,37 @@
         <v>784</v>
       </c>
     </row>
-    <row r="558" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="558" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B558" s="1" t="s">
         <v>557</v>
       </c>
       <c r="C558" s="1" t="s">
-        <v>784</v>
-      </c>
-    </row>
-    <row r="559" spans="2:3" x14ac:dyDescent="0.25">
+        <v>786</v>
+      </c>
+      <c r="D558" s="1" t="s">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="559" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B559" s="1" t="s">
         <v>558</v>
       </c>
       <c r="C559" s="1" t="s">
-        <v>784</v>
-      </c>
-    </row>
-    <row r="560" spans="2:3" x14ac:dyDescent="0.25">
+        <v>786</v>
+      </c>
+      <c r="D559" s="1" t="s">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="560" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B560" s="1" t="s">
         <v>559</v>
       </c>
       <c r="C560" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
+      </c>
+      <c r="D560" s="1" t="s">
+        <v>785</v>
       </c>
     </row>
     <row r="561" spans="2:3" x14ac:dyDescent="0.25">
@@ -7343,7 +7478,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="577" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="577" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B577" s="1" t="s">
         <v>576</v>
       </c>
@@ -7351,7 +7486,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="578" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="578" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B578" s="1" t="s">
         <v>577</v>
       </c>
@@ -7359,7 +7494,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="579" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="579" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B579" s="1" t="s">
         <v>578</v>
       </c>
@@ -7367,7 +7502,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="580" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="580" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B580" s="1" t="s">
         <v>579</v>
       </c>
@@ -7375,7 +7510,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="581" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="581" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B581" s="1" t="s">
         <v>580</v>
       </c>
@@ -7383,7 +7518,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="582" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="582" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B582" s="1" t="s">
         <v>581</v>
       </c>
@@ -7391,15 +7526,18 @@
         <v>784</v>
       </c>
     </row>
-    <row r="583" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="583" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B583" s="1" t="s">
         <v>582</v>
       </c>
       <c r="C583" s="1" t="s">
-        <v>784</v>
-      </c>
-    </row>
-    <row r="584" spans="2:3" x14ac:dyDescent="0.25">
+        <v>786</v>
+      </c>
+      <c r="D583" s="1" t="s">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="584" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B584" s="1" t="s">
         <v>583</v>
       </c>
@@ -7407,23 +7545,29 @@
         <v>784</v>
       </c>
     </row>
-    <row r="585" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="585" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B585" s="1" t="s">
         <v>584</v>
       </c>
       <c r="C585" s="1" t="s">
-        <v>784</v>
-      </c>
-    </row>
-    <row r="586" spans="2:3" x14ac:dyDescent="0.25">
+        <v>786</v>
+      </c>
+      <c r="D585" s="1" t="s">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="586" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B586" s="1" t="s">
         <v>585</v>
       </c>
       <c r="C586" s="1" t="s">
-        <v>784</v>
-      </c>
-    </row>
-    <row r="587" spans="2:3" x14ac:dyDescent="0.25">
+        <v>786</v>
+      </c>
+      <c r="D586" s="1" t="s">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="587" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B587" s="1" t="s">
         <v>586</v>
       </c>
@@ -7431,7 +7575,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="588" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="588" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B588" s="1" t="s">
         <v>587</v>
       </c>
@@ -7439,7 +7583,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="589" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="589" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B589" s="1" t="s">
         <v>588</v>
       </c>
@@ -7447,7 +7591,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="590" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="590" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B590" s="1" t="s">
         <v>589</v>
       </c>
@@ -7455,7 +7599,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="591" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="591" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B591" s="1" t="s">
         <v>590</v>
       </c>
@@ -7463,7 +7607,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="592" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="592" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B592" s="1" t="s">
         <v>591</v>
       </c>
@@ -7471,7 +7615,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="593" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="593" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B593" s="1" t="s">
         <v>592</v>
       </c>
@@ -7479,7 +7623,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="594" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="594" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B594" s="1" t="s">
         <v>593</v>
       </c>
@@ -7487,15 +7631,18 @@
         <v>784</v>
       </c>
     </row>
-    <row r="595" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="595" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B595" s="1" t="s">
         <v>594</v>
       </c>
       <c r="C595" s="1" t="s">
-        <v>784</v>
-      </c>
-    </row>
-    <row r="596" spans="2:3" x14ac:dyDescent="0.25">
+        <v>786</v>
+      </c>
+      <c r="D595" s="1" t="s">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="596" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B596" s="1" t="s">
         <v>595</v>
       </c>
@@ -7503,7 +7650,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="597" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="597" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B597" s="1" t="s">
         <v>596</v>
       </c>
@@ -7511,7 +7658,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="598" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="598" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B598" s="1" t="s">
         <v>597</v>
       </c>
@@ -7519,7 +7666,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="599" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="599" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B599" s="1" t="s">
         <v>598</v>
       </c>
@@ -7527,7 +7674,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="600" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="600" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B600" s="1" t="s">
         <v>599</v>
       </c>
@@ -7535,7 +7682,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="601" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="601" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B601" s="1" t="s">
         <v>600</v>
       </c>
@@ -7543,7 +7690,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="602" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="602" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B602" s="1" t="s">
         <v>601</v>
       </c>
@@ -7551,7 +7698,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="603" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="603" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B603" s="1" t="s">
         <v>602</v>
       </c>
@@ -7559,7 +7706,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="604" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="604" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B604" s="1" t="s">
         <v>603</v>
       </c>
@@ -7567,7 +7714,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="605" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="605" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B605" s="1" t="s">
         <v>604</v>
       </c>
@@ -7575,7 +7722,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="606" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="606" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B606" s="1" t="s">
         <v>605</v>
       </c>
@@ -7583,7 +7730,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="607" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="607" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B607" s="1" t="s">
         <v>606</v>
       </c>
@@ -7591,7 +7738,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="608" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="608" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B608" s="1" t="s">
         <v>607</v>
       </c>
@@ -7599,7 +7746,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="609" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="609" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B609" s="1" t="s">
         <v>608</v>
       </c>
@@ -7607,7 +7754,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="610" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="610" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B610" s="1" t="s">
         <v>609</v>
       </c>
@@ -7615,7 +7762,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="611" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="611" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B611" s="1" t="s">
         <v>610</v>
       </c>
@@ -7623,7 +7770,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="612" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="612" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B612" s="1" t="s">
         <v>611</v>
       </c>
@@ -7631,7 +7778,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="613" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="613" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B613" s="1" t="s">
         <v>612</v>
       </c>
@@ -7639,7 +7786,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="614" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="614" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B614" s="1" t="s">
         <v>613</v>
       </c>
@@ -7647,7 +7794,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="615" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="615" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B615" s="1" t="s">
         <v>614</v>
       </c>
@@ -7655,7 +7802,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="616" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="616" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B616" s="1" t="s">
         <v>615</v>
       </c>
@@ -7663,7 +7810,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="617" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="617" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B617" s="1" t="s">
         <v>616</v>
       </c>
@@ -7671,23 +7818,29 @@
         <v>784</v>
       </c>
     </row>
-    <row r="618" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="618" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B618" s="1" t="s">
         <v>617</v>
       </c>
       <c r="C618" s="1" t="s">
-        <v>784</v>
-      </c>
-    </row>
-    <row r="619" spans="2:3" x14ac:dyDescent="0.25">
+        <v>786</v>
+      </c>
+      <c r="D618" s="1" t="s">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="619" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B619" s="1" t="s">
         <v>618</v>
       </c>
       <c r="C619" s="1" t="s">
-        <v>784</v>
-      </c>
-    </row>
-    <row r="620" spans="2:3" x14ac:dyDescent="0.25">
+        <v>786</v>
+      </c>
+      <c r="D619" s="1" t="s">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="620" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B620" s="1" t="s">
         <v>619</v>
       </c>
@@ -7695,7 +7848,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="621" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="621" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B621" s="1" t="s">
         <v>620</v>
       </c>
@@ -7703,7 +7856,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="622" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="622" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B622" s="1" t="s">
         <v>621</v>
       </c>
@@ -7711,7 +7864,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="623" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="623" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B623" s="1" t="s">
         <v>622</v>
       </c>
@@ -7719,7 +7872,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="624" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="624" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B624" s="1" t="s">
         <v>623</v>
       </c>
@@ -7727,7 +7880,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="625" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="625" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B625" s="1" t="s">
         <v>624</v>
       </c>
@@ -7735,7 +7888,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="626" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="626" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B626" s="1" t="s">
         <v>625</v>
       </c>
@@ -7743,7 +7896,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="627" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="627" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B627" s="1" t="s">
         <v>626</v>
       </c>
@@ -7751,7 +7904,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="628" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="628" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B628" s="1" t="s">
         <v>627</v>
       </c>
@@ -7759,7 +7912,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="629" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="629" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B629" s="1" t="s">
         <v>628</v>
       </c>
@@ -7767,7 +7920,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="630" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="630" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B630" s="1" t="s">
         <v>629</v>
       </c>
@@ -7775,7 +7928,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="631" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="631" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B631" s="1" t="s">
         <v>630</v>
       </c>
@@ -7783,7 +7936,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="632" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="632" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B632" s="1" t="s">
         <v>631</v>
       </c>
@@ -7791,7 +7944,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="633" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="633" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B633" s="1" t="s">
         <v>632</v>
       </c>
@@ -7799,7 +7952,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="634" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="634" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B634" s="1" t="s">
         <v>633</v>
       </c>
@@ -7807,7 +7960,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="635" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="635" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B635" s="1" t="s">
         <v>634</v>
       </c>
@@ -7815,7 +7968,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="636" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="636" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B636" s="1" t="s">
         <v>635</v>
       </c>
@@ -7823,7 +7976,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="637" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="637" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B637" s="1" t="s">
         <v>636</v>
       </c>
@@ -7831,7 +7984,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="638" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="638" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B638" s="1" t="s">
         <v>637</v>
       </c>
@@ -7839,7 +7992,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="639" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="639" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B639" s="1" t="s">
         <v>638</v>
       </c>
@@ -7847,23 +8000,29 @@
         <v>784</v>
       </c>
     </row>
-    <row r="640" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="640" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B640" s="1" t="s">
         <v>639</v>
       </c>
       <c r="C640" s="1" t="s">
-        <v>784</v>
-      </c>
-    </row>
-    <row r="641" spans="2:3" x14ac:dyDescent="0.25">
+        <v>786</v>
+      </c>
+      <c r="D640" s="1" t="s">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="641" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B641" s="1" t="s">
         <v>640</v>
       </c>
       <c r="C641" s="1" t="s">
-        <v>784</v>
-      </c>
-    </row>
-    <row r="642" spans="2:3" x14ac:dyDescent="0.25">
+        <v>786</v>
+      </c>
+      <c r="D641" s="1" t="s">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="642" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B642" s="1" t="s">
         <v>641</v>
       </c>
@@ -7871,7 +8030,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="643" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="643" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B643" s="1" t="s">
         <v>642</v>
       </c>
@@ -7879,7 +8038,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="644" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="644" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B644" s="1" t="s">
         <v>643</v>
       </c>
@@ -7887,7 +8046,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="645" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="645" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B645" s="1" t="s">
         <v>644</v>
       </c>
@@ -7895,7 +8054,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="646" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="646" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B646" s="1" t="s">
         <v>645</v>
       </c>
@@ -7903,15 +8062,18 @@
         <v>784</v>
       </c>
     </row>
-    <row r="647" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="647" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B647" s="1" t="s">
         <v>646</v>
       </c>
       <c r="C647" s="1" t="s">
-        <v>784</v>
-      </c>
-    </row>
-    <row r="648" spans="2:3" x14ac:dyDescent="0.25">
+        <v>786</v>
+      </c>
+      <c r="D647" s="1" t="s">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="648" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B648" s="1" t="s">
         <v>647</v>
       </c>
@@ -7919,7 +8081,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="649" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="649" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B649" s="1" t="s">
         <v>648</v>
       </c>
@@ -7927,7 +8089,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="650" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="650" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B650" s="1" t="s">
         <v>649</v>
       </c>
@@ -7935,7 +8097,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="651" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="651" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B651" s="1" t="s">
         <v>650</v>
       </c>
@@ -7943,7 +8105,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="652" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="652" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B652" s="1" t="s">
         <v>651</v>
       </c>
@@ -7951,7 +8113,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="653" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="653" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B653" s="1" t="s">
         <v>652</v>
       </c>
@@ -7959,7 +8121,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="654" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="654" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B654" s="1" t="s">
         <v>653</v>
       </c>
@@ -7967,7 +8129,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="655" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="655" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B655" s="1" t="s">
         <v>654</v>
       </c>
@@ -7975,7 +8137,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="656" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="656" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B656" s="1" t="s">
         <v>655</v>
       </c>
@@ -7983,7 +8145,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="657" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="657" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B657" s="1" t="s">
         <v>656</v>
       </c>
@@ -7991,7 +8153,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="658" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="658" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B658" s="1" t="s">
         <v>657</v>
       </c>
@@ -7999,7 +8161,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="659" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="659" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B659" s="1" t="s">
         <v>658</v>
       </c>
@@ -8007,7 +8169,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="660" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="660" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B660" s="1" t="s">
         <v>659</v>
       </c>
@@ -8015,7 +8177,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="661" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="661" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B661" s="1" t="s">
         <v>660</v>
       </c>
@@ -8023,7 +8185,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="662" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="662" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B662" s="1" t="s">
         <v>661</v>
       </c>
@@ -8031,7 +8193,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="663" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="663" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B663" s="1" t="s">
         <v>662</v>
       </c>
@@ -8039,15 +8201,18 @@
         <v>784</v>
       </c>
     </row>
-    <row r="664" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="664" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B664" s="1" t="s">
         <v>663</v>
       </c>
       <c r="C664" s="1" t="s">
-        <v>784</v>
-      </c>
-    </row>
-    <row r="665" spans="2:3" x14ac:dyDescent="0.25">
+        <v>786</v>
+      </c>
+      <c r="D664" s="1" t="s">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="665" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B665" s="1" t="s">
         <v>664</v>
       </c>
@@ -8055,7 +8220,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="666" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="666" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B666" s="1" t="s">
         <v>665</v>
       </c>
@@ -8063,7 +8228,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="667" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="667" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B667" s="1" t="s">
         <v>666</v>
       </c>
@@ -8071,7 +8236,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="668" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="668" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B668" s="1" t="s">
         <v>667</v>
       </c>
@@ -8079,7 +8244,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="669" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="669" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B669" s="1" t="s">
         <v>668</v>
       </c>
@@ -8087,7 +8252,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="670" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="670" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B670" s="1" t="s">
         <v>669</v>
       </c>
@@ -8095,7 +8260,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="671" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="671" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B671" s="1" t="s">
         <v>670</v>
       </c>
@@ -8103,7 +8268,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="672" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="672" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B672" s="1" t="s">
         <v>671</v>
       </c>
@@ -8239,7 +8404,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="689" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="689" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B689" s="1" t="s">
         <v>688</v>
       </c>
@@ -8247,7 +8412,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="690" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="690" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B690" s="1" t="s">
         <v>689</v>
       </c>
@@ -8255,7 +8420,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="691" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="691" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B691" s="1" t="s">
         <v>690</v>
       </c>
@@ -8263,7 +8428,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="692" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="692" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B692" s="1" t="s">
         <v>691</v>
       </c>
@@ -8271,15 +8436,18 @@
         <v>784</v>
       </c>
     </row>
-    <row r="693" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="693" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B693" s="1" t="s">
         <v>692</v>
       </c>
       <c r="C693" s="1" t="s">
-        <v>784</v>
-      </c>
-    </row>
-    <row r="694" spans="2:3" x14ac:dyDescent="0.25">
+        <v>786</v>
+      </c>
+      <c r="D693" s="1" t="s">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="694" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B694" s="1" t="s">
         <v>693</v>
       </c>
@@ -8287,7 +8455,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="695" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="695" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B695" s="1" t="s">
         <v>694</v>
       </c>
@@ -8295,7 +8463,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="696" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="696" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B696" s="1" t="s">
         <v>695</v>
       </c>
@@ -8303,7 +8471,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="697" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="697" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B697" s="1" t="s">
         <v>696</v>
       </c>
@@ -8311,7 +8479,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="698" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="698" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B698" s="1" t="s">
         <v>697</v>
       </c>
@@ -8319,52 +8487,70 @@
         <v>784</v>
       </c>
     </row>
-    <row r="699" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="699" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B699" s="1" t="s">
         <v>698</v>
       </c>
       <c r="C699" s="1" t="s">
-        <v>784</v>
-      </c>
-    </row>
-    <row r="700" spans="2:3" x14ac:dyDescent="0.25">
+        <v>786</v>
+      </c>
+      <c r="D699" s="1" t="s">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="700" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B700" s="1" t="s">
         <v>699</v>
       </c>
       <c r="C700" s="1" t="s">
-        <v>784</v>
-      </c>
-    </row>
-    <row r="701" spans="2:3" x14ac:dyDescent="0.25">
+        <v>786</v>
+      </c>
+      <c r="D700" s="1" t="s">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="701" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B701" s="1" t="s">
         <v>700</v>
       </c>
       <c r="C701" s="1" t="s">
-        <v>784</v>
-      </c>
-    </row>
-    <row r="702" spans="2:3" x14ac:dyDescent="0.25">
+        <v>786</v>
+      </c>
+      <c r="D701" s="1" t="s">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="702" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B702" s="1" t="s">
         <v>701</v>
       </c>
       <c r="C702" s="1" t="s">
-        <v>784</v>
-      </c>
-    </row>
-    <row r="703" spans="2:3" x14ac:dyDescent="0.25">
+        <v>786</v>
+      </c>
+      <c r="D702" s="1" t="s">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="703" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B703" s="1" t="s">
         <v>702</v>
       </c>
       <c r="C703" s="1" t="s">
-        <v>784</v>
-      </c>
-    </row>
-    <row r="704" spans="2:3" x14ac:dyDescent="0.25">
+        <v>786</v>
+      </c>
+      <c r="D703" s="1" t="s">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="704" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B704" s="1" t="s">
         <v>703</v>
       </c>
       <c r="C704" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
+      </c>
+      <c r="D704" s="1" t="s">
+        <v>785</v>
       </c>
     </row>
     <row r="705" spans="2:3" x14ac:dyDescent="0.25">
@@ -8623,7 +8809,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="737" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="737" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B737" s="1" t="s">
         <v>736</v>
       </c>
@@ -8631,7 +8817,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="738" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="738" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B738" s="1" t="s">
         <v>737</v>
       </c>
@@ -8639,7 +8825,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="739" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="739" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B739" s="1" t="s">
         <v>738</v>
       </c>
@@ -8647,7 +8833,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="740" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="740" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B740" s="1" t="s">
         <v>739</v>
       </c>
@@ -8655,23 +8841,29 @@
         <v>784</v>
       </c>
     </row>
-    <row r="741" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="741" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B741" s="1" t="s">
         <v>740</v>
       </c>
       <c r="C741" s="1" t="s">
-        <v>784</v>
-      </c>
-    </row>
-    <row r="742" spans="2:3" x14ac:dyDescent="0.25">
+        <v>786</v>
+      </c>
+      <c r="D741" s="1" t="s">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="742" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B742" s="1" t="s">
         <v>741</v>
       </c>
       <c r="C742" s="1" t="s">
-        <v>784</v>
-      </c>
-    </row>
-    <row r="743" spans="2:3" x14ac:dyDescent="0.25">
+        <v>786</v>
+      </c>
+      <c r="D742" s="1" t="s">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="743" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B743" s="1" t="s">
         <v>742</v>
       </c>
@@ -8679,7 +8871,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="744" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="744" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B744" s="1" t="s">
         <v>743</v>
       </c>
@@ -8687,7 +8879,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="745" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="745" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B745" s="1" t="s">
         <v>744</v>
       </c>
@@ -8695,7 +8887,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="746" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="746" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B746" s="1" t="s">
         <v>745</v>
       </c>
@@ -8703,7 +8895,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="747" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="747" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B747" s="1" t="s">
         <v>746</v>
       </c>
@@ -8711,7 +8903,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="748" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="748" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B748" s="1" t="s">
         <v>747</v>
       </c>
@@ -8719,7 +8911,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="749" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="749" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B749" s="1" t="s">
         <v>748</v>
       </c>
@@ -8727,7 +8919,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="750" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="750" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B750" s="1" t="s">
         <v>749</v>
       </c>
@@ -8735,7 +8927,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="751" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="751" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B751" s="1" t="s">
         <v>750</v>
       </c>
@@ -8743,12 +8935,15 @@
         <v>784</v>
       </c>
     </row>
-    <row r="752" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="752" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B752" s="1" t="s">
         <v>751</v>
       </c>
       <c r="C752" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
+      </c>
+      <c r="D752" s="1" t="s">
+        <v>785</v>
       </c>
     </row>
     <row r="753" spans="2:3" x14ac:dyDescent="0.25">
@@ -8879,7 +9074,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="769" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="769" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B769" s="1" t="s">
         <v>768</v>
       </c>
@@ -8887,7 +9082,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="770" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="770" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B770" s="1" t="s">
         <v>769</v>
       </c>
@@ -8895,7 +9090,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="771" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="771" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B771" s="1" t="s">
         <v>770</v>
       </c>
@@ -8903,7 +9098,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="772" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="772" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B772" s="1" t="s">
         <v>771</v>
       </c>
@@ -8911,7 +9106,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="773" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="773" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B773" s="1" t="s">
         <v>772</v>
       </c>
@@ -8919,7 +9114,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="774" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="774" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B774" s="1" t="s">
         <v>773</v>
       </c>
@@ -8927,7 +9122,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="775" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="775" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B775" s="1" t="s">
         <v>774</v>
       </c>
@@ -8935,15 +9130,18 @@
         <v>784</v>
       </c>
     </row>
-    <row r="776" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="776" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B776" s="1" t="s">
         <v>775</v>
       </c>
       <c r="C776" s="1" t="s">
-        <v>784</v>
-      </c>
-    </row>
-    <row r="777" spans="2:3" x14ac:dyDescent="0.25">
+        <v>786</v>
+      </c>
+      <c r="D776" s="1" t="s">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="777" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B777" s="1" t="s">
         <v>776</v>
       </c>
@@ -8951,15 +9149,18 @@
         <v>784</v>
       </c>
     </row>
-    <row r="778" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="778" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B778" s="1" t="s">
         <v>777</v>
       </c>
       <c r="C778" s="1" t="s">
-        <v>784</v>
-      </c>
-    </row>
-    <row r="779" spans="2:3" x14ac:dyDescent="0.25">
+        <v>786</v>
+      </c>
+      <c r="D778" s="1" t="s">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="779" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B779" s="1" t="s">
         <v>778</v>
       </c>
@@ -8967,7 +9168,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="780" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="780" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B780" s="1" t="s">
         <v>779</v>
       </c>
@@ -8975,7 +9176,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="781" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="781" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B781" s="1" t="s">
         <v>780</v>
       </c>
@@ -8983,12 +9184,15 @@
         <v>784</v>
       </c>
     </row>
-    <row r="782" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="782" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B782" s="1" t="s">
         <v>781</v>
       </c>
       <c r="C782" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
+      </c>
+      <c r="D782" s="1" t="s">
+        <v>785</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ARQUIVOS QUE FALTAM 1 OU 2 FRASES A SE TRADUZIR EV013_us.u16 EV512_us.u16 mes_bg07_01_us.u16 mes_wd01_01_us.u16
</commit_message>
<xml_diff>
--- a/arquivos-tradutor.xlsx
+++ b/arquivos-tradutor.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1631" uniqueCount="787">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1635" uniqueCount="788">
   <si>
     <t>Arquivo</t>
   </si>
@@ -2385,6 +2385,9 @@
   </si>
   <si>
     <t>SIM</t>
+  </si>
+  <si>
+    <t>*SIM</t>
   </si>
 </sst>
 </file>
@@ -2727,8 +2730,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:D782"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C322" sqref="C322"/>
+    <sheetView tabSelected="1" topLeftCell="A753" workbookViewId="0">
+      <selection activeCell="D761" sqref="D761"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5348,7 +5351,10 @@
         <v>320</v>
       </c>
       <c r="C321" s="1" t="s">
-        <v>784</v>
+        <v>787</v>
+      </c>
+      <c r="D321" s="1" t="s">
+        <v>785</v>
       </c>
     </row>
     <row r="322" spans="2:4" x14ac:dyDescent="0.25">
@@ -7735,7 +7741,10 @@
         <v>606</v>
       </c>
       <c r="C607" s="1" t="s">
-        <v>784</v>
+        <v>787</v>
+      </c>
+      <c r="D607" s="1" t="s">
+        <v>785</v>
       </c>
     </row>
     <row r="608" spans="2:4" x14ac:dyDescent="0.25">
@@ -7885,7 +7894,10 @@
         <v>624</v>
       </c>
       <c r="C625" s="1" t="s">
-        <v>784</v>
+        <v>787</v>
+      </c>
+      <c r="D625" s="1" t="s">
+        <v>785</v>
       </c>
     </row>
     <row r="626" spans="2:4" x14ac:dyDescent="0.25">
@@ -8946,7 +8958,7 @@
         <v>785</v>
       </c>
     </row>
-    <row r="753" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="753" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B753" s="1" t="s">
         <v>752</v>
       </c>
@@ -8954,7 +8966,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="754" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="754" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B754" s="1" t="s">
         <v>753</v>
       </c>
@@ -8962,7 +8974,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="755" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="755" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B755" s="1" t="s">
         <v>754</v>
       </c>
@@ -8970,7 +8982,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="756" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="756" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B756" s="1" t="s">
         <v>755</v>
       </c>
@@ -8978,7 +8990,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="757" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="757" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B757" s="1" t="s">
         <v>756</v>
       </c>
@@ -8986,7 +8998,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="758" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="758" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B758" s="1" t="s">
         <v>757</v>
       </c>
@@ -8994,7 +9006,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="759" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="759" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B759" s="1" t="s">
         <v>758</v>
       </c>
@@ -9002,15 +9014,18 @@
         <v>784</v>
       </c>
     </row>
-    <row r="760" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="760" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B760" s="1" t="s">
         <v>759</v>
       </c>
       <c r="C760" s="1" t="s">
-        <v>784</v>
-      </c>
-    </row>
-    <row r="761" spans="2:3" x14ac:dyDescent="0.25">
+        <v>787</v>
+      </c>
+      <c r="D760" s="1" t="s">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="761" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B761" s="1" t="s">
         <v>760</v>
       </c>
@@ -9018,7 +9033,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="762" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="762" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B762" s="1" t="s">
         <v>761</v>
       </c>
@@ -9026,7 +9041,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="763" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="763" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B763" s="1" t="s">
         <v>762</v>
       </c>
@@ -9034,7 +9049,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="764" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="764" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B764" s="1" t="s">
         <v>763</v>
       </c>
@@ -9042,7 +9057,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="765" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="765" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B765" s="1" t="s">
         <v>764</v>
       </c>
@@ -9050,7 +9065,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="766" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="766" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B766" s="1" t="s">
         <v>765</v>
       </c>
@@ -9058,7 +9073,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="767" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="767" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B767" s="1" t="s">
         <v>766</v>
       </c>
@@ -9066,7 +9081,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="768" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="768" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B768" s="1" t="s">
         <v>767</v>
       </c>

</xml_diff>

<commit_message>
Traduzidos: EV010_us.u16 EV012_us.u16 EV014_us.u16
</commit_message>
<xml_diff>
--- a/arquivos-tradutor.xlsx
+++ b/arquivos-tradutor.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1635" uniqueCount="788">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1638" uniqueCount="788">
   <si>
     <t>Arquivo</t>
   </si>
@@ -2730,8 +2730,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:D782"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A753" workbookViewId="0">
-      <selection activeCell="D761" sqref="D761"/>
+    <sheetView tabSelected="1" topLeftCell="A311" workbookViewId="0">
+      <selection activeCell="D323" sqref="D323"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5324,7 +5324,10 @@
         <v>317</v>
       </c>
       <c r="C318" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
+      </c>
+      <c r="D318" s="1" t="s">
+        <v>785</v>
       </c>
     </row>
     <row r="319" spans="2:4" x14ac:dyDescent="0.25">
@@ -5343,7 +5346,10 @@
         <v>319</v>
       </c>
       <c r="C320" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
+      </c>
+      <c r="D320" s="1" t="s">
+        <v>785</v>
       </c>
     </row>
     <row r="321" spans="2:4" x14ac:dyDescent="0.25">
@@ -5362,7 +5368,10 @@
         <v>321</v>
       </c>
       <c r="C322" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
+      </c>
+      <c r="D322" s="1" t="s">
+        <v>785</v>
       </c>
     </row>
     <row r="323" spans="2:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
enviado EV016_us.u16 EV017_us.u16 EV019_us.u16
</commit_message>
<xml_diff>
--- a/arquivos-tradutor.xlsx
+++ b/arquivos-tradutor.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1638" uniqueCount="788">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1641" uniqueCount="788">
   <si>
     <t>Arquivo</t>
   </si>
@@ -2730,8 +2730,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:D782"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A311" workbookViewId="0">
-      <selection activeCell="D323" sqref="D323"/>
+    <sheetView tabSelected="1" topLeftCell="A317" workbookViewId="0">
+      <selection activeCell="C326" sqref="C326"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5379,7 +5379,10 @@
         <v>322</v>
       </c>
       <c r="C323" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
+      </c>
+      <c r="D323" s="1" t="s">
+        <v>785</v>
       </c>
     </row>
     <row r="324" spans="2:4" x14ac:dyDescent="0.25">
@@ -5387,7 +5390,10 @@
         <v>323</v>
       </c>
       <c r="C324" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
+      </c>
+      <c r="D324" s="1" t="s">
+        <v>785</v>
       </c>
     </row>
     <row r="325" spans="2:4" x14ac:dyDescent="0.25">
@@ -5406,7 +5412,10 @@
         <v>325</v>
       </c>
       <c r="C326" s="1" t="s">
-        <v>784</v>
+        <v>787</v>
+      </c>
+      <c r="D326" s="1" t="s">
+        <v>785</v>
       </c>
     </row>
     <row r="327" spans="2:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
TRADUZIDOS EV020_us.u16 EV021_us.u16 EV022_us.u16
</commit_message>
<xml_diff>
--- a/arquivos-tradutor.xlsx
+++ b/arquivos-tradutor.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1641" uniqueCount="788">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1645" uniqueCount="788">
   <si>
     <t>Arquivo</t>
   </si>
@@ -2731,7 +2731,7 @@
   <dimension ref="B1:D782"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A317" workbookViewId="0">
-      <selection activeCell="C326" sqref="C326"/>
+      <selection activeCell="C330" sqref="C330"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5423,7 +5423,10 @@
         <v>326</v>
       </c>
       <c r="C327" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
+      </c>
+      <c r="D327" s="1" t="s">
+        <v>785</v>
       </c>
     </row>
     <row r="328" spans="2:4" x14ac:dyDescent="0.25">
@@ -5431,7 +5434,10 @@
         <v>327</v>
       </c>
       <c r="C328" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
+      </c>
+      <c r="D328" s="1" t="s">
+        <v>785</v>
       </c>
     </row>
     <row r="329" spans="2:4" x14ac:dyDescent="0.25">
@@ -5439,7 +5445,10 @@
         <v>328</v>
       </c>
       <c r="C329" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
+      </c>
+      <c r="D329" s="1" t="s">
+        <v>785</v>
       </c>
     </row>
     <row r="330" spans="2:4" x14ac:dyDescent="0.25">
@@ -5447,7 +5456,10 @@
         <v>329</v>
       </c>
       <c r="C330" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
+      </c>
+      <c r="D330" s="1" t="s">
+        <v>785</v>
       </c>
     </row>
     <row r="331" spans="2:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Traduzidos EV026_us.u16 EV028_us.u16 EV030_us.u16 EV031_us.u16
</commit_message>
<xml_diff>
--- a/arquivos-tradutor.xlsx
+++ b/arquivos-tradutor.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1646" uniqueCount="788">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1650" uniqueCount="788">
   <si>
     <t>Arquivo</t>
   </si>
@@ -2730,8 +2730,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:D782"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A317" workbookViewId="0">
-      <selection activeCell="C332" sqref="C332"/>
+    <sheetView tabSelected="1" topLeftCell="A331" workbookViewId="0">
+      <selection activeCell="C335" sqref="C335"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5478,7 +5478,10 @@
         <v>331</v>
       </c>
       <c r="C332" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
+      </c>
+      <c r="D332" s="1" t="s">
+        <v>785</v>
       </c>
     </row>
     <row r="333" spans="2:4" x14ac:dyDescent="0.25">
@@ -5486,7 +5489,10 @@
         <v>332</v>
       </c>
       <c r="C333" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
+      </c>
+      <c r="D333" s="1" t="s">
+        <v>785</v>
       </c>
     </row>
     <row r="334" spans="2:4" x14ac:dyDescent="0.25">
@@ -5494,7 +5500,10 @@
         <v>333</v>
       </c>
       <c r="C334" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
+      </c>
+      <c r="D334" s="1" t="s">
+        <v>785</v>
       </c>
     </row>
     <row r="335" spans="2:4" x14ac:dyDescent="0.25">
@@ -5502,7 +5511,10 @@
         <v>334</v>
       </c>
       <c r="C335" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
+      </c>
+      <c r="D335" s="1" t="s">
+        <v>785</v>
       </c>
     </row>
     <row r="336" spans="2:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Planilha atualizada com os arquivos reservados para juminho (outer space)
</commit_message>
<xml_diff>
--- a/arquivos-tradutor.xlsx
+++ b/arquivos-tradutor.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1650" uniqueCount="788">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1680" uniqueCount="789">
   <si>
     <t>Arquivo</t>
   </si>
@@ -2388,6 +2388,9 @@
   </si>
   <si>
     <t>*SIM</t>
+  </si>
+  <si>
+    <t>juminho</t>
   </si>
 </sst>
 </file>
@@ -2730,8 +2733,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:D782"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A331" workbookViewId="0">
-      <selection activeCell="C335" sqref="C335"/>
+    <sheetView tabSelected="1" topLeftCell="A222" workbookViewId="0">
+      <selection activeCell="D222" sqref="D222"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5554,6 +5557,9 @@
       <c r="C339" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D339" s="1" t="s">
+        <v>788</v>
+      </c>
     </row>
     <row r="340" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B340" s="1" t="s">
@@ -5562,6 +5568,9 @@
       <c r="C340" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D340" s="1" t="s">
+        <v>788</v>
+      </c>
     </row>
     <row r="341" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B341" s="1" t="s">
@@ -5570,6 +5579,9 @@
       <c r="C341" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D341" s="1" t="s">
+        <v>788</v>
+      </c>
     </row>
     <row r="342" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B342" s="1" t="s">
@@ -5578,6 +5590,9 @@
       <c r="C342" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D342" s="1" t="s">
+        <v>788</v>
+      </c>
     </row>
     <row r="343" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B343" s="1" t="s">
@@ -5586,6 +5601,9 @@
       <c r="C343" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D343" s="1" t="s">
+        <v>788</v>
+      </c>
     </row>
     <row r="344" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B344" s="1" t="s">
@@ -5605,6 +5623,9 @@
       <c r="C345" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D345" s="1" t="s">
+        <v>788</v>
+      </c>
     </row>
     <row r="346" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B346" s="1" t="s">
@@ -5613,6 +5634,9 @@
       <c r="C346" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D346" s="1" t="s">
+        <v>788</v>
+      </c>
     </row>
     <row r="347" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B347" s="1" t="s">
@@ -5621,6 +5645,9 @@
       <c r="C347" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D347" s="1" t="s">
+        <v>788</v>
+      </c>
     </row>
     <row r="348" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B348" s="1" t="s">
@@ -5629,6 +5656,9 @@
       <c r="C348" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D348" s="1" t="s">
+        <v>788</v>
+      </c>
     </row>
     <row r="349" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B349" s="1" t="s">
@@ -5637,6 +5667,9 @@
       <c r="C349" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D349" s="1" t="s">
+        <v>788</v>
+      </c>
     </row>
     <row r="350" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B350" s="1" t="s">
@@ -5645,6 +5678,9 @@
       <c r="C350" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D350" s="1" t="s">
+        <v>788</v>
+      </c>
     </row>
     <row r="351" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B351" s="1" t="s">
@@ -5664,6 +5700,9 @@
       <c r="C352" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D352" s="1" t="s">
+        <v>788</v>
+      </c>
     </row>
     <row r="353" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B353" s="1" t="s">
@@ -5672,6 +5711,9 @@
       <c r="C353" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D353" s="1" t="s">
+        <v>788</v>
+      </c>
     </row>
     <row r="354" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B354" s="1" t="s">
@@ -5680,6 +5722,9 @@
       <c r="C354" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D354" s="1" t="s">
+        <v>788</v>
+      </c>
     </row>
     <row r="355" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B355" s="1" t="s">
@@ -5699,6 +5744,9 @@
       <c r="C356" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D356" s="1" t="s">
+        <v>788</v>
+      </c>
     </row>
     <row r="357" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B357" s="1" t="s">
@@ -5707,6 +5755,9 @@
       <c r="C357" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D357" s="1" t="s">
+        <v>788</v>
+      </c>
     </row>
     <row r="358" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B358" s="1" t="s">
@@ -5726,6 +5777,9 @@
       <c r="C359" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D359" s="1" t="s">
+        <v>788</v>
+      </c>
     </row>
     <row r="360" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B360" s="1" t="s">
@@ -5734,6 +5788,9 @@
       <c r="C360" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D360" s="1" t="s">
+        <v>788</v>
+      </c>
     </row>
     <row r="361" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B361" s="1" t="s">
@@ -5742,6 +5799,9 @@
       <c r="C361" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D361" s="1" t="s">
+        <v>788</v>
+      </c>
     </row>
     <row r="362" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B362" s="1" t="s">
@@ -5750,6 +5810,9 @@
       <c r="C362" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D362" s="1" t="s">
+        <v>788</v>
+      </c>
     </row>
     <row r="363" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B363" s="1" t="s">
@@ -5758,6 +5821,9 @@
       <c r="C363" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D363" s="1" t="s">
+        <v>788</v>
+      </c>
     </row>
     <row r="364" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B364" s="1" t="s">
@@ -5766,6 +5832,9 @@
       <c r="C364" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D364" s="1" t="s">
+        <v>788</v>
+      </c>
     </row>
     <row r="365" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B365" s="1" t="s">
@@ -5774,6 +5843,9 @@
       <c r="C365" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D365" s="1" t="s">
+        <v>788</v>
+      </c>
     </row>
     <row r="366" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B366" s="1" t="s">
@@ -5782,6 +5854,9 @@
       <c r="C366" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D366" s="1" t="s">
+        <v>788</v>
+      </c>
     </row>
     <row r="367" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B367" s="1" t="s">
@@ -5790,6 +5865,9 @@
       <c r="C367" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D367" s="1" t="s">
+        <v>788</v>
+      </c>
     </row>
     <row r="368" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B368" s="1" t="s">
@@ -5798,40 +5876,55 @@
       <c r="C368" s="1" t="s">
         <v>784</v>
       </c>
-    </row>
-    <row r="369" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D368" s="1" t="s">
+        <v>788</v>
+      </c>
+    </row>
+    <row r="369" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B369" s="1" t="s">
         <v>368</v>
       </c>
       <c r="C369" s="1" t="s">
         <v>784</v>
       </c>
-    </row>
-    <row r="370" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D369" s="1" t="s">
+        <v>788</v>
+      </c>
+    </row>
+    <row r="370" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B370" s="1" t="s">
         <v>369</v>
       </c>
       <c r="C370" s="1" t="s">
         <v>784</v>
       </c>
-    </row>
-    <row r="371" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D370" s="1" t="s">
+        <v>788</v>
+      </c>
+    </row>
+    <row r="371" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B371" s="1" t="s">
         <v>370</v>
       </c>
       <c r="C371" s="1" t="s">
         <v>784</v>
       </c>
-    </row>
-    <row r="372" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D371" s="1" t="s">
+        <v>788</v>
+      </c>
+    </row>
+    <row r="372" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B372" s="1" t="s">
         <v>371</v>
       </c>
       <c r="C372" s="1" t="s">
         <v>784</v>
       </c>
-    </row>
-    <row r="373" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D372" s="1" t="s">
+        <v>788</v>
+      </c>
+    </row>
+    <row r="373" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B373" s="1" t="s">
         <v>372</v>
       </c>
@@ -5839,7 +5932,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="374" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="374" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B374" s="1" t="s">
         <v>373</v>
       </c>
@@ -5847,7 +5940,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="375" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="375" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B375" s="1" t="s">
         <v>374</v>
       </c>
@@ -5855,7 +5948,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="376" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="376" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B376" s="1" t="s">
         <v>375</v>
       </c>
@@ -5863,7 +5956,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="377" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="377" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B377" s="1" t="s">
         <v>376</v>
       </c>
@@ -5871,7 +5964,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="378" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="378" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B378" s="1" t="s">
         <v>377</v>
       </c>
@@ -5879,7 +5972,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="379" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="379" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B379" s="1" t="s">
         <v>378</v>
       </c>
@@ -5887,7 +5980,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="380" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="380" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B380" s="1" t="s">
         <v>379</v>
       </c>
@@ -5895,7 +5988,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="381" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="381" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B381" s="1" t="s">
         <v>380</v>
       </c>
@@ -5903,7 +5996,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="382" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="382" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B382" s="1" t="s">
         <v>381</v>
       </c>
@@ -5911,7 +6004,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="383" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="383" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B383" s="1" t="s">
         <v>382</v>
       </c>
@@ -5919,7 +6012,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="384" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="384" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B384" s="1" t="s">
         <v>383</v>
       </c>

</xml_diff>

<commit_message>
traudizidos EV033_us.u16 EV079_us.u16 EV081_us.u16 EV082_us.u16 EV083_us.u16 EV084_us.u16
</commit_message>
<xml_diff>
--- a/arquivos-tradutor.xlsx
+++ b/arquivos-tradutor.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1680" uniqueCount="789">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1686" uniqueCount="789">
   <si>
     <t>Arquivo</t>
   </si>
@@ -2733,8 +2733,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:D782"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A222" workbookViewId="0">
-      <selection activeCell="D222" sqref="D222"/>
+    <sheetView tabSelected="1" topLeftCell="A371" workbookViewId="0">
+      <selection activeCell="C374" sqref="C374"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5536,7 +5536,10 @@
         <v>336</v>
       </c>
       <c r="C337" s="1" t="s">
-        <v>784</v>
+        <v>787</v>
+      </c>
+      <c r="D337" s="1" t="s">
+        <v>785</v>
       </c>
     </row>
     <row r="338" spans="2:4" x14ac:dyDescent="0.25">
@@ -5929,7 +5932,10 @@
         <v>372</v>
       </c>
       <c r="C373" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
+      </c>
+      <c r="D373" s="1" t="s">
+        <v>785</v>
       </c>
     </row>
     <row r="374" spans="2:4" x14ac:dyDescent="0.25">
@@ -5937,7 +5943,10 @@
         <v>373</v>
       </c>
       <c r="C374" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
+      </c>
+      <c r="D374" s="1" t="s">
+        <v>785</v>
       </c>
     </row>
     <row r="375" spans="2:4" x14ac:dyDescent="0.25">
@@ -5945,7 +5954,10 @@
         <v>374</v>
       </c>
       <c r="C375" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
+      </c>
+      <c r="D375" s="1" t="s">
+        <v>785</v>
       </c>
     </row>
     <row r="376" spans="2:4" x14ac:dyDescent="0.25">
@@ -5953,7 +5965,10 @@
         <v>375</v>
       </c>
       <c r="C376" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
+      </c>
+      <c r="D376" s="1" t="s">
+        <v>785</v>
       </c>
     </row>
     <row r="377" spans="2:4" x14ac:dyDescent="0.25">
@@ -5961,7 +5976,10 @@
         <v>376</v>
       </c>
       <c r="C377" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
+      </c>
+      <c r="D377" s="1" t="s">
+        <v>785</v>
       </c>
     </row>
     <row r="378" spans="2:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Arquivos traduzidos por juminho
</commit_message>
<xml_diff>
--- a/arquivos-tradutor.xlsx
+++ b/arquivos-tradutor.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1705" uniqueCount="789">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1745" uniqueCount="789">
   <si>
     <t>Arquivo</t>
   </si>
@@ -2733,8 +2733,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:D782"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A441" workbookViewId="0">
-      <selection activeCell="D441" sqref="D441"/>
+    <sheetView tabSelected="1" topLeftCell="A425" workbookViewId="0">
+      <selection activeCell="D445" sqref="D445"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5558,7 +5558,7 @@
         <v>338</v>
       </c>
       <c r="C339" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D339" s="1" t="s">
         <v>788</v>
@@ -5569,7 +5569,7 @@
         <v>339</v>
       </c>
       <c r="C340" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D340" s="1" t="s">
         <v>788</v>
@@ -5580,7 +5580,7 @@
         <v>340</v>
       </c>
       <c r="C341" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D341" s="1" t="s">
         <v>788</v>
@@ -5591,7 +5591,7 @@
         <v>341</v>
       </c>
       <c r="C342" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D342" s="1" t="s">
         <v>788</v>
@@ -5602,7 +5602,7 @@
         <v>342</v>
       </c>
       <c r="C343" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D343" s="1" t="s">
         <v>788</v>
@@ -5624,7 +5624,7 @@
         <v>344</v>
       </c>
       <c r="C345" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D345" s="1" t="s">
         <v>788</v>
@@ -5635,7 +5635,7 @@
         <v>345</v>
       </c>
       <c r="C346" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D346" s="1" t="s">
         <v>788</v>
@@ -5646,7 +5646,7 @@
         <v>346</v>
       </c>
       <c r="C347" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D347" s="1" t="s">
         <v>788</v>
@@ -5657,7 +5657,7 @@
         <v>347</v>
       </c>
       <c r="C348" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D348" s="1" t="s">
         <v>788</v>
@@ -5668,7 +5668,7 @@
         <v>348</v>
       </c>
       <c r="C349" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D349" s="1" t="s">
         <v>788</v>
@@ -5679,7 +5679,7 @@
         <v>349</v>
       </c>
       <c r="C350" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D350" s="1" t="s">
         <v>788</v>
@@ -5701,7 +5701,7 @@
         <v>351</v>
       </c>
       <c r="C352" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D352" s="1" t="s">
         <v>788</v>
@@ -5712,7 +5712,7 @@
         <v>352</v>
       </c>
       <c r="C353" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D353" s="1" t="s">
         <v>788</v>
@@ -5723,7 +5723,7 @@
         <v>353</v>
       </c>
       <c r="C354" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D354" s="1" t="s">
         <v>788</v>
@@ -5745,7 +5745,7 @@
         <v>355</v>
       </c>
       <c r="C356" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D356" s="1" t="s">
         <v>788</v>
@@ -5756,7 +5756,7 @@
         <v>356</v>
       </c>
       <c r="C357" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D357" s="1" t="s">
         <v>788</v>
@@ -5778,7 +5778,7 @@
         <v>358</v>
       </c>
       <c r="C359" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D359" s="1" t="s">
         <v>788</v>
@@ -5789,7 +5789,7 @@
         <v>359</v>
       </c>
       <c r="C360" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D360" s="1" t="s">
         <v>788</v>
@@ -5800,7 +5800,7 @@
         <v>360</v>
       </c>
       <c r="C361" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D361" s="1" t="s">
         <v>788</v>
@@ -5811,7 +5811,7 @@
         <v>361</v>
       </c>
       <c r="C362" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D362" s="1" t="s">
         <v>788</v>
@@ -5822,7 +5822,7 @@
         <v>362</v>
       </c>
       <c r="C363" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D363" s="1" t="s">
         <v>788</v>
@@ -5833,7 +5833,7 @@
         <v>363</v>
       </c>
       <c r="C364" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D364" s="1" t="s">
         <v>788</v>
@@ -5844,7 +5844,7 @@
         <v>364</v>
       </c>
       <c r="C365" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D365" s="1" t="s">
         <v>788</v>
@@ -5855,7 +5855,7 @@
         <v>365</v>
       </c>
       <c r="C366" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D366" s="1" t="s">
         <v>788</v>
@@ -5866,7 +5866,7 @@
         <v>366</v>
       </c>
       <c r="C367" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D367" s="1" t="s">
         <v>788</v>
@@ -5877,7 +5877,7 @@
         <v>367</v>
       </c>
       <c r="C368" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D368" s="1" t="s">
         <v>788</v>
@@ -5888,7 +5888,7 @@
         <v>368</v>
       </c>
       <c r="C369" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D369" s="1" t="s">
         <v>788</v>
@@ -5899,7 +5899,7 @@
         <v>369</v>
       </c>
       <c r="C370" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D370" s="1" t="s">
         <v>788</v>
@@ -5910,7 +5910,7 @@
         <v>370</v>
       </c>
       <c r="C371" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D371" s="1" t="s">
         <v>788</v>
@@ -5921,7 +5921,7 @@
         <v>371</v>
       </c>
       <c r="C372" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D372" s="1" t="s">
         <v>788</v>
@@ -5989,6 +5989,9 @@
       <c r="C378" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D378" s="1" t="s">
+        <v>788</v>
+      </c>
     </row>
     <row r="379" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B379" s="1" t="s">
@@ -5997,6 +6000,9 @@
       <c r="C379" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D379" s="1" t="s">
+        <v>788</v>
+      </c>
     </row>
     <row r="380" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B380" s="1" t="s">
@@ -6005,6 +6011,9 @@
       <c r="C380" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D380" s="1" t="s">
+        <v>788</v>
+      </c>
     </row>
     <row r="381" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B381" s="1" t="s">
@@ -6013,6 +6022,9 @@
       <c r="C381" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D381" s="1" t="s">
+        <v>788</v>
+      </c>
     </row>
     <row r="382" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B382" s="1" t="s">
@@ -6021,6 +6033,9 @@
       <c r="C382" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D382" s="1" t="s">
+        <v>788</v>
+      </c>
     </row>
     <row r="383" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B383" s="1" t="s">
@@ -6029,6 +6044,9 @@
       <c r="C383" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D383" s="1" t="s">
+        <v>788</v>
+      </c>
     </row>
     <row r="384" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B384" s="1" t="s">
@@ -6037,133 +6055,184 @@
       <c r="C384" s="1" t="s">
         <v>784</v>
       </c>
-    </row>
-    <row r="385" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D384" s="1" t="s">
+        <v>788</v>
+      </c>
+    </row>
+    <row r="385" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B385" s="1" t="s">
         <v>384</v>
       </c>
       <c r="C385" s="1" t="s">
         <v>784</v>
       </c>
-    </row>
-    <row r="386" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D385" s="1" t="s">
+        <v>788</v>
+      </c>
+    </row>
+    <row r="386" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B386" s="1" t="s">
         <v>385</v>
       </c>
       <c r="C386" s="1" t="s">
         <v>784</v>
       </c>
-    </row>
-    <row r="387" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D386" s="1" t="s">
+        <v>788</v>
+      </c>
+    </row>
+    <row r="387" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B387" s="1" t="s">
         <v>386</v>
       </c>
       <c r="C387" s="1" t="s">
         <v>784</v>
       </c>
-    </row>
-    <row r="388" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D387" s="1" t="s">
+        <v>788</v>
+      </c>
+    </row>
+    <row r="388" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B388" s="1" t="s">
         <v>387</v>
       </c>
       <c r="C388" s="1" t="s">
         <v>784</v>
       </c>
-    </row>
-    <row r="389" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D388" s="1" t="s">
+        <v>788</v>
+      </c>
+    </row>
+    <row r="389" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B389" s="1" t="s">
         <v>388</v>
       </c>
       <c r="C389" s="1" t="s">
         <v>784</v>
       </c>
-    </row>
-    <row r="390" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D389" s="1" t="s">
+        <v>788</v>
+      </c>
+    </row>
+    <row r="390" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B390" s="1" t="s">
         <v>389</v>
       </c>
       <c r="C390" s="1" t="s">
         <v>784</v>
       </c>
-    </row>
-    <row r="391" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D390" s="1" t="s">
+        <v>788</v>
+      </c>
+    </row>
+    <row r="391" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B391" s="1" t="s">
         <v>390</v>
       </c>
       <c r="C391" s="1" t="s">
         <v>784</v>
       </c>
-    </row>
-    <row r="392" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D391" s="1" t="s">
+        <v>788</v>
+      </c>
+    </row>
+    <row r="392" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B392" s="1" t="s">
         <v>391</v>
       </c>
       <c r="C392" s="1" t="s">
         <v>784</v>
       </c>
-    </row>
-    <row r="393" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D392" s="1" t="s">
+        <v>788</v>
+      </c>
+    </row>
+    <row r="393" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B393" s="1" t="s">
         <v>392</v>
       </c>
       <c r="C393" s="1" t="s">
         <v>784</v>
       </c>
-    </row>
-    <row r="394" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D393" s="1" t="s">
+        <v>788</v>
+      </c>
+    </row>
+    <row r="394" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B394" s="1" t="s">
         <v>393</v>
       </c>
       <c r="C394" s="1" t="s">
         <v>784</v>
       </c>
-    </row>
-    <row r="395" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D394" s="1" t="s">
+        <v>788</v>
+      </c>
+    </row>
+    <row r="395" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B395" s="1" t="s">
         <v>394</v>
       </c>
       <c r="C395" s="1" t="s">
         <v>784</v>
       </c>
-    </row>
-    <row r="396" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D395" s="1" t="s">
+        <v>788</v>
+      </c>
+    </row>
+    <row r="396" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B396" s="1" t="s">
         <v>395</v>
       </c>
       <c r="C396" s="1" t="s">
         <v>784</v>
       </c>
-    </row>
-    <row r="397" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D396" s="1" t="s">
+        <v>788</v>
+      </c>
+    </row>
+    <row r="397" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B397" s="1" t="s">
         <v>396</v>
       </c>
       <c r="C397" s="1" t="s">
         <v>784</v>
       </c>
-    </row>
-    <row r="398" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D397" s="1" t="s">
+        <v>788</v>
+      </c>
+    </row>
+    <row r="398" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B398" s="1" t="s">
         <v>397</v>
       </c>
       <c r="C398" s="1" t="s">
         <v>784</v>
       </c>
-    </row>
-    <row r="399" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D398" s="1" t="s">
+        <v>788</v>
+      </c>
+    </row>
+    <row r="399" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B399" s="1" t="s">
         <v>398</v>
       </c>
       <c r="C399" s="1" t="s">
         <v>784</v>
       </c>
-    </row>
-    <row r="400" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D399" s="1" t="s">
+        <v>788</v>
+      </c>
+    </row>
+    <row r="400" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B400" s="1" t="s">
         <v>399</v>
       </c>
       <c r="C400" s="1" t="s">
         <v>784</v>
+      </c>
+      <c r="D400" s="1" t="s">
+        <v>788</v>
       </c>
     </row>
     <row r="401" spans="2:4" x14ac:dyDescent="0.25">
@@ -6173,6 +6242,9 @@
       <c r="C401" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D401" s="1" t="s">
+        <v>788</v>
+      </c>
     </row>
     <row r="402" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B402" s="1" t="s">
@@ -6456,6 +6528,9 @@
       <c r="C427" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D427" s="1" t="s">
+        <v>788</v>
+      </c>
     </row>
     <row r="428" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B428" s="1" t="s">
@@ -6464,6 +6539,9 @@
       <c r="C428" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D428" s="1" t="s">
+        <v>788</v>
+      </c>
     </row>
     <row r="429" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B429" s="1" t="s">
@@ -6472,6 +6550,9 @@
       <c r="C429" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D429" s="1" t="s">
+        <v>788</v>
+      </c>
     </row>
     <row r="430" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B430" s="1" t="s">
@@ -6480,6 +6561,9 @@
       <c r="C430" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D430" s="1" t="s">
+        <v>788</v>
+      </c>
     </row>
     <row r="431" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B431" s="1" t="s">
@@ -6488,6 +6572,9 @@
       <c r="C431" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D431" s="1" t="s">
+        <v>788</v>
+      </c>
     </row>
     <row r="432" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B432" s="1" t="s">
@@ -6496,6 +6583,9 @@
       <c r="C432" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D432" s="1" t="s">
+        <v>788</v>
+      </c>
     </row>
     <row r="433" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B433" s="1" t="s">
@@ -6515,6 +6605,9 @@
       <c r="C434" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D434" s="1" t="s">
+        <v>788</v>
+      </c>
     </row>
     <row r="435" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B435" s="1" t="s">
@@ -6523,6 +6616,9 @@
       <c r="C435" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D435" s="1" t="s">
+        <v>788</v>
+      </c>
     </row>
     <row r="436" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B436" s="1" t="s">
@@ -6531,6 +6627,9 @@
       <c r="C436" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D436" s="1" t="s">
+        <v>788</v>
+      </c>
     </row>
     <row r="437" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B437" s="1" t="s">
@@ -6539,6 +6638,9 @@
       <c r="C437" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D437" s="1" t="s">
+        <v>788</v>
+      </c>
     </row>
     <row r="438" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B438" s="1" t="s">
@@ -6558,6 +6660,9 @@
       <c r="C439" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D439" s="1" t="s">
+        <v>788</v>
+      </c>
     </row>
     <row r="440" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B440" s="1" t="s">
@@ -6566,6 +6671,9 @@
       <c r="C440" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D440" s="1" t="s">
+        <v>788</v>
+      </c>
     </row>
     <row r="441" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B441" s="1" t="s">
@@ -6574,6 +6682,9 @@
       <c r="C441" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D441" s="1" t="s">
+        <v>788</v>
+      </c>
     </row>
     <row r="442" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B442" s="1" t="s">
@@ -6582,6 +6693,9 @@
       <c r="C442" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D442" s="1" t="s">
+        <v>788</v>
+      </c>
     </row>
     <row r="443" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B443" s="1" t="s">
@@ -6590,6 +6704,9 @@
       <c r="C443" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D443" s="1" t="s">
+        <v>788</v>
+      </c>
     </row>
     <row r="444" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B444" s="1" t="s">
@@ -6608,6 +6725,9 @@
       </c>
       <c r="C445" s="1" t="s">
         <v>784</v>
+      </c>
+      <c r="D445" s="1" t="s">
+        <v>788</v>
       </c>
     </row>
     <row r="446" spans="2:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Arq traduzidos EV191_us.u16 EV192_us.u16 EV195_us.u16
</commit_message>
<xml_diff>
--- a/arquivos-tradutor.xlsx
+++ b/arquivos-tradutor.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1745" uniqueCount="789">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1748" uniqueCount="789">
   <si>
     <t>Arquivo</t>
   </si>
@@ -2733,8 +2733,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:D782"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A425" workbookViewId="0">
-      <selection activeCell="D445" sqref="D445"/>
+    <sheetView tabSelected="1" topLeftCell="A446" workbookViewId="0">
+      <selection activeCell="C455" sqref="C455"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6816,7 +6816,10 @@
         <v>454</v>
       </c>
       <c r="C455" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
+      </c>
+      <c r="D455" s="1" t="s">
+        <v>785</v>
       </c>
     </row>
     <row r="456" spans="2:4" x14ac:dyDescent="0.25">
@@ -6824,7 +6827,10 @@
         <v>455</v>
       </c>
       <c r="C456" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
+      </c>
+      <c r="D456" s="1" t="s">
+        <v>785</v>
       </c>
     </row>
     <row r="457" spans="2:4" x14ac:dyDescent="0.25">
@@ -6843,7 +6849,10 @@
         <v>457</v>
       </c>
       <c r="C458" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
+      </c>
+      <c r="D458" s="1" t="s">
+        <v>785</v>
       </c>
     </row>
     <row r="459" spans="2:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
traduzidos EV120_us.u16 EV121_us.u16 EV122_us.u16
</commit_message>
<xml_diff>
--- a/arquivos-tradutor.xlsx
+++ b/arquivos-tradutor.xlsx
@@ -2733,8 +2733,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:D782"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A446" workbookViewId="0">
-      <selection activeCell="C455" sqref="C455"/>
+    <sheetView tabSelected="1" topLeftCell="A401" workbookViewId="0">
+      <selection activeCell="C405" sqref="C405"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6262,7 +6262,7 @@
         <v>402</v>
       </c>
       <c r="C403" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D403" s="1" t="s">
         <v>785</v>
@@ -6273,7 +6273,7 @@
         <v>403</v>
       </c>
       <c r="C404" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D404" s="1" t="s">
         <v>785</v>
@@ -6284,7 +6284,7 @@
         <v>404</v>
       </c>
       <c r="C405" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D405" s="1" t="s">
         <v>785</v>

</xml_diff>

<commit_message>
traduzidos mes_dg21_01_us.u16 mes_dg21_02_us.u16 mes_dg21_03_us.u16 mes_dg21_04_us.u16 mes_dg21_05_us.u16
</commit_message>
<xml_diff>
--- a/arquivos-tradutor.xlsx
+++ b/arquivos-tradutor.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1749" uniqueCount="789">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1754" uniqueCount="789">
   <si>
     <t>Arquivo</t>
   </si>
@@ -2733,8 +2733,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:D782"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A765" workbookViewId="0">
-      <selection activeCell="D777" sqref="D777"/>
+    <sheetView tabSelected="1" topLeftCell="A248" workbookViewId="0">
+      <selection activeCell="C248" sqref="C248"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8806,7 +8806,10 @@
         <v>693</v>
       </c>
       <c r="C694" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
+      </c>
+      <c r="D694" s="1" t="s">
+        <v>785</v>
       </c>
     </row>
     <row r="695" spans="2:4" x14ac:dyDescent="0.25">
@@ -8814,7 +8817,10 @@
         <v>694</v>
       </c>
       <c r="C695" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
+      </c>
+      <c r="D695" s="1" t="s">
+        <v>785</v>
       </c>
     </row>
     <row r="696" spans="2:4" x14ac:dyDescent="0.25">
@@ -8822,7 +8828,10 @@
         <v>695</v>
       </c>
       <c r="C696" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
+      </c>
+      <c r="D696" s="1" t="s">
+        <v>785</v>
       </c>
     </row>
     <row r="697" spans="2:4" x14ac:dyDescent="0.25">
@@ -8830,7 +8839,10 @@
         <v>696</v>
       </c>
       <c r="C697" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
+      </c>
+      <c r="D697" s="1" t="s">
+        <v>785</v>
       </c>
     </row>
     <row r="698" spans="2:4" x14ac:dyDescent="0.25">
@@ -8838,7 +8850,10 @@
         <v>697</v>
       </c>
       <c r="C698" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
+      </c>
+      <c r="D698" s="1" t="s">
+        <v>785</v>
       </c>
     </row>
     <row r="699" spans="2:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
atualização da tradução svld_mes_us.u16
</commit_message>
<xml_diff>
--- a/arquivos-tradutor.xlsx
+++ b/arquivos-tradutor.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1754" uniqueCount="789">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1755" uniqueCount="789">
   <si>
     <t>Arquivo</t>
   </si>
@@ -2733,8 +2733,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:D782"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A248" workbookViewId="0">
-      <selection activeCell="C248" sqref="C248"/>
+    <sheetView tabSelected="1" topLeftCell="A629" workbookViewId="0">
+      <selection activeCell="D643" sqref="D643"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8383,6 +8383,9 @@
       <c r="C642" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D642" s="1" t="s">
+        <v>785</v>
+      </c>
     </row>
     <row r="643" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B643" s="1" t="s">

</xml_diff>

<commit_message>
traduzidos EV245_us.u16 EV247_us.u16 EV249_us.u16
</commit_message>
<xml_diff>
--- a/arquivos-tradutor.xlsx
+++ b/arquivos-tradutor.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1767" uniqueCount="789">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1770" uniqueCount="790">
   <si>
     <t>Arquivo</t>
   </si>
@@ -2391,6 +2391,9 @@
   </si>
   <si>
     <t>juminho</t>
+  </si>
+  <si>
+    <t>sIM</t>
   </si>
 </sst>
 </file>
@@ -2733,8 +2736,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:D782"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A453" workbookViewId="0">
-      <selection activeCell="D460" sqref="D460"/>
+    <sheetView tabSelected="1" topLeftCell="A240" workbookViewId="0">
+      <selection activeCell="C504" sqref="C504"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7202,7 +7205,10 @@
         <v>497</v>
       </c>
       <c r="C498" s="1" t="s">
-        <v>784</v>
+        <v>789</v>
+      </c>
+      <c r="D498" s="1" t="s">
+        <v>785</v>
       </c>
     </row>
     <row r="499" spans="2:4" x14ac:dyDescent="0.25">
@@ -7218,7 +7224,10 @@
         <v>499</v>
       </c>
       <c r="C500" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
+      </c>
+      <c r="D500" s="1" t="s">
+        <v>785</v>
       </c>
     </row>
     <row r="501" spans="2:4" x14ac:dyDescent="0.25">
@@ -7237,7 +7246,10 @@
         <v>501</v>
       </c>
       <c r="C502" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
+      </c>
+      <c r="D502" s="1" t="s">
+        <v>785</v>
       </c>
     </row>
     <row r="503" spans="2:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Reservados arquivos inn para cfarl.
</commit_message>
<xml_diff>
--- a/arquivos-tradutor.xlsx
+++ b/arquivos-tradutor.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Moacyr\Desktop\GITHUB-BD\traducao-blue-dragon-xbox360\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20940" windowHeight="12180"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1770" uniqueCount="790">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1774" uniqueCount="791">
   <si>
     <t>Arquivo</t>
   </si>
@@ -2394,6 +2389,9 @@
   </si>
   <si>
     <t>sIM</t>
+  </si>
+  <si>
+    <t>cfarl</t>
   </si>
 </sst>
 </file>
@@ -2514,7 +2512,7 @@
     </a:clrScheme>
     <a:fontScheme name="Escritório">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2549,7 +2547,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2726,7 +2724,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2736,8 +2734,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:D782"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A240" workbookViewId="0">
-      <selection activeCell="C504" sqref="C504"/>
+    <sheetView tabSelected="1" topLeftCell="A747" workbookViewId="0">
+      <selection activeCell="G756" sqref="G756"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9389,6 +9387,9 @@
       <c r="C755" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D755" s="1" t="s">
+        <v>790</v>
+      </c>
     </row>
     <row r="756" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B756" s="1" t="s">
@@ -9397,6 +9398,9 @@
       <c r="C756" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D756" s="1" t="s">
+        <v>790</v>
+      </c>
     </row>
     <row r="757" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B757" s="1" t="s">
@@ -9405,6 +9409,9 @@
       <c r="C757" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D757" s="1" t="s">
+        <v>790</v>
+      </c>
     </row>
     <row r="758" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B758" s="1" t="s">
@@ -9412,6 +9419,9 @@
       </c>
       <c r="C758" s="1" t="s">
         <v>784</v>
+      </c>
+      <c r="D758" s="1" t="s">
+        <v>790</v>
       </c>
     </row>
     <row r="759" spans="2:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Corrigido o EV013_us.u16 e o EV017_us.u16
</commit_message>
<xml_diff>
--- a/arquivos-tradutor.xlsx
+++ b/arquivos-tradutor.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1774" uniqueCount="791">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1776" uniqueCount="792">
   <si>
     <t>Arquivo</t>
   </si>
@@ -2392,6 +2392,9 @@
   </si>
   <si>
     <t>cfarl</t>
+  </si>
+  <si>
+    <t>Revisado e retirado * por cfarl</t>
   </si>
 </sst>
 </file>
@@ -2421,7 +2424,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -2444,14 +2447,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2724,7 +2737,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2732,10 +2745,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:D782"/>
+  <dimension ref="B1:E782"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A747" workbookViewId="0">
-      <selection activeCell="G756" sqref="G756"/>
+    <sheetView tabSelected="1" topLeftCell="A316" workbookViewId="0">
+      <selection activeCell="B321" sqref="B321"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5356,18 +5369,21 @@
         <v>785</v>
       </c>
     </row>
-    <row r="321" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="321" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B321" s="1" t="s">
         <v>320</v>
       </c>
       <c r="C321" s="1" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="D321" s="1" t="s">
         <v>785</v>
       </c>
-    </row>
-    <row r="322" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E321" s="3" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="322" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B322" s="1" t="s">
         <v>321</v>
       </c>
@@ -5378,7 +5394,7 @@
         <v>785</v>
       </c>
     </row>
-    <row r="323" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="323" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B323" s="1" t="s">
         <v>322</v>
       </c>
@@ -5389,18 +5405,21 @@
         <v>785</v>
       </c>
     </row>
-    <row r="324" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="324" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B324" s="1" t="s">
         <v>323</v>
       </c>
       <c r="C324" s="1" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="D324" s="1" t="s">
         <v>785</v>
       </c>
-    </row>
-    <row r="325" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E324" s="3" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="325" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B325" s="1" t="s">
         <v>324</v>
       </c>
@@ -5411,7 +5430,7 @@
         <v>785</v>
       </c>
     </row>
-    <row r="326" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="326" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B326" s="1" t="s">
         <v>325</v>
       </c>
@@ -5422,7 +5441,7 @@
         <v>785</v>
       </c>
     </row>
-    <row r="327" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="327" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B327" s="1" t="s">
         <v>326</v>
       </c>
@@ -5433,7 +5452,7 @@
         <v>785</v>
       </c>
     </row>
-    <row r="328" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="328" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B328" s="1" t="s">
         <v>327</v>
       </c>
@@ -5444,7 +5463,7 @@
         <v>785</v>
       </c>
     </row>
-    <row r="329" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="329" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B329" s="1" t="s">
         <v>328</v>
       </c>
@@ -5455,7 +5474,7 @@
         <v>785</v>
       </c>
     </row>
-    <row r="330" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="330" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B330" s="1" t="s">
         <v>329</v>
       </c>
@@ -5466,7 +5485,7 @@
         <v>785</v>
       </c>
     </row>
-    <row r="331" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="331" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B331" s="1" t="s">
         <v>330</v>
       </c>
@@ -5477,7 +5496,7 @@
         <v>785</v>
       </c>
     </row>
-    <row r="332" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="332" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B332" s="1" t="s">
         <v>331</v>
       </c>
@@ -5488,7 +5507,7 @@
         <v>785</v>
       </c>
     </row>
-    <row r="333" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="333" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B333" s="1" t="s">
         <v>332</v>
       </c>
@@ -5499,7 +5518,7 @@
         <v>785</v>
       </c>
     </row>
-    <row r="334" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="334" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B334" s="1" t="s">
         <v>333</v>
       </c>
@@ -5510,7 +5529,7 @@
         <v>785</v>
       </c>
     </row>
-    <row r="335" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="335" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B335" s="1" t="s">
         <v>334</v>
       </c>
@@ -5521,7 +5540,7 @@
         <v>785</v>
       </c>
     </row>
-    <row r="336" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="336" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B336" s="1" t="s">
         <v>335</v>
       </c>

</xml_diff>

<commit_message>
Reservado arquivos para cfarl
</commit_message>
<xml_diff>
--- a/arquivos-tradutor.xlsx
+++ b/arquivos-tradutor.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Moacyr\Desktop\GITHUB-BD\traducao-blue-dragon-xbox360\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\danger\traducoes\blue-dragon\traducao-blue-dragon-xbox360\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1774" uniqueCount="790">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1819" uniqueCount="792">
   <si>
     <t>Arquivo</t>
   </si>
@@ -2394,6 +2394,12 @@
   </si>
   <si>
     <t>sIM</t>
+  </si>
+  <si>
+    <t>cfarl</t>
+  </si>
+  <si>
+    <t>Sim</t>
   </si>
 </sst>
 </file>
@@ -2736,8 +2742,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:D782"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A498" workbookViewId="0">
-      <selection activeCell="D509" sqref="D509"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E758" sqref="E758"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7746,132 +7752,180 @@
         <v>785</v>
       </c>
     </row>
-    <row r="561" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="561" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B561" s="1" t="s">
         <v>560</v>
       </c>
       <c r="C561" s="1" t="s">
         <v>784</v>
       </c>
-    </row>
-    <row r="562" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D561" s="1" t="s">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="562" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B562" s="1" t="s">
         <v>561</v>
       </c>
       <c r="C562" s="1" t="s">
         <v>784</v>
       </c>
-    </row>
-    <row r="563" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D562" s="1" t="s">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="563" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B563" s="1" t="s">
         <v>562</v>
       </c>
       <c r="C563" s="1" t="s">
         <v>784</v>
       </c>
-    </row>
-    <row r="564" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D563" s="1" t="s">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="564" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B564" s="1" t="s">
         <v>563</v>
       </c>
       <c r="C564" s="1" t="s">
         <v>784</v>
       </c>
-    </row>
-    <row r="565" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D564" s="1" t="s">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="565" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B565" s="1" t="s">
         <v>564</v>
       </c>
       <c r="C565" s="1" t="s">
         <v>784</v>
       </c>
-    </row>
-    <row r="566" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D565" s="1" t="s">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="566" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B566" s="1" t="s">
         <v>565</v>
       </c>
       <c r="C566" s="1" t="s">
         <v>784</v>
       </c>
-    </row>
-    <row r="567" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D566" s="1" t="s">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="567" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B567" s="1" t="s">
         <v>566</v>
       </c>
       <c r="C567" s="1" t="s">
         <v>784</v>
       </c>
-    </row>
-    <row r="568" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D567" s="1" t="s">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="568" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B568" s="1" t="s">
         <v>567</v>
       </c>
       <c r="C568" s="1" t="s">
         <v>784</v>
       </c>
-    </row>
-    <row r="569" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D568" s="1" t="s">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="569" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B569" s="1" t="s">
         <v>568</v>
       </c>
       <c r="C569" s="1" t="s">
         <v>784</v>
       </c>
-    </row>
-    <row r="570" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D569" s="1" t="s">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="570" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B570" s="1" t="s">
         <v>569</v>
       </c>
       <c r="C570" s="1" t="s">
         <v>784</v>
       </c>
-    </row>
-    <row r="571" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D570" s="1" t="s">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="571" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B571" s="1" t="s">
         <v>570</v>
       </c>
       <c r="C571" s="1" t="s">
         <v>784</v>
       </c>
-    </row>
-    <row r="572" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D571" s="1" t="s">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="572" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B572" s="1" t="s">
         <v>571</v>
       </c>
       <c r="C572" s="1" t="s">
         <v>784</v>
       </c>
-    </row>
-    <row r="573" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D572" s="1" t="s">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="573" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B573" s="1" t="s">
         <v>572</v>
       </c>
       <c r="C573" s="1" t="s">
         <v>784</v>
       </c>
-    </row>
-    <row r="574" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D573" s="1" t="s">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="574" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B574" s="1" t="s">
         <v>573</v>
       </c>
       <c r="C574" s="1" t="s">
         <v>784</v>
       </c>
-    </row>
-    <row r="575" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D574" s="1" t="s">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="575" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B575" s="1" t="s">
         <v>574</v>
       </c>
       <c r="C575" s="1" t="s">
         <v>784</v>
       </c>
-    </row>
-    <row r="576" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D575" s="1" t="s">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="576" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B576" s="1" t="s">
         <v>575</v>
       </c>
       <c r="C576" s="1" t="s">
         <v>784</v>
+      </c>
+      <c r="D576" s="1" t="s">
+        <v>790</v>
       </c>
     </row>
     <row r="577" spans="2:4" x14ac:dyDescent="0.25">
@@ -7881,6 +7935,9 @@
       <c r="C577" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D577" s="1" t="s">
+        <v>790</v>
+      </c>
     </row>
     <row r="578" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B578" s="1" t="s">
@@ -7889,6 +7946,9 @@
       <c r="C578" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D578" s="1" t="s">
+        <v>790</v>
+      </c>
     </row>
     <row r="579" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B579" s="1" t="s">
@@ -7897,6 +7957,9 @@
       <c r="C579" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D579" s="1" t="s">
+        <v>790</v>
+      </c>
     </row>
     <row r="580" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B580" s="1" t="s">
@@ -7905,6 +7968,9 @@
       <c r="C580" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D580" s="1" t="s">
+        <v>790</v>
+      </c>
     </row>
     <row r="581" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B581" s="1" t="s">
@@ -7913,6 +7979,9 @@
       <c r="C581" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D581" s="1" t="s">
+        <v>790</v>
+      </c>
     </row>
     <row r="582" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B582" s="1" t="s">
@@ -7921,6 +7990,9 @@
       <c r="C582" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D582" s="1" t="s">
+        <v>790</v>
+      </c>
     </row>
     <row r="583" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B583" s="1" t="s">
@@ -7970,6 +8042,9 @@
       <c r="C587" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D587" s="1" t="s">
+        <v>790</v>
+      </c>
     </row>
     <row r="588" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B588" s="1" t="s">
@@ -7978,6 +8053,9 @@
       <c r="C588" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D588" s="1" t="s">
+        <v>790</v>
+      </c>
     </row>
     <row r="589" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B589" s="1" t="s">
@@ -7986,6 +8064,9 @@
       <c r="C589" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D589" s="1" t="s">
+        <v>790</v>
+      </c>
     </row>
     <row r="590" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B590" s="1" t="s">
@@ -7994,6 +8075,9 @@
       <c r="C590" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D590" s="1" t="s">
+        <v>790</v>
+      </c>
     </row>
     <row r="591" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B591" s="1" t="s">
@@ -8002,6 +8086,9 @@
       <c r="C591" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D591" s="1" t="s">
+        <v>790</v>
+      </c>
     </row>
     <row r="592" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B592" s="1" t="s">
@@ -8010,6 +8097,9 @@
       <c r="C592" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D592" s="1" t="s">
+        <v>790</v>
+      </c>
     </row>
     <row r="593" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B593" s="1" t="s">
@@ -8018,6 +8108,9 @@
       <c r="C593" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D593" s="1" t="s">
+        <v>790</v>
+      </c>
     </row>
     <row r="594" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B594" s="1" t="s">
@@ -8026,6 +8119,9 @@
       <c r="C594" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D594" s="1" t="s">
+        <v>790</v>
+      </c>
     </row>
     <row r="595" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B595" s="1" t="s">
@@ -8045,6 +8141,9 @@
       <c r="C596" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D596" s="1" t="s">
+        <v>790</v>
+      </c>
     </row>
     <row r="597" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B597" s="1" t="s">
@@ -8053,6 +8152,9 @@
       <c r="C597" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D597" s="1" t="s">
+        <v>790</v>
+      </c>
     </row>
     <row r="598" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B598" s="1" t="s">
@@ -8061,6 +8163,9 @@
       <c r="C598" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D598" s="1" t="s">
+        <v>790</v>
+      </c>
     </row>
     <row r="599" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B599" s="1" t="s">
@@ -8069,6 +8174,9 @@
       <c r="C599" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D599" s="1" t="s">
+        <v>790</v>
+      </c>
     </row>
     <row r="600" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B600" s="1" t="s">
@@ -8077,6 +8185,9 @@
       <c r="C600" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D600" s="1" t="s">
+        <v>790</v>
+      </c>
     </row>
     <row r="601" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B601" s="1" t="s">
@@ -8085,6 +8196,9 @@
       <c r="C601" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D601" s="1" t="s">
+        <v>790</v>
+      </c>
     </row>
     <row r="602" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B602" s="1" t="s">
@@ -8093,6 +8207,9 @@
       <c r="C602" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D602" s="1" t="s">
+        <v>790</v>
+      </c>
     </row>
     <row r="603" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B603" s="1" t="s">
@@ -8101,6 +8218,9 @@
       <c r="C603" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D603" s="1" t="s">
+        <v>790</v>
+      </c>
     </row>
     <row r="604" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B604" s="1" t="s">
@@ -8109,6 +8229,9 @@
       <c r="C604" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D604" s="1" t="s">
+        <v>790</v>
+      </c>
     </row>
     <row r="605" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B605" s="1" t="s">
@@ -8117,6 +8240,9 @@
       <c r="C605" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D605" s="1" t="s">
+        <v>790</v>
+      </c>
     </row>
     <row r="606" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B606" s="1" t="s">
@@ -8125,6 +8251,9 @@
       <c r="C606" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D606" s="1" t="s">
+        <v>790</v>
+      </c>
     </row>
     <row r="607" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B607" s="1" t="s">
@@ -9399,7 +9528,10 @@
         <v>754</v>
       </c>
       <c r="C755" s="1" t="s">
-        <v>784</v>
+        <v>791</v>
+      </c>
+      <c r="D755" s="1" t="s">
+        <v>790</v>
       </c>
     </row>
     <row r="756" spans="2:4" x14ac:dyDescent="0.25">
@@ -9407,7 +9539,10 @@
         <v>755</v>
       </c>
       <c r="C756" s="1" t="s">
-        <v>784</v>
+        <v>791</v>
+      </c>
+      <c r="D756" s="1" t="s">
+        <v>790</v>
       </c>
     </row>
     <row r="757" spans="2:4" x14ac:dyDescent="0.25">
@@ -9415,7 +9550,10 @@
         <v>756</v>
       </c>
       <c r="C757" s="1" t="s">
-        <v>784</v>
+        <v>791</v>
+      </c>
+      <c r="D757" s="1" t="s">
+        <v>790</v>
       </c>
     </row>
     <row r="758" spans="2:4" x14ac:dyDescent="0.25">
@@ -9423,7 +9561,10 @@
         <v>757</v>
       </c>
       <c r="C758" s="1" t="s">
-        <v>784</v>
+        <v>791</v>
+      </c>
+      <c r="D758" s="1" t="s">
+        <v>790</v>
       </c>
     </row>
     <row r="759" spans="2:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
traduzidos EV200_us.u16 EV201_us.u16 EV202_us.u16 EV203_us.u16 EV204_us.u16
</commit_message>
<xml_diff>
--- a/arquivos-tradutor.xlsx
+++ b/arquivos-tradutor.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\danger\traducoes\blue-dragon\traducao-blue-dragon-xbox360\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Moacyr\Desktop\GITHUB-BD\traducao-blue-dragon-xbox360\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1819" uniqueCount="792">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1824" uniqueCount="792">
   <si>
     <t>Arquivo</t>
   </si>
@@ -2742,8 +2742,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:D782"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A544" workbookViewId="0">
-      <selection activeCell="F551" sqref="F551"/>
+    <sheetView tabSelected="1" topLeftCell="A462" workbookViewId="0">
+      <selection activeCell="D467" sqref="D467"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6931,7 +6931,10 @@
         <v>462</v>
       </c>
       <c r="C463" s="1" t="s">
-        <v>784</v>
+        <v>789</v>
+      </c>
+      <c r="D463" s="1" t="s">
+        <v>785</v>
       </c>
     </row>
     <row r="464" spans="2:4" x14ac:dyDescent="0.25">
@@ -6939,7 +6942,10 @@
         <v>463</v>
       </c>
       <c r="C464" s="1" t="s">
-        <v>784</v>
+        <v>789</v>
+      </c>
+      <c r="D464" s="1" t="s">
+        <v>785</v>
       </c>
     </row>
     <row r="465" spans="2:4" x14ac:dyDescent="0.25">
@@ -6947,7 +6953,10 @@
         <v>464</v>
       </c>
       <c r="C465" s="1" t="s">
-        <v>784</v>
+        <v>789</v>
+      </c>
+      <c r="D465" s="1" t="s">
+        <v>785</v>
       </c>
     </row>
     <row r="466" spans="2:4" x14ac:dyDescent="0.25">
@@ -6955,7 +6964,10 @@
         <v>465</v>
       </c>
       <c r="C466" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
+      </c>
+      <c r="D466" s="1" t="s">
+        <v>785</v>
       </c>
     </row>
     <row r="467" spans="2:4" x14ac:dyDescent="0.25">
@@ -6963,7 +6975,10 @@
         <v>466</v>
       </c>
       <c r="C467" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
+      </c>
+      <c r="D467" s="1" t="s">
+        <v>785</v>
       </c>
     </row>
     <row r="468" spans="2:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
traduzidos EV140_us.u16 EV142_us.u16 EV146_us.u16 EV147_us.u16
</commit_message>
<xml_diff>
--- a/arquivos-tradutor.xlsx
+++ b/arquivos-tradutor.xlsx
@@ -2769,8 +2769,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:D782"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A402" workbookViewId="0">
-      <selection activeCell="D410" sqref="D410"/>
+    <sheetView tabSelected="1" topLeftCell="A414" workbookViewId="0">
+      <selection activeCell="C425" sqref="C425"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6485,7 +6485,7 @@
         <v>419</v>
       </c>
       <c r="C420" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D420" s="1" t="s">
         <v>785</v>
@@ -6507,7 +6507,7 @@
         <v>421</v>
       </c>
       <c r="C422" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D422" s="1" t="s">
         <v>785</v>
@@ -6518,7 +6518,7 @@
         <v>422</v>
       </c>
       <c r="C423" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D423" s="1" t="s">
         <v>785</v>
@@ -6529,7 +6529,7 @@
         <v>423</v>
       </c>
       <c r="C424" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D424" s="1" t="s">
         <v>785</v>

</xml_diff>

<commit_message>
arquivos enviados para juminho 3 leva
</commit_message>
<xml_diff>
--- a/arquivos-tradutor.xlsx
+++ b/arquivos-tradutor.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1827" uniqueCount="793">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1851" uniqueCount="793">
   <si>
     <t>Arquivo</t>
   </si>
@@ -2769,8 +2769,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:D782"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A465" workbookViewId="0">
-      <selection activeCell="C487" sqref="C487"/>
+    <sheetView tabSelected="1" topLeftCell="A509" workbookViewId="0">
+      <selection activeCell="D511" sqref="D511"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7015,6 +7015,9 @@
       <c r="C468" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D468" s="1" t="s">
+        <v>788</v>
+      </c>
     </row>
     <row r="469" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B469" s="1" t="s">
@@ -7023,6 +7026,9 @@
       <c r="C469" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D469" s="1" t="s">
+        <v>788</v>
+      </c>
     </row>
     <row r="470" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B470" s="1" t="s">
@@ -7031,6 +7037,9 @@
       <c r="C470" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D470" s="1" t="s">
+        <v>788</v>
+      </c>
     </row>
     <row r="471" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B471" s="1" t="s">
@@ -7039,6 +7048,9 @@
       <c r="C471" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D471" s="1" t="s">
+        <v>788</v>
+      </c>
     </row>
     <row r="472" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B472" s="1" t="s">
@@ -7047,6 +7059,9 @@
       <c r="C472" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D472" s="1" t="s">
+        <v>788</v>
+      </c>
     </row>
     <row r="473" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B473" s="1" t="s">
@@ -7055,6 +7070,9 @@
       <c r="C473" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D473" s="1" t="s">
+        <v>788</v>
+      </c>
     </row>
     <row r="474" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B474" s="1" t="s">
@@ -7063,6 +7081,9 @@
       <c r="C474" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D474" s="1" t="s">
+        <v>788</v>
+      </c>
     </row>
     <row r="475" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B475" s="1" t="s">
@@ -7071,6 +7092,9 @@
       <c r="C475" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D475" s="1" t="s">
+        <v>788</v>
+      </c>
     </row>
     <row r="476" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B476" s="1" t="s">
@@ -7079,6 +7103,9 @@
       <c r="C476" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D476" s="1" t="s">
+        <v>788</v>
+      </c>
     </row>
     <row r="477" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B477" s="1" t="s">
@@ -7087,6 +7114,9 @@
       <c r="C477" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D477" s="1" t="s">
+        <v>788</v>
+      </c>
     </row>
     <row r="478" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B478" s="1" t="s">
@@ -7106,6 +7136,9 @@
       <c r="C479" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D479" s="1" t="s">
+        <v>788</v>
+      </c>
     </row>
     <row r="480" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B480" s="1" t="s">
@@ -7114,6 +7147,9 @@
       <c r="C480" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D480" s="1" t="s">
+        <v>788</v>
+      </c>
     </row>
     <row r="481" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B481" s="1" t="s">
@@ -7171,6 +7207,9 @@
       <c r="C486" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D486" s="1" t="s">
+        <v>788</v>
+      </c>
     </row>
     <row r="487" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B487" s="1" t="s">
@@ -7179,6 +7218,9 @@
       <c r="C487" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D487" s="1" t="s">
+        <v>788</v>
+      </c>
     </row>
     <row r="488" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B488" s="1" t="s">
@@ -7187,6 +7229,9 @@
       <c r="C488" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D488" s="1" t="s">
+        <v>788</v>
+      </c>
     </row>
     <row r="489" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B489" s="1" t="s">
@@ -7195,6 +7240,9 @@
       <c r="C489" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D489" s="1" t="s">
+        <v>788</v>
+      </c>
     </row>
     <row r="490" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B490" s="1" t="s">
@@ -7203,6 +7251,9 @@
       <c r="C490" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D490" s="1" t="s">
+        <v>788</v>
+      </c>
     </row>
     <row r="491" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B491" s="1" t="s">
@@ -7211,6 +7262,9 @@
       <c r="C491" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D491" s="1" t="s">
+        <v>788</v>
+      </c>
     </row>
     <row r="492" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B492" s="1" t="s">
@@ -7219,6 +7273,9 @@
       <c r="C492" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D492" s="1" t="s">
+        <v>788</v>
+      </c>
     </row>
     <row r="493" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B493" s="1" t="s">
@@ -7227,6 +7284,9 @@
       <c r="C493" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D493" s="1" t="s">
+        <v>788</v>
+      </c>
     </row>
     <row r="494" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B494" s="1" t="s">
@@ -7235,6 +7295,9 @@
       <c r="C494" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D494" s="1" t="s">
+        <v>788</v>
+      </c>
     </row>
     <row r="495" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B495" s="1" t="s">
@@ -7243,6 +7306,9 @@
       <c r="C495" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D495" s="1" t="s">
+        <v>788</v>
+      </c>
     </row>
     <row r="496" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B496" s="1" t="s">
@@ -7251,6 +7317,9 @@
       <c r="C496" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D496" s="1" t="s">
+        <v>788</v>
+      </c>
     </row>
     <row r="497" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B497" s="1" t="s">
@@ -7258,6 +7327,9 @@
       </c>
       <c r="C497" s="1" t="s">
         <v>784</v>
+      </c>
+      <c r="D497" s="1" t="s">
+        <v>788</v>
       </c>
     </row>
     <row r="498" spans="2:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Reservado arquivo para cfarl
</commit_message>
<xml_diff>
--- a/arquivos-tradutor.xlsx
+++ b/arquivos-tradutor.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Moacyr\Desktop\GITHUB-BD\traducao-blue-dragon-xbox360\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20940" windowHeight="12180"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1853" uniqueCount="794">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1883" uniqueCount="794">
   <si>
     <t>Arquivo</t>
   </si>
@@ -2470,7 +2465,45 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="7">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -2550,7 +2583,7 @@
     </a:clrScheme>
     <a:fontScheme name="Escritório">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2585,7 +2618,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2762,7 +2795,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2772,8 +2805,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:D782"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A521" workbookViewId="0">
-      <selection activeCell="D527" sqref="D527"/>
+    <sheetView tabSelected="1" topLeftCell="A525" workbookViewId="0">
+      <selection activeCell="E530" sqref="E530"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7601,6 +7634,9 @@
       <c r="C527" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D527" s="1" t="s">
+        <v>790</v>
+      </c>
     </row>
     <row r="528" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B528" s="1" t="s">
@@ -7609,6 +7645,9 @@
       <c r="C528" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D528" s="1" t="s">
+        <v>790</v>
+      </c>
     </row>
     <row r="529" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B529" s="1" t="s">
@@ -7617,6 +7656,9 @@
       <c r="C529" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D529" s="1" t="s">
+        <v>790</v>
+      </c>
     </row>
     <row r="530" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B530" s="1" t="s">
@@ -7625,6 +7667,9 @@
       <c r="C530" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D530" s="1" t="s">
+        <v>790</v>
+      </c>
     </row>
     <row r="531" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B531" s="1" t="s">
@@ -7633,6 +7678,9 @@
       <c r="C531" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D531" s="1" t="s">
+        <v>790</v>
+      </c>
     </row>
     <row r="532" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B532" s="1" t="s">
@@ -7641,6 +7689,9 @@
       <c r="C532" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D532" s="1" t="s">
+        <v>790</v>
+      </c>
     </row>
     <row r="533" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B533" s="1" t="s">
@@ -7649,6 +7700,9 @@
       <c r="C533" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D533" s="1" t="s">
+        <v>790</v>
+      </c>
     </row>
     <row r="534" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B534" s="1" t="s">
@@ -7657,6 +7711,9 @@
       <c r="C534" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D534" s="1" t="s">
+        <v>790</v>
+      </c>
     </row>
     <row r="535" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B535" s="1" t="s">
@@ -7665,6 +7722,9 @@
       <c r="C535" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D535" s="1" t="s">
+        <v>790</v>
+      </c>
     </row>
     <row r="536" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B536" s="1" t="s">
@@ -7684,6 +7744,9 @@
       <c r="C537" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D537" s="1" t="s">
+        <v>790</v>
+      </c>
     </row>
     <row r="538" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B538" s="1" t="s">
@@ -7692,6 +7755,9 @@
       <c r="C538" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D538" s="1" t="s">
+        <v>790</v>
+      </c>
     </row>
     <row r="539" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B539" s="1" t="s">
@@ -7700,6 +7766,9 @@
       <c r="C539" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D539" s="1" t="s">
+        <v>790</v>
+      </c>
     </row>
     <row r="540" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B540" s="1" t="s">
@@ -7708,6 +7777,9 @@
       <c r="C540" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D540" s="1" t="s">
+        <v>790</v>
+      </c>
     </row>
     <row r="541" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B541" s="1" t="s">
@@ -7716,6 +7788,9 @@
       <c r="C541" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D541" s="1" t="s">
+        <v>790</v>
+      </c>
     </row>
     <row r="542" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B542" s="1" t="s">
@@ -7724,6 +7799,9 @@
       <c r="C542" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D542" s="1" t="s">
+        <v>790</v>
+      </c>
     </row>
     <row r="543" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B543" s="1" t="s">
@@ -7732,6 +7810,9 @@
       <c r="C543" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D543" s="1" t="s">
+        <v>790</v>
+      </c>
     </row>
     <row r="544" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B544" s="1" t="s">
@@ -7740,6 +7821,9 @@
       <c r="C544" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D544" s="1" t="s">
+        <v>790</v>
+      </c>
     </row>
     <row r="545" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B545" s="1" t="s">
@@ -7748,6 +7832,9 @@
       <c r="C545" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D545" s="1" t="s">
+        <v>790</v>
+      </c>
     </row>
     <row r="546" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B546" s="1" t="s">
@@ -7756,6 +7843,9 @@
       <c r="C546" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D546" s="1" t="s">
+        <v>790</v>
+      </c>
     </row>
     <row r="547" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B547" s="1" t="s">
@@ -7764,6 +7854,9 @@
       <c r="C547" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D547" s="1" t="s">
+        <v>790</v>
+      </c>
     </row>
     <row r="548" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B548" s="1" t="s">
@@ -7772,6 +7865,9 @@
       <c r="C548" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D548" s="1" t="s">
+        <v>790</v>
+      </c>
     </row>
     <row r="549" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B549" s="1" t="s">
@@ -7780,6 +7876,9 @@
       <c r="C549" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D549" s="1" t="s">
+        <v>790</v>
+      </c>
     </row>
     <row r="550" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B550" s="1" t="s">
@@ -7788,6 +7887,9 @@
       <c r="C550" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D550" s="1" t="s">
+        <v>790</v>
+      </c>
     </row>
     <row r="551" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B551" s="1" t="s">
@@ -7796,6 +7898,9 @@
       <c r="C551" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D551" s="1" t="s">
+        <v>790</v>
+      </c>
     </row>
     <row r="552" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B552" s="1" t="s">
@@ -7804,6 +7909,9 @@
       <c r="C552" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D552" s="1" t="s">
+        <v>790</v>
+      </c>
     </row>
     <row r="553" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B553" s="1" t="s">
@@ -7812,6 +7920,9 @@
       <c r="C553" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D553" s="1" t="s">
+        <v>790</v>
+      </c>
     </row>
     <row r="554" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B554" s="1" t="s">
@@ -7820,6 +7931,9 @@
       <c r="C554" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D554" s="1" t="s">
+        <v>790</v>
+      </c>
     </row>
     <row r="555" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B555" s="1" t="s">
@@ -7828,6 +7942,9 @@
       <c r="C555" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D555" s="1" t="s">
+        <v>790</v>
+      </c>
     </row>
     <row r="556" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B556" s="1" t="s">
@@ -7836,6 +7953,9 @@
       <c r="C556" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D556" s="1" t="s">
+        <v>790</v>
+      </c>
     </row>
     <row r="557" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B557" s="1" t="s">
@@ -7844,6 +7964,9 @@
       <c r="C557" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D557" s="1" t="s">
+        <v>790</v>
+      </c>
     </row>
     <row r="558" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B558" s="1" t="s">
@@ -8268,7 +8391,7 @@
         <v>595</v>
       </c>
       <c r="C596" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D596" s="1" t="s">
         <v>790</v>
@@ -8279,7 +8402,7 @@
         <v>596</v>
       </c>
       <c r="C597" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D597" s="1" t="s">
         <v>790</v>
@@ -8290,7 +8413,7 @@
         <v>597</v>
       </c>
       <c r="C598" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D598" s="1" t="s">
         <v>790</v>
@@ -8301,7 +8424,7 @@
         <v>598</v>
       </c>
       <c r="C599" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D599" s="1" t="s">
         <v>790</v>
@@ -8312,7 +8435,7 @@
         <v>599</v>
       </c>
       <c r="C600" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D600" s="1" t="s">
         <v>790</v>
@@ -8323,7 +8446,7 @@
         <v>600</v>
       </c>
       <c r="C601" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D601" s="1" t="s">
         <v>790</v>
@@ -8334,7 +8457,7 @@
         <v>601</v>
       </c>
       <c r="C602" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D602" s="1" t="s">
         <v>790</v>
@@ -8345,7 +8468,7 @@
         <v>602</v>
       </c>
       <c r="C603" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D603" s="1" t="s">
         <v>790</v>
@@ -8356,7 +8479,7 @@
         <v>603</v>
       </c>
       <c r="C604" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D604" s="1" t="s">
         <v>790</v>
@@ -8367,7 +8490,7 @@
         <v>604</v>
       </c>
       <c r="C605" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D605" s="1" t="s">
         <v>790</v>
@@ -8378,7 +8501,7 @@
         <v>605</v>
       </c>
       <c r="C606" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D606" s="1" t="s">
         <v>790</v>
@@ -9918,12 +10041,12 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
       <formula>"SIM"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="notContainsBlanks" dxfId="0" priority="4">
+    <cfRule type="notContainsBlanks" dxfId="5" priority="4">
       <formula>LEN(TRIM(D1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
correção dos arquivos EV017_us.u16 EV019_us.u16 EV024_us.u16
</commit_message>
<xml_diff>
--- a/arquivos-tradutor.xlsx
+++ b/arquivos-tradutor.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Moacyr\Desktop\GITHUB-BD\traducao-blue-dragon-xbox360\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
@@ -2465,45 +2470,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <fill>
         <patternFill>
@@ -2795,7 +2762,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2805,8 +2772,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:D782"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A525" workbookViewId="0">
-      <selection activeCell="E530" sqref="E530"/>
+    <sheetView tabSelected="1" topLeftCell="A650" workbookViewId="0">
+      <selection activeCell="D672" sqref="D672"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5432,7 +5399,7 @@
         <v>320</v>
       </c>
       <c r="C321" s="1" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="D321" s="1" t="s">
         <v>785</v>
@@ -5465,7 +5432,7 @@
         <v>323</v>
       </c>
       <c r="C324" s="1" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="D324" s="1" t="s">
         <v>785</v>
@@ -5487,7 +5454,7 @@
         <v>325</v>
       </c>
       <c r="C326" s="1" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="D326" s="1" t="s">
         <v>785</v>
@@ -5498,7 +5465,7 @@
         <v>326</v>
       </c>
       <c r="C327" s="1" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="D327" s="1" t="s">
         <v>785</v>
@@ -5542,7 +5509,7 @@
         <v>330</v>
       </c>
       <c r="C331" s="1" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="D331" s="1" t="s">
         <v>785</v>
@@ -5608,7 +5575,7 @@
         <v>336</v>
       </c>
       <c r="C337" s="1" t="s">
-        <v>787</v>
+        <v>789</v>
       </c>
       <c r="D337" s="1" t="s">
         <v>785</v>
@@ -10041,12 +10008,12 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"SIM"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="notContainsBlanks" dxfId="5" priority="4">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="4">
       <formula>LEN(TRIM(D1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Marcados arquivos para cfarl traduzir Adicionados arquivos em espanhol
</commit_message>
<xml_diff>
--- a/arquivos-tradutor.xlsx
+++ b/arquivos-tradutor.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Moacyr\Desktop\GITHUB-BD\traducao-blue-dragon-xbox360\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1884" uniqueCount="794">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1904" uniqueCount="794">
   <si>
     <t>Arquivo</t>
   </si>
@@ -2470,7 +2465,76 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="11">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -2762,7 +2826,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2772,8 +2836,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:D782"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A609" workbookViewId="0">
-      <selection activeCell="D618" sqref="D618"/>
+    <sheetView tabSelected="1" topLeftCell="A494" workbookViewId="0">
+      <selection activeCell="D503" sqref="D503"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7353,6 +7417,9 @@
       <c r="C499" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D499" s="1" t="s">
+        <v>790</v>
+      </c>
     </row>
     <row r="500" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B500" s="1" t="s">
@@ -7394,6 +7461,9 @@
       <c r="C503" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D503" s="1" t="s">
+        <v>790</v>
+      </c>
     </row>
     <row r="504" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B504" s="1" t="s">
@@ -7413,6 +7483,9 @@
       <c r="C505" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D505" s="1" t="s">
+        <v>790</v>
+      </c>
     </row>
     <row r="506" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B506" s="1" t="s">
@@ -7421,6 +7494,9 @@
       <c r="C506" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D506" s="1" t="s">
+        <v>790</v>
+      </c>
     </row>
     <row r="507" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B507" s="1" t="s">
@@ -7429,6 +7505,9 @@
       <c r="C507" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D507" s="1" t="s">
+        <v>790</v>
+      </c>
     </row>
     <row r="508" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B508" s="1" t="s">
@@ -7437,6 +7516,9 @@
       <c r="C508" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D508" s="1" t="s">
+        <v>790</v>
+      </c>
     </row>
     <row r="509" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B509" s="1" t="s">
@@ -7467,6 +7549,9 @@
       <c r="C511" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D511" s="1" t="s">
+        <v>790</v>
+      </c>
     </row>
     <row r="512" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B512" s="1" t="s">
@@ -7475,6 +7560,9 @@
       <c r="C512" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D512" s="1" t="s">
+        <v>790</v>
+      </c>
     </row>
     <row r="513" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B513" s="1" t="s">
@@ -7483,6 +7571,9 @@
       <c r="C513" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D513" s="1" t="s">
+        <v>790</v>
+      </c>
     </row>
     <row r="514" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B514" s="1" t="s">
@@ -7491,6 +7582,9 @@
       <c r="C514" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D514" s="1" t="s">
+        <v>790</v>
+      </c>
     </row>
     <row r="515" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B515" s="1" t="s">
@@ -7499,6 +7593,9 @@
       <c r="C515" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D515" s="1" t="s">
+        <v>790</v>
+      </c>
     </row>
     <row r="516" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B516" s="1" t="s">
@@ -7507,6 +7604,9 @@
       <c r="C516" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D516" s="1" t="s">
+        <v>790</v>
+      </c>
     </row>
     <row r="517" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B517" s="1" t="s">
@@ -7515,6 +7615,9 @@
       <c r="C517" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D517" s="1" t="s">
+        <v>790</v>
+      </c>
     </row>
     <row r="518" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B518" s="1" t="s">
@@ -7523,6 +7626,9 @@
       <c r="C518" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D518" s="1" t="s">
+        <v>790</v>
+      </c>
     </row>
     <row r="519" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B519" s="1" t="s">
@@ -7531,6 +7637,9 @@
       <c r="C519" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D519" s="1" t="s">
+        <v>790</v>
+      </c>
     </row>
     <row r="520" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B520" s="1" t="s">
@@ -7539,6 +7648,9 @@
       <c r="C520" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D520" s="1" t="s">
+        <v>790</v>
+      </c>
     </row>
     <row r="521" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B521" s="1" t="s">
@@ -7547,6 +7659,9 @@
       <c r="C521" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D521" s="1" t="s">
+        <v>790</v>
+      </c>
     </row>
     <row r="522" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B522" s="1" t="s">
@@ -7555,6 +7670,9 @@
       <c r="C522" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D522" s="1" t="s">
+        <v>790</v>
+      </c>
     </row>
     <row r="523" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B523" s="1" t="s">
@@ -7574,6 +7692,9 @@
       <c r="C524" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D524" s="1" t="s">
+        <v>790</v>
+      </c>
     </row>
     <row r="525" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B525" s="1" t="s">
@@ -7582,6 +7703,9 @@
       <c r="C525" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D525" s="1" t="s">
+        <v>790</v>
+      </c>
     </row>
     <row r="526" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B526" s="1" t="s">
@@ -7599,7 +7723,7 @@
         <v>526</v>
       </c>
       <c r="C527" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D527" s="1" t="s">
         <v>790</v>
@@ -7610,7 +7734,7 @@
         <v>527</v>
       </c>
       <c r="C528" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D528" s="1" t="s">
         <v>790</v>
@@ -7621,7 +7745,7 @@
         <v>528</v>
       </c>
       <c r="C529" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D529" s="1" t="s">
         <v>790</v>
@@ -7632,7 +7756,7 @@
         <v>529</v>
       </c>
       <c r="C530" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D530" s="1" t="s">
         <v>790</v>
@@ -7643,7 +7767,7 @@
         <v>530</v>
       </c>
       <c r="C531" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D531" s="1" t="s">
         <v>790</v>
@@ -7654,7 +7778,7 @@
         <v>531</v>
       </c>
       <c r="C532" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D532" s="1" t="s">
         <v>790</v>
@@ -7665,7 +7789,7 @@
         <v>532</v>
       </c>
       <c r="C533" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D533" s="1" t="s">
         <v>790</v>
@@ -7676,7 +7800,7 @@
         <v>533</v>
       </c>
       <c r="C534" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D534" s="1" t="s">
         <v>790</v>
@@ -7687,7 +7811,7 @@
         <v>534</v>
       </c>
       <c r="C535" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D535" s="1" t="s">
         <v>790</v>
@@ -7709,7 +7833,7 @@
         <v>536</v>
       </c>
       <c r="C537" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D537" s="1" t="s">
         <v>790</v>
@@ -7720,7 +7844,7 @@
         <v>537</v>
       </c>
       <c r="C538" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D538" s="1" t="s">
         <v>790</v>
@@ -7731,7 +7855,7 @@
         <v>538</v>
       </c>
       <c r="C539" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D539" s="1" t="s">
         <v>790</v>
@@ -7742,7 +7866,7 @@
         <v>539</v>
       </c>
       <c r="C540" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D540" s="1" t="s">
         <v>790</v>
@@ -7753,7 +7877,7 @@
         <v>540</v>
       </c>
       <c r="C541" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D541" s="1" t="s">
         <v>790</v>
@@ -7764,7 +7888,7 @@
         <v>541</v>
       </c>
       <c r="C542" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D542" s="1" t="s">
         <v>790</v>
@@ -7775,7 +7899,7 @@
         <v>542</v>
       </c>
       <c r="C543" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D543" s="1" t="s">
         <v>790</v>
@@ -7786,7 +7910,7 @@
         <v>543</v>
       </c>
       <c r="C544" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D544" s="1" t="s">
         <v>790</v>
@@ -7797,7 +7921,7 @@
         <v>544</v>
       </c>
       <c r="C545" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D545" s="1" t="s">
         <v>790</v>
@@ -7808,7 +7932,7 @@
         <v>545</v>
       </c>
       <c r="C546" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D546" s="1" t="s">
         <v>790</v>
@@ -7819,7 +7943,7 @@
         <v>546</v>
       </c>
       <c r="C547" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D547" s="1" t="s">
         <v>790</v>
@@ -7830,7 +7954,7 @@
         <v>547</v>
       </c>
       <c r="C548" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D548" s="1" t="s">
         <v>790</v>
@@ -7841,7 +7965,7 @@
         <v>548</v>
       </c>
       <c r="C549" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D549" s="1" t="s">
         <v>790</v>
@@ -7852,7 +7976,7 @@
         <v>549</v>
       </c>
       <c r="C550" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D550" s="1" t="s">
         <v>790</v>
@@ -7863,7 +7987,7 @@
         <v>550</v>
       </c>
       <c r="C551" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D551" s="1" t="s">
         <v>790</v>
@@ -7874,7 +7998,7 @@
         <v>551</v>
       </c>
       <c r="C552" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D552" s="1" t="s">
         <v>790</v>
@@ -7885,7 +8009,7 @@
         <v>552</v>
       </c>
       <c r="C553" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D553" s="1" t="s">
         <v>790</v>
@@ -7896,7 +8020,7 @@
         <v>553</v>
       </c>
       <c r="C554" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D554" s="1" t="s">
         <v>790</v>
@@ -7907,7 +8031,7 @@
         <v>554</v>
       </c>
       <c r="C555" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D555" s="1" t="s">
         <v>790</v>
@@ -7918,7 +8042,7 @@
         <v>555</v>
       </c>
       <c r="C556" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D556" s="1" t="s">
         <v>790</v>
@@ -7929,7 +8053,7 @@
         <v>556</v>
       </c>
       <c r="C557" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D557" s="1" t="s">
         <v>790</v>
@@ -10011,12 +10135,12 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="2" operator="equal">
       <formula>"SIM"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="notContainsBlanks" dxfId="0" priority="4">
+    <cfRule type="notContainsBlanks" dxfId="9" priority="4">
       <formula>LEN(TRIM(D1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Traduzido cfarl EV266_us.u16 EV267_us.u16 EV268_us.u16 EV269_us.u16 EV270_us.u16 EV271_us.u16 EV272_us.u16 EV274_us.u16 EV275_us.u16
</commit_message>
<xml_diff>
--- a/arquivos-tradutor.xlsx
+++ b/arquivos-tradutor.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\danger\traducoes\blue-dragon\traducao-blue-dragon-xbox360\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1904" uniqueCount="794">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1914" uniqueCount="794">
   <si>
     <t>Arquivo</t>
   </si>
@@ -2465,7 +2470,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="11">
+  <dxfs count="8">
     <dxf>
       <fill>
         <patternFill>
@@ -2474,6 +2479,9 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
@@ -2481,6 +2489,9 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
@@ -2488,27 +2499,9 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
@@ -2826,7 +2819,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2836,8 +2829,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:D782"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A494" workbookViewId="0">
-      <selection activeCell="D503" sqref="D503"/>
+    <sheetView tabSelected="1" topLeftCell="A737" workbookViewId="0">
+      <selection activeCell="D743" sqref="D743:D751"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7415,7 +7408,7 @@
         <v>498</v>
       </c>
       <c r="C499" s="1" t="s">
-        <v>784</v>
+        <v>789</v>
       </c>
       <c r="D499" s="1" t="s">
         <v>790</v>
@@ -7459,7 +7452,7 @@
         <v>502</v>
       </c>
       <c r="C503" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D503" s="1" t="s">
         <v>790</v>
@@ -7481,7 +7474,7 @@
         <v>504</v>
       </c>
       <c r="C505" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D505" s="1" t="s">
         <v>790</v>
@@ -7492,7 +7485,7 @@
         <v>505</v>
       </c>
       <c r="C506" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D506" s="1" t="s">
         <v>790</v>
@@ -7503,7 +7496,7 @@
         <v>506</v>
       </c>
       <c r="C507" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D507" s="1" t="s">
         <v>790</v>
@@ -7514,7 +7507,7 @@
         <v>507</v>
       </c>
       <c r="C508" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D508" s="1" t="s">
         <v>790</v>
@@ -7547,7 +7540,7 @@
         <v>510</v>
       </c>
       <c r="C511" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D511" s="1" t="s">
         <v>790</v>
@@ -7558,7 +7551,7 @@
         <v>511</v>
       </c>
       <c r="C512" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D512" s="1" t="s">
         <v>790</v>
@@ -7569,7 +7562,7 @@
         <v>512</v>
       </c>
       <c r="C513" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D513" s="1" t="s">
         <v>790</v>
@@ -7580,7 +7573,7 @@
         <v>513</v>
       </c>
       <c r="C514" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D514" s="1" t="s">
         <v>790</v>
@@ -7591,7 +7584,7 @@
         <v>514</v>
       </c>
       <c r="C515" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D515" s="1" t="s">
         <v>790</v>
@@ -7602,7 +7595,7 @@
         <v>515</v>
       </c>
       <c r="C516" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D516" s="1" t="s">
         <v>790</v>
@@ -7613,7 +7606,7 @@
         <v>516</v>
       </c>
       <c r="C517" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D517" s="1" t="s">
         <v>790</v>
@@ -7624,7 +7617,7 @@
         <v>517</v>
       </c>
       <c r="C518" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D518" s="1" t="s">
         <v>790</v>
@@ -7635,7 +7628,7 @@
         <v>518</v>
       </c>
       <c r="C519" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D519" s="1" t="s">
         <v>790</v>
@@ -7646,7 +7639,7 @@
         <v>519</v>
       </c>
       <c r="C520" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D520" s="1" t="s">
         <v>790</v>
@@ -7657,7 +7650,7 @@
         <v>520</v>
       </c>
       <c r="C521" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D521" s="1" t="s">
         <v>790</v>
@@ -7668,7 +7661,7 @@
         <v>521</v>
       </c>
       <c r="C522" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D522" s="1" t="s">
         <v>790</v>
@@ -7690,7 +7683,7 @@
         <v>523</v>
       </c>
       <c r="C524" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D524" s="1" t="s">
         <v>790</v>
@@ -7701,7 +7694,7 @@
         <v>524</v>
       </c>
       <c r="C525" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D525" s="1" t="s">
         <v>790</v>
@@ -9777,6 +9770,9 @@
       <c r="C743" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D743" s="1" t="s">
+        <v>790</v>
+      </c>
     </row>
     <row r="744" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B744" s="1" t="s">
@@ -9785,6 +9781,9 @@
       <c r="C744" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D744" s="1" t="s">
+        <v>790</v>
+      </c>
     </row>
     <row r="745" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B745" s="1" t="s">
@@ -9793,6 +9792,9 @@
       <c r="C745" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D745" s="1" t="s">
+        <v>790</v>
+      </c>
     </row>
     <row r="746" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B746" s="1" t="s">
@@ -9801,6 +9803,9 @@
       <c r="C746" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D746" s="1" t="s">
+        <v>790</v>
+      </c>
     </row>
     <row r="747" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B747" s="1" t="s">
@@ -9809,6 +9814,9 @@
       <c r="C747" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D747" s="1" t="s">
+        <v>790</v>
+      </c>
     </row>
     <row r="748" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B748" s="1" t="s">
@@ -9817,6 +9825,9 @@
       <c r="C748" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D748" s="1" t="s">
+        <v>790</v>
+      </c>
     </row>
     <row r="749" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B749" s="1" t="s">
@@ -9825,6 +9836,9 @@
       <c r="C749" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D749" s="1" t="s">
+        <v>790</v>
+      </c>
     </row>
     <row r="750" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B750" s="1" t="s">
@@ -9833,6 +9847,9 @@
       <c r="C750" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D750" s="1" t="s">
+        <v>790</v>
+      </c>
     </row>
     <row r="751" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B751" s="1" t="s">
@@ -9841,6 +9858,9 @@
       <c r="C751" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D751" s="1" t="s">
+        <v>790</v>
+      </c>
     </row>
     <row r="752" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B752" s="1" t="s">
@@ -9870,6 +9890,9 @@
       </c>
       <c r="C754" s="1" t="s">
         <v>784</v>
+      </c>
+      <c r="D754" s="1" t="s">
+        <v>790</v>
       </c>
     </row>
     <row r="755" spans="2:4" x14ac:dyDescent="0.25">
@@ -10135,12 +10158,12 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="2" operator="equal">
       <formula>"SIM"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="notContainsBlanks" dxfId="9" priority="4">
+    <cfRule type="notContainsBlanks" dxfId="6" priority="4">
       <formula>LEN(TRIM(D1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
traduzidos EV123_us.u16 EV126_us.u16 EV128_us.u16
</commit_message>
<xml_diff>
--- a/arquivos-tradutor.xlsx
+++ b/arquivos-tradutor.xlsx
@@ -2772,8 +2772,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:D782"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A478" workbookViewId="0">
-      <selection activeCell="D485" sqref="D485"/>
+    <sheetView tabSelected="1" topLeftCell="A402" workbookViewId="0">
+      <selection activeCell="C412" sqref="C412"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6334,7 +6334,7 @@
         <v>405</v>
       </c>
       <c r="C406" s="1" t="s">
-        <v>792</v>
+        <v>786</v>
       </c>
       <c r="D406" s="1" t="s">
         <v>785</v>
@@ -6367,7 +6367,7 @@
         <v>408</v>
       </c>
       <c r="C409" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D409" s="1" t="s">
         <v>785</v>
@@ -6389,7 +6389,7 @@
         <v>410</v>
       </c>
       <c r="C411" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D411" s="1" t="s">
         <v>785</v>

</xml_diff>

<commit_message>
Alterada planilha para reserva cfarl
</commit_message>
<xml_diff>
--- a/arquivos-tradutor.xlsx
+++ b/arquivos-tradutor.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Moacyr\Desktop\GITHUB-BD\traducao-blue-dragon-xbox360\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\danger\traducoes\blue-dragon\traducao-blue-dragon-xbox360\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1923" uniqueCount="794">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1943" uniqueCount="794">
   <si>
     <t>Arquivo</t>
   </si>
@@ -2470,7 +2470,34 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="5">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -2772,8 +2799,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:D782"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A402" workbookViewId="0">
-      <selection activeCell="C412" sqref="C412"/>
+    <sheetView tabSelected="1" topLeftCell="A711" workbookViewId="0">
+      <selection activeCell="B721" sqref="B721"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9551,132 +9578,180 @@
         <v>784</v>
       </c>
     </row>
-    <row r="721" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="721" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B721" s="1" t="s">
         <v>720</v>
       </c>
       <c r="C721" s="1" t="s">
         <v>784</v>
       </c>
-    </row>
-    <row r="722" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D721" s="1" t="s">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="722" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B722" s="1" t="s">
         <v>721</v>
       </c>
       <c r="C722" s="1" t="s">
         <v>784</v>
       </c>
-    </row>
-    <row r="723" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D722" s="1" t="s">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="723" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B723" s="1" t="s">
         <v>722</v>
       </c>
       <c r="C723" s="1" t="s">
         <v>784</v>
       </c>
-    </row>
-    <row r="724" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D723" s="1" t="s">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="724" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B724" s="1" t="s">
         <v>723</v>
       </c>
       <c r="C724" s="1" t="s">
         <v>784</v>
       </c>
-    </row>
-    <row r="725" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D724" s="1" t="s">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="725" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B725" s="1" t="s">
         <v>724</v>
       </c>
       <c r="C725" s="1" t="s">
         <v>784</v>
       </c>
-    </row>
-    <row r="726" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D725" s="1" t="s">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="726" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B726" s="1" t="s">
         <v>725</v>
       </c>
       <c r="C726" s="1" t="s">
         <v>784</v>
       </c>
-    </row>
-    <row r="727" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D726" s="1" t="s">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="727" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B727" s="1" t="s">
         <v>726</v>
       </c>
       <c r="C727" s="1" t="s">
         <v>784</v>
       </c>
-    </row>
-    <row r="728" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D727" s="1" t="s">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="728" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B728" s="1" t="s">
         <v>727</v>
       </c>
       <c r="C728" s="1" t="s">
         <v>784</v>
       </c>
-    </row>
-    <row r="729" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D728" s="1" t="s">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="729" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B729" s="1" t="s">
         <v>728</v>
       </c>
       <c r="C729" s="1" t="s">
         <v>784</v>
       </c>
-    </row>
-    <row r="730" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D729" s="1" t="s">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="730" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B730" s="1" t="s">
         <v>729</v>
       </c>
       <c r="C730" s="1" t="s">
         <v>784</v>
       </c>
-    </row>
-    <row r="731" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D730" s="1" t="s">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="731" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B731" s="1" t="s">
         <v>730</v>
       </c>
       <c r="C731" s="1" t="s">
         <v>784</v>
       </c>
-    </row>
-    <row r="732" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D731" s="1" t="s">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="732" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B732" s="1" t="s">
         <v>731</v>
       </c>
       <c r="C732" s="1" t="s">
         <v>784</v>
       </c>
-    </row>
-    <row r="733" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D732" s="1" t="s">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="733" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B733" s="1" t="s">
         <v>732</v>
       </c>
       <c r="C733" s="1" t="s">
         <v>784</v>
       </c>
-    </row>
-    <row r="734" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D733" s="1" t="s">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="734" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B734" s="1" t="s">
         <v>733</v>
       </c>
       <c r="C734" s="1" t="s">
         <v>784</v>
       </c>
-    </row>
-    <row r="735" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D734" s="1" t="s">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="735" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B735" s="1" t="s">
         <v>734</v>
       </c>
       <c r="C735" s="1" t="s">
         <v>784</v>
       </c>
-    </row>
-    <row r="736" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D735" s="1" t="s">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="736" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B736" s="1" t="s">
         <v>735</v>
       </c>
       <c r="C736" s="1" t="s">
         <v>784</v>
+      </c>
+      <c r="D736" s="1" t="s">
+        <v>790</v>
       </c>
     </row>
     <row r="737" spans="2:4" x14ac:dyDescent="0.25">
@@ -9686,6 +9761,9 @@
       <c r="C737" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D737" s="1" t="s">
+        <v>790</v>
+      </c>
     </row>
     <row r="738" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B738" s="1" t="s">
@@ -9694,6 +9772,9 @@
       <c r="C738" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D738" s="1" t="s">
+        <v>790</v>
+      </c>
     </row>
     <row r="739" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B739" s="1" t="s">
@@ -9702,6 +9783,9 @@
       <c r="C739" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D739" s="1" t="s">
+        <v>790</v>
+      </c>
     </row>
     <row r="740" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B740" s="1" t="s">
@@ -9710,6 +9794,9 @@
       <c r="C740" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D740" s="1" t="s">
+        <v>790</v>
+      </c>
     </row>
     <row r="741" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B741" s="1" t="s">
@@ -9738,7 +9825,7 @@
         <v>742</v>
       </c>
       <c r="C743" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D743" s="1" t="s">
         <v>790</v>
@@ -9749,7 +9836,7 @@
         <v>743</v>
       </c>
       <c r="C744" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D744" s="1" t="s">
         <v>790</v>
@@ -9760,7 +9847,7 @@
         <v>744</v>
       </c>
       <c r="C745" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D745" s="1" t="s">
         <v>790</v>
@@ -9771,7 +9858,7 @@
         <v>745</v>
       </c>
       <c r="C746" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D746" s="1" t="s">
         <v>790</v>
@@ -9782,7 +9869,7 @@
         <v>746</v>
       </c>
       <c r="C747" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D747" s="1" t="s">
         <v>790</v>
@@ -9793,7 +9880,7 @@
         <v>747</v>
       </c>
       <c r="C748" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D748" s="1" t="s">
         <v>790</v>
@@ -9804,7 +9891,7 @@
         <v>748</v>
       </c>
       <c r="C749" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D749" s="1" t="s">
         <v>790</v>
@@ -9815,7 +9902,7 @@
         <v>749</v>
       </c>
       <c r="C750" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D750" s="1" t="s">
         <v>790</v>
@@ -9826,7 +9913,7 @@
         <v>750</v>
       </c>
       <c r="C751" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D751" s="1" t="s">
         <v>790</v>
@@ -9859,7 +9946,7 @@
         <v>753</v>
       </c>
       <c r="C754" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D754" s="1" t="s">
         <v>790</v>
@@ -10128,12 +10215,12 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
       <formula>"SIM"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="notContainsBlanks" dxfId="0" priority="4">
+    <cfRule type="notContainsBlanks" dxfId="3" priority="4">
       <formula>LEN(TRIM(D1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Traduzidos cfarl mes_dg29_01_us.u16 mes_dg29_02_us.u16
</commit_message>
<xml_diff>
--- a/arquivos-tradutor.xlsx
+++ b/arquivos-tradutor.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Moacyr\Desktop\GITHUB-BD\traducao-blue-dragon-xbox360\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\danger\traducoes\blue-dragon\traducao-blue-dragon-xbox360\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -2470,7 +2470,17 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -2772,8 +2782,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:D782"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A602" workbookViewId="0">
-      <selection activeCell="C624" sqref="C624"/>
+    <sheetView tabSelected="1" topLeftCell="A680" workbookViewId="0">
+      <selection activeCell="C741" sqref="C721:C741"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9598,7 +9608,7 @@
         <v>720</v>
       </c>
       <c r="C721" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D721" s="1" t="s">
         <v>790</v>
@@ -9609,7 +9619,7 @@
         <v>721</v>
       </c>
       <c r="C722" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D722" s="1" t="s">
         <v>790</v>
@@ -9620,7 +9630,7 @@
         <v>722</v>
       </c>
       <c r="C723" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D723" s="1" t="s">
         <v>790</v>
@@ -9631,7 +9641,7 @@
         <v>723</v>
       </c>
       <c r="C724" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D724" s="1" t="s">
         <v>790</v>
@@ -9642,7 +9652,7 @@
         <v>724</v>
       </c>
       <c r="C725" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D725" s="1" t="s">
         <v>790</v>
@@ -9653,7 +9663,7 @@
         <v>725</v>
       </c>
       <c r="C726" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D726" s="1" t="s">
         <v>790</v>
@@ -9664,7 +9674,7 @@
         <v>726</v>
       </c>
       <c r="C727" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D727" s="1" t="s">
         <v>790</v>
@@ -9675,7 +9685,7 @@
         <v>727</v>
       </c>
       <c r="C728" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D728" s="1" t="s">
         <v>790</v>
@@ -9686,7 +9696,7 @@
         <v>728</v>
       </c>
       <c r="C729" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D729" s="1" t="s">
         <v>790</v>
@@ -9697,7 +9707,7 @@
         <v>729</v>
       </c>
       <c r="C730" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D730" s="1" t="s">
         <v>790</v>
@@ -9708,7 +9718,7 @@
         <v>730</v>
       </c>
       <c r="C731" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D731" s="1" t="s">
         <v>790</v>
@@ -9719,7 +9729,7 @@
         <v>731</v>
       </c>
       <c r="C732" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D732" s="1" t="s">
         <v>790</v>
@@ -9730,7 +9740,7 @@
         <v>732</v>
       </c>
       <c r="C733" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D733" s="1" t="s">
         <v>790</v>
@@ -9741,7 +9751,7 @@
         <v>733</v>
       </c>
       <c r="C734" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D734" s="1" t="s">
         <v>790</v>
@@ -9752,7 +9762,7 @@
         <v>734</v>
       </c>
       <c r="C735" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D735" s="1" t="s">
         <v>790</v>
@@ -9763,7 +9773,7 @@
         <v>735</v>
       </c>
       <c r="C736" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D736" s="1" t="s">
         <v>790</v>
@@ -9774,7 +9784,7 @@
         <v>736</v>
       </c>
       <c r="C737" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D737" s="1" t="s">
         <v>790</v>
@@ -9785,7 +9795,7 @@
         <v>737</v>
       </c>
       <c r="C738" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D738" s="1" t="s">
         <v>790</v>
@@ -9796,7 +9806,7 @@
         <v>738</v>
       </c>
       <c r="C739" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D739" s="1" t="s">
         <v>790</v>
@@ -9807,7 +9817,7 @@
         <v>739</v>
       </c>
       <c r="C740" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D740" s="1" t="s">
         <v>790</v>
@@ -10230,12 +10240,12 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>"SIM"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="notContainsBlanks" dxfId="0" priority="4">
+    <cfRule type="notContainsBlanks" dxfId="1" priority="4">
       <formula>LEN(TRIM(D1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Reservados arquivos para cfarl
</commit_message>
<xml_diff>
--- a/arquivos-tradutor.xlsx
+++ b/arquivos-tradutor.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1957" uniqueCount="794">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1987" uniqueCount="794">
   <si>
     <t>Arquivo</t>
   </si>
@@ -2470,11 +2470,15 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="4">
     <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
@@ -2782,8 +2786,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:D782"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A680" workbookViewId="0">
-      <selection activeCell="C741" sqref="C721:C741"/>
+    <sheetView tabSelected="1" topLeftCell="A581" workbookViewId="0">
+      <selection activeCell="D665" sqref="D665:D692"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9084,6 +9088,9 @@
       <c r="C665" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D665" s="1" t="s">
+        <v>790</v>
+      </c>
     </row>
     <row r="666" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B666" s="1" t="s">
@@ -9092,6 +9099,9 @@
       <c r="C666" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D666" s="1" t="s">
+        <v>790</v>
+      </c>
     </row>
     <row r="667" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B667" s="1" t="s">
@@ -9100,6 +9110,9 @@
       <c r="C667" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D667" s="1" t="s">
+        <v>790</v>
+      </c>
     </row>
     <row r="668" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B668" s="1" t="s">
@@ -9108,6 +9121,9 @@
       <c r="C668" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D668" s="1" t="s">
+        <v>790</v>
+      </c>
     </row>
     <row r="669" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B669" s="1" t="s">
@@ -9116,6 +9132,9 @@
       <c r="C669" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D669" s="1" t="s">
+        <v>790</v>
+      </c>
     </row>
     <row r="670" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B670" s="1" t="s">
@@ -9124,6 +9143,9 @@
       <c r="C670" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D670" s="1" t="s">
+        <v>790</v>
+      </c>
     </row>
     <row r="671" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B671" s="1" t="s">
@@ -9132,6 +9154,9 @@
       <c r="C671" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D671" s="1" t="s">
+        <v>790</v>
+      </c>
     </row>
     <row r="672" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B672" s="1" t="s">
@@ -9140,133 +9165,184 @@
       <c r="C672" s="1" t="s">
         <v>784</v>
       </c>
-    </row>
-    <row r="673" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D672" s="1" t="s">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="673" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B673" s="1" t="s">
         <v>672</v>
       </c>
       <c r="C673" s="1" t="s">
         <v>784</v>
       </c>
-    </row>
-    <row r="674" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D673" s="1" t="s">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="674" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B674" s="1" t="s">
         <v>673</v>
       </c>
       <c r="C674" s="1" t="s">
         <v>784</v>
       </c>
-    </row>
-    <row r="675" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D674" s="1" t="s">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="675" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B675" s="1" t="s">
         <v>674</v>
       </c>
       <c r="C675" s="1" t="s">
         <v>784</v>
       </c>
-    </row>
-    <row r="676" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D675" s="1" t="s">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="676" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B676" s="1" t="s">
         <v>675</v>
       </c>
       <c r="C676" s="1" t="s">
         <v>784</v>
       </c>
-    </row>
-    <row r="677" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D676" s="1" t="s">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="677" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B677" s="1" t="s">
         <v>676</v>
       </c>
       <c r="C677" s="1" t="s">
         <v>784</v>
       </c>
-    </row>
-    <row r="678" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D677" s="1" t="s">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="678" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B678" s="1" t="s">
         <v>677</v>
       </c>
       <c r="C678" s="1" t="s">
         <v>784</v>
       </c>
-    </row>
-    <row r="679" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D678" s="1" t="s">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="679" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B679" s="1" t="s">
         <v>678</v>
       </c>
       <c r="C679" s="1" t="s">
         <v>784</v>
       </c>
-    </row>
-    <row r="680" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D679" s="1" t="s">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="680" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B680" s="1" t="s">
         <v>679</v>
       </c>
       <c r="C680" s="1" t="s">
         <v>784</v>
       </c>
-    </row>
-    <row r="681" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D680" s="1" t="s">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="681" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B681" s="1" t="s">
         <v>680</v>
       </c>
       <c r="C681" s="1" t="s">
         <v>784</v>
       </c>
-    </row>
-    <row r="682" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D681" s="1" t="s">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="682" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B682" s="1" t="s">
         <v>681</v>
       </c>
       <c r="C682" s="1" t="s">
         <v>784</v>
       </c>
-    </row>
-    <row r="683" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D682" s="1" t="s">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="683" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B683" s="1" t="s">
         <v>682</v>
       </c>
       <c r="C683" s="1" t="s">
         <v>784</v>
       </c>
-    </row>
-    <row r="684" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D683" s="1" t="s">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="684" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B684" s="1" t="s">
         <v>683</v>
       </c>
       <c r="C684" s="1" t="s">
         <v>784</v>
       </c>
-    </row>
-    <row r="685" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D684" s="1" t="s">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="685" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B685" s="1" t="s">
         <v>684</v>
       </c>
       <c r="C685" s="1" t="s">
         <v>784</v>
       </c>
-    </row>
-    <row r="686" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D685" s="1" t="s">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="686" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B686" s="1" t="s">
         <v>685</v>
       </c>
       <c r="C686" s="1" t="s">
         <v>784</v>
       </c>
-    </row>
-    <row r="687" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D686" s="1" t="s">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="687" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B687" s="1" t="s">
         <v>686</v>
       </c>
       <c r="C687" s="1" t="s">
         <v>784</v>
       </c>
-    </row>
-    <row r="688" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D687" s="1" t="s">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="688" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B688" s="1" t="s">
         <v>687</v>
       </c>
       <c r="C688" s="1" t="s">
         <v>784</v>
+      </c>
+      <c r="D688" s="1" t="s">
+        <v>790</v>
       </c>
     </row>
     <row r="689" spans="2:4" x14ac:dyDescent="0.25">
@@ -9276,6 +9352,9 @@
       <c r="C689" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D689" s="1" t="s">
+        <v>790</v>
+      </c>
     </row>
     <row r="690" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B690" s="1" t="s">
@@ -9284,6 +9363,9 @@
       <c r="C690" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D690" s="1" t="s">
+        <v>790</v>
+      </c>
     </row>
     <row r="691" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B691" s="1" t="s">
@@ -9292,6 +9374,9 @@
       <c r="C691" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D691" s="1" t="s">
+        <v>790</v>
+      </c>
     </row>
     <row r="692" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B692" s="1" t="s">
@@ -9300,6 +9385,9 @@
       <c r="C692" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D692" s="1" t="s">
+        <v>790</v>
+      </c>
     </row>
     <row r="693" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B693" s="1" t="s">
@@ -9594,6 +9682,9 @@
       <c r="C719" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D719" s="1" t="s">
+        <v>790</v>
+      </c>
     </row>
     <row r="720" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B720" s="1" t="s">
@@ -9601,6 +9692,9 @@
       </c>
       <c r="C720" s="1" t="s">
         <v>784</v>
+      </c>
+      <c r="D720" s="1" t="s">
+        <v>790</v>
       </c>
     </row>
     <row r="721" spans="2:4" x14ac:dyDescent="0.25">
@@ -10240,12 +10334,12 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
       <formula>"SIM"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="notContainsBlanks" dxfId="1" priority="4">
+    <cfRule type="notContainsBlanks" dxfId="2" priority="4">
       <formula>LEN(TRIM(D1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
traduzidos EV185_us.u16 EV514_us.u16 EV515_us.u16
</commit_message>
<xml_diff>
--- a/arquivos-tradutor.xlsx
+++ b/arquivos-tradutor.xlsx
@@ -2772,8 +2772,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:D782"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A442" workbookViewId="0">
-      <selection activeCell="C453" sqref="C453"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="C610" sqref="C610"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6807,7 +6807,7 @@
         <v>448</v>
       </c>
       <c r="C449" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D449" s="1" t="s">
         <v>785</v>
@@ -8545,7 +8545,7 @@
         <v>606</v>
       </c>
       <c r="C607" s="1" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="D607" s="1" t="s">
         <v>785</v>
@@ -8556,7 +8556,7 @@
         <v>607</v>
       </c>
       <c r="C608" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D608" s="1" t="s">
         <v>785</v>
@@ -8567,7 +8567,7 @@
         <v>608</v>
       </c>
       <c r="C609" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D609" s="1" t="s">
         <v>785</v>

</xml_diff>

<commit_message>
Reservados arquivos. temp cfarl
</commit_message>
<xml_diff>
--- a/arquivos-tradutor.xlsx
+++ b/arquivos-tradutor.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Moacyr\Desktop\GITHUB-BD\traducao-blue-dragon-xbox360\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\danger\traducoes\traducao-blue-dragon-xbox360\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1991" uniqueCount="794">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2007" uniqueCount="794">
   <si>
     <t>Arquivo</t>
   </si>
@@ -2470,7 +2470,51 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="7">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -2772,8 +2816,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:D782"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A625" workbookViewId="0">
-      <selection activeCell="D629" sqref="D629"/>
+    <sheetView tabSelected="1" topLeftCell="A679" workbookViewId="0">
+      <selection activeCell="C665" sqref="C665"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8938,6 +8982,9 @@
       <c r="C648" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D648" s="1" t="s">
+        <v>790</v>
+      </c>
     </row>
     <row r="649" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B649" s="1" t="s">
@@ -8946,6 +8993,9 @@
       <c r="C649" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D649" s="1" t="s">
+        <v>790</v>
+      </c>
     </row>
     <row r="650" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B650" s="1" t="s">
@@ -8954,6 +9004,9 @@
       <c r="C650" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D650" s="1" t="s">
+        <v>790</v>
+      </c>
     </row>
     <row r="651" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B651" s="1" t="s">
@@ -8962,6 +9015,9 @@
       <c r="C651" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D651" s="1" t="s">
+        <v>790</v>
+      </c>
     </row>
     <row r="652" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B652" s="1" t="s">
@@ -8970,6 +9026,9 @@
       <c r="C652" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D652" s="1" t="s">
+        <v>790</v>
+      </c>
     </row>
     <row r="653" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B653" s="1" t="s">
@@ -8978,6 +9037,9 @@
       <c r="C653" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D653" s="1" t="s">
+        <v>790</v>
+      </c>
     </row>
     <row r="654" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B654" s="1" t="s">
@@ -8986,6 +9048,9 @@
       <c r="C654" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D654" s="1" t="s">
+        <v>790</v>
+      </c>
     </row>
     <row r="655" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B655" s="1" t="s">
@@ -8994,6 +9059,9 @@
       <c r="C655" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D655" s="1" t="s">
+        <v>790</v>
+      </c>
     </row>
     <row r="656" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B656" s="1" t="s">
@@ -9002,6 +9070,9 @@
       <c r="C656" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D656" s="1" t="s">
+        <v>790</v>
+      </c>
     </row>
     <row r="657" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B657" s="1" t="s">
@@ -9010,6 +9081,9 @@
       <c r="C657" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D657" s="1" t="s">
+        <v>790</v>
+      </c>
     </row>
     <row r="658" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B658" s="1" t="s">
@@ -9018,6 +9092,9 @@
       <c r="C658" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D658" s="1" t="s">
+        <v>790</v>
+      </c>
     </row>
     <row r="659" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B659" s="1" t="s">
@@ -9026,6 +9103,9 @@
       <c r="C659" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D659" s="1" t="s">
+        <v>790</v>
+      </c>
     </row>
     <row r="660" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B660" s="1" t="s">
@@ -9034,6 +9114,9 @@
       <c r="C660" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D660" s="1" t="s">
+        <v>790</v>
+      </c>
     </row>
     <row r="661" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B661" s="1" t="s">
@@ -9042,6 +9125,9 @@
       <c r="C661" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D661" s="1" t="s">
+        <v>790</v>
+      </c>
     </row>
     <row r="662" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B662" s="1" t="s">
@@ -9050,6 +9136,9 @@
       <c r="C662" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D662" s="1" t="s">
+        <v>790</v>
+      </c>
     </row>
     <row r="663" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B663" s="1" t="s">
@@ -9058,6 +9147,9 @@
       <c r="C663" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="D663" s="1" t="s">
+        <v>790</v>
+      </c>
     </row>
     <row r="664" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B664" s="1" t="s">
@@ -9075,7 +9167,7 @@
         <v>664</v>
       </c>
       <c r="C665" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D665" s="1" t="s">
         <v>790</v>
@@ -9086,7 +9178,7 @@
         <v>665</v>
       </c>
       <c r="C666" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D666" s="1" t="s">
         <v>790</v>
@@ -9097,7 +9189,7 @@
         <v>666</v>
       </c>
       <c r="C667" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D667" s="1" t="s">
         <v>790</v>
@@ -9108,7 +9200,7 @@
         <v>667</v>
       </c>
       <c r="C668" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D668" s="1" t="s">
         <v>790</v>
@@ -9119,7 +9211,7 @@
         <v>668</v>
       </c>
       <c r="C669" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D669" s="1" t="s">
         <v>790</v>
@@ -9130,7 +9222,7 @@
         <v>669</v>
       </c>
       <c r="C670" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D670" s="1" t="s">
         <v>790</v>
@@ -9141,7 +9233,7 @@
         <v>670</v>
       </c>
       <c r="C671" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D671" s="1" t="s">
         <v>790</v>
@@ -9152,7 +9244,7 @@
         <v>671</v>
       </c>
       <c r="C672" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D672" s="1" t="s">
         <v>790</v>
@@ -9163,7 +9255,7 @@
         <v>672</v>
       </c>
       <c r="C673" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D673" s="1" t="s">
         <v>790</v>
@@ -9174,7 +9266,7 @@
         <v>673</v>
       </c>
       <c r="C674" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D674" s="1" t="s">
         <v>790</v>
@@ -9185,7 +9277,7 @@
         <v>674</v>
       </c>
       <c r="C675" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D675" s="1" t="s">
         <v>790</v>
@@ -9196,7 +9288,7 @@
         <v>675</v>
       </c>
       <c r="C676" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D676" s="1" t="s">
         <v>790</v>
@@ -9207,7 +9299,7 @@
         <v>676</v>
       </c>
       <c r="C677" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D677" s="1" t="s">
         <v>790</v>
@@ -9218,7 +9310,7 @@
         <v>677</v>
       </c>
       <c r="C678" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D678" s="1" t="s">
         <v>790</v>
@@ -9229,7 +9321,7 @@
         <v>678</v>
       </c>
       <c r="C679" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D679" s="1" t="s">
         <v>790</v>
@@ -9240,7 +9332,7 @@
         <v>679</v>
       </c>
       <c r="C680" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D680" s="1" t="s">
         <v>790</v>
@@ -9251,7 +9343,7 @@
         <v>680</v>
       </c>
       <c r="C681" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D681" s="1" t="s">
         <v>790</v>
@@ -9262,7 +9354,7 @@
         <v>681</v>
       </c>
       <c r="C682" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D682" s="1" t="s">
         <v>790</v>
@@ -9273,7 +9365,7 @@
         <v>682</v>
       </c>
       <c r="C683" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D683" s="1" t="s">
         <v>790</v>
@@ -9284,7 +9376,7 @@
         <v>683</v>
       </c>
       <c r="C684" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D684" s="1" t="s">
         <v>790</v>
@@ -9295,7 +9387,7 @@
         <v>684</v>
       </c>
       <c r="C685" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D685" s="1" t="s">
         <v>790</v>
@@ -9328,7 +9420,7 @@
         <v>687</v>
       </c>
       <c r="C688" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D688" s="1" t="s">
         <v>790</v>
@@ -9339,7 +9431,7 @@
         <v>688</v>
       </c>
       <c r="C689" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D689" s="1" t="s">
         <v>790</v>
@@ -9350,7 +9442,7 @@
         <v>689</v>
       </c>
       <c r="C690" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D690" s="1" t="s">
         <v>790</v>
@@ -9361,7 +9453,7 @@
         <v>690</v>
       </c>
       <c r="C691" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D691" s="1" t="s">
         <v>790</v>
@@ -9372,7 +9464,7 @@
         <v>691</v>
       </c>
       <c r="C692" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D692" s="1" t="s">
         <v>790</v>
@@ -9669,7 +9761,7 @@
         <v>718</v>
       </c>
       <c r="C719" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D719" s="1" t="s">
         <v>790</v>
@@ -9680,7 +9772,7 @@
         <v>719</v>
       </c>
       <c r="C720" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D720" s="1" t="s">
         <v>790</v>
@@ -10332,12 +10424,12 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
       <formula>"SIM"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="notContainsBlanks" dxfId="0" priority="4">
+    <cfRule type="notContainsBlanks" dxfId="5" priority="4">
       <formula>LEN(TRIM(D1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Traduzidos cfarl mes_dg16_01_us.u16 mes_dg17_01_us.u16
</commit_message>
<xml_diff>
--- a/arquivos-tradutor.xlsx
+++ b/arquivos-tradutor.xlsx
@@ -2470,41 +2470,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -2816,8 +2782,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:D782"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A679" workbookViewId="0">
-      <selection activeCell="C665" sqref="C665"/>
+    <sheetView tabSelected="1" topLeftCell="A676" workbookViewId="0">
+      <selection activeCell="C685" sqref="C685:C687"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9398,7 +9364,7 @@
         <v>685</v>
       </c>
       <c r="C686" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D686" s="1" t="s">
         <v>790</v>
@@ -9409,7 +9375,7 @@
         <v>686</v>
       </c>
       <c r="C687" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D687" s="1" t="s">
         <v>790</v>
@@ -10424,12 +10390,12 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>"SIM"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="notContainsBlanks" dxfId="5" priority="4">
+    <cfRule type="notContainsBlanks" dxfId="1" priority="4">
       <formula>LEN(TRIM(D1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Reservados todos arquivos bg di e db para cfarl.
</commit_message>
<xml_diff>
--- a/arquivos-tradutor.xlsx
+++ b/arquivos-tradutor.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2020" uniqueCount="793">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2315" uniqueCount="793">
   <si>
     <t>Arquivo</t>
   </si>
@@ -2467,7 +2467,31 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="5">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -2770,7 +2794,7 @@
   <dimension ref="B1:D781"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C663" sqref="C663"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2875,6 +2899,9 @@
       <c r="C9" s="1" t="s">
         <v>783</v>
       </c>
+      <c r="D9" s="1" t="s">
+        <v>789</v>
+      </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
@@ -2883,6 +2910,9 @@
       <c r="C10" s="1" t="s">
         <v>783</v>
       </c>
+      <c r="D10" s="1" t="s">
+        <v>789</v>
+      </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
@@ -2891,6 +2921,9 @@
       <c r="C11" s="1" t="s">
         <v>783</v>
       </c>
+      <c r="D11" s="1" t="s">
+        <v>789</v>
+      </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
@@ -2899,6 +2932,9 @@
       <c r="C12" s="1" t="s">
         <v>783</v>
       </c>
+      <c r="D12" s="1" t="s">
+        <v>789</v>
+      </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
@@ -2907,6 +2943,9 @@
       <c r="C13" s="1" t="s">
         <v>783</v>
       </c>
+      <c r="D13" s="1" t="s">
+        <v>789</v>
+      </c>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
@@ -2915,6 +2954,9 @@
       <c r="C14" s="1" t="s">
         <v>783</v>
       </c>
+      <c r="D14" s="1" t="s">
+        <v>789</v>
+      </c>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
@@ -2923,6 +2965,9 @@
       <c r="C15" s="1" t="s">
         <v>783</v>
       </c>
+      <c r="D15" s="1" t="s">
+        <v>789</v>
+      </c>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
@@ -2931,1680 +2976,2310 @@
       <c r="C16" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D16" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D17" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D18" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D19" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D20" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D21" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D22" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B23" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D23" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B24" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D24" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B25" s="1" t="s">
         <v>24</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D25" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B26" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D26" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B27" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D27" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B28" s="1" t="s">
         <v>27</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D28" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B29" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D29" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B30" s="1" t="s">
         <v>29</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D30" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B31" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D31" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B32" s="1" t="s">
         <v>31</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D32" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B33" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D33" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B34" s="1" t="s">
         <v>33</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D34" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B35" s="1" t="s">
         <v>34</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D35" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B36" s="1" t="s">
         <v>35</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D36" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B37" s="1" t="s">
         <v>36</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D37" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B38" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D38" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B39" s="1" t="s">
         <v>38</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D39" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B40" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D40" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B41" s="1" t="s">
         <v>40</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="42" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D41" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B42" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="43" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D42" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B43" s="1" t="s">
         <v>42</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="44" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D43" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B44" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="45" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D44" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B45" s="1" t="s">
         <v>44</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="46" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D45" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B46" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="47" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D46" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="47" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B47" s="1" t="s">
         <v>46</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="48" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D47" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="48" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B48" s="1" t="s">
         <v>47</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D48" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B49" s="1" t="s">
         <v>48</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D49" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B50" s="1" t="s">
         <v>49</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="51" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D50" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B51" s="1" t="s">
         <v>50</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="52" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D51" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B52" s="1" t="s">
         <v>51</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="53" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D52" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="53" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B53" s="1" t="s">
         <v>52</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="54" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D53" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="54" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B54" s="1" t="s">
         <v>53</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="55" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D54" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="55" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B55" s="1" t="s">
         <v>54</v>
       </c>
       <c r="C55" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="56" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D55" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="56" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B56" s="1" t="s">
         <v>55</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="57" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D56" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="57" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B57" s="1" t="s">
         <v>56</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="58" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D57" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="58" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B58" s="1" t="s">
         <v>57</v>
       </c>
       <c r="C58" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="59" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D58" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="59" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B59" s="1" t="s">
         <v>58</v>
       </c>
       <c r="C59" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="60" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D59" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="60" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B60" s="1" t="s">
         <v>59</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="61" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D60" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="61" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B61" s="1" t="s">
         <v>60</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="62" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D61" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="62" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B62" s="1" t="s">
         <v>61</v>
       </c>
       <c r="C62" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="63" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D62" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="63" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B63" s="1" t="s">
         <v>62</v>
       </c>
       <c r="C63" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="64" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D63" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="64" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B64" s="1" t="s">
         <v>63</v>
       </c>
       <c r="C64" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="65" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D64" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="65" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B65" s="1" t="s">
         <v>64</v>
       </c>
       <c r="C65" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="66" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D65" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="66" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B66" s="1" t="s">
         <v>65</v>
       </c>
       <c r="C66" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="67" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D66" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="67" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B67" s="1" t="s">
         <v>66</v>
       </c>
       <c r="C67" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="68" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D67" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="68" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B68" s="1" t="s">
         <v>67</v>
       </c>
       <c r="C68" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="69" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D68" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="69" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B69" s="1" t="s">
         <v>68</v>
       </c>
       <c r="C69" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="70" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D69" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="70" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B70" s="1" t="s">
         <v>69</v>
       </c>
       <c r="C70" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="71" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D70" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="71" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B71" s="1" t="s">
         <v>70</v>
       </c>
       <c r="C71" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="72" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D71" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="72" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B72" s="1" t="s">
         <v>71</v>
       </c>
       <c r="C72" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="73" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D72" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="73" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B73" s="1" t="s">
         <v>72</v>
       </c>
       <c r="C73" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="74" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D73" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="74" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B74" s="1" t="s">
         <v>73</v>
       </c>
       <c r="C74" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="75" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D74" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="75" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B75" s="1" t="s">
         <v>74</v>
       </c>
       <c r="C75" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="76" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D75" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="76" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B76" s="1" t="s">
         <v>75</v>
       </c>
       <c r="C76" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="77" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D76" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="77" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B77" s="1" t="s">
         <v>76</v>
       </c>
       <c r="C77" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="78" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D77" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="78" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B78" s="1" t="s">
         <v>77</v>
       </c>
       <c r="C78" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="79" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D78" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="79" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B79" s="1" t="s">
         <v>78</v>
       </c>
       <c r="C79" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="80" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D79" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="80" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B80" s="1" t="s">
         <v>79</v>
       </c>
       <c r="C80" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="81" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D80" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="81" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B81" s="1" t="s">
         <v>80</v>
       </c>
       <c r="C81" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="82" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D81" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="82" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B82" s="1" t="s">
         <v>81</v>
       </c>
       <c r="C82" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="83" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D82" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="83" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B83" s="1" t="s">
         <v>82</v>
       </c>
       <c r="C83" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="84" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D83" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="84" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B84" s="1" t="s">
         <v>83</v>
       </c>
       <c r="C84" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="85" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D84" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="85" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B85" s="1" t="s">
         <v>84</v>
       </c>
       <c r="C85" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="86" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D85" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="86" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B86" s="1" t="s">
         <v>85</v>
       </c>
       <c r="C86" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="87" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D86" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="87" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B87" s="1" t="s">
         <v>86</v>
       </c>
       <c r="C87" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="88" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D87" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="88" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B88" s="1" t="s">
         <v>87</v>
       </c>
       <c r="C88" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="89" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D88" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="89" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B89" s="1" t="s">
         <v>88</v>
       </c>
       <c r="C89" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="90" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D89" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="90" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B90" s="1" t="s">
         <v>89</v>
       </c>
       <c r="C90" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="91" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D90" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="91" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B91" s="1" t="s">
         <v>90</v>
       </c>
       <c r="C91" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="92" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D91" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="92" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B92" s="1" t="s">
         <v>91</v>
       </c>
       <c r="C92" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="93" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D92" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="93" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B93" s="1" t="s">
         <v>92</v>
       </c>
       <c r="C93" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="94" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D93" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="94" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B94" s="1" t="s">
         <v>93</v>
       </c>
       <c r="C94" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="95" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D94" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="95" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B95" s="1" t="s">
         <v>94</v>
       </c>
       <c r="C95" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="96" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D95" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="96" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B96" s="1" t="s">
         <v>95</v>
       </c>
       <c r="C96" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="97" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D96" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="97" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B97" s="1" t="s">
         <v>96</v>
       </c>
       <c r="C97" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="98" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D97" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="98" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B98" s="1" t="s">
         <v>97</v>
       </c>
       <c r="C98" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="99" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D98" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="99" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B99" s="1" t="s">
         <v>98</v>
       </c>
       <c r="C99" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="100" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D99" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="100" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B100" s="1" t="s">
         <v>99</v>
       </c>
       <c r="C100" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="101" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D100" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="101" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B101" s="1" t="s">
         <v>100</v>
       </c>
       <c r="C101" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="102" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D101" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="102" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B102" s="1" t="s">
         <v>101</v>
       </c>
       <c r="C102" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="103" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D102" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="103" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B103" s="1" t="s">
         <v>102</v>
       </c>
       <c r="C103" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="104" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D103" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="104" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B104" s="1" t="s">
         <v>103</v>
       </c>
       <c r="C104" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="105" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D104" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="105" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B105" s="1" t="s">
         <v>104</v>
       </c>
       <c r="C105" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="106" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D105" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="106" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B106" s="1" t="s">
         <v>105</v>
       </c>
       <c r="C106" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="107" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D106" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="107" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B107" s="1" t="s">
         <v>106</v>
       </c>
       <c r="C107" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="108" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D107" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="108" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B108" s="1" t="s">
         <v>107</v>
       </c>
       <c r="C108" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="109" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D108" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="109" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B109" s="1" t="s">
         <v>108</v>
       </c>
       <c r="C109" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="110" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D109" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="110" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B110" s="1" t="s">
         <v>109</v>
       </c>
       <c r="C110" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="111" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D110" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="111" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B111" s="1" t="s">
         <v>110</v>
       </c>
       <c r="C111" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="112" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D111" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="112" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B112" s="1" t="s">
         <v>111</v>
       </c>
       <c r="C112" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="113" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D112" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="113" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B113" s="1" t="s">
         <v>112</v>
       </c>
       <c r="C113" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="114" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D113" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="114" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B114" s="1" t="s">
         <v>113</v>
       </c>
       <c r="C114" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="115" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D114" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="115" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B115" s="1" t="s">
         <v>114</v>
       </c>
       <c r="C115" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="116" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D115" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="116" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B116" s="1" t="s">
         <v>115</v>
       </c>
       <c r="C116" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="117" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D116" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="117" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B117" s="1" t="s">
         <v>116</v>
       </c>
       <c r="C117" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="118" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D117" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="118" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B118" s="1" t="s">
         <v>117</v>
       </c>
       <c r="C118" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="119" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D118" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="119" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B119" s="1" t="s">
         <v>118</v>
       </c>
       <c r="C119" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="120" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D119" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="120" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B120" s="1" t="s">
         <v>119</v>
       </c>
       <c r="C120" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="121" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D120" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="121" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B121" s="1" t="s">
         <v>120</v>
       </c>
       <c r="C121" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="122" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D121" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="122" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B122" s="1" t="s">
         <v>121</v>
       </c>
       <c r="C122" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="123" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D122" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="123" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B123" s="1" t="s">
         <v>122</v>
       </c>
       <c r="C123" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="124" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D123" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="124" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B124" s="1" t="s">
         <v>123</v>
       </c>
       <c r="C124" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="125" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D124" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="125" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B125" s="1" t="s">
         <v>124</v>
       </c>
       <c r="C125" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="126" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D125" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="126" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B126" s="1" t="s">
         <v>125</v>
       </c>
       <c r="C126" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="127" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D126" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="127" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B127" s="1" t="s">
         <v>126</v>
       </c>
       <c r="C127" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="128" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D127" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="128" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B128" s="1" t="s">
         <v>127</v>
       </c>
       <c r="C128" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="129" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D128" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="129" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B129" s="1" t="s">
         <v>128</v>
       </c>
       <c r="C129" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="130" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D129" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="130" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B130" s="1" t="s">
         <v>129</v>
       </c>
       <c r="C130" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="131" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D130" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="131" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B131" s="1" t="s">
         <v>130</v>
       </c>
       <c r="C131" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="132" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D131" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="132" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B132" s="1" t="s">
         <v>131</v>
       </c>
       <c r="C132" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="133" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D132" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="133" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B133" s="1" t="s">
         <v>132</v>
       </c>
       <c r="C133" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="134" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D133" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="134" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B134" s="1" t="s">
         <v>133</v>
       </c>
       <c r="C134" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="135" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D134" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="135" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B135" s="1" t="s">
         <v>134</v>
       </c>
       <c r="C135" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="136" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D135" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="136" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B136" s="1" t="s">
         <v>135</v>
       </c>
       <c r="C136" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="137" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D136" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="137" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B137" s="1" t="s">
         <v>136</v>
       </c>
       <c r="C137" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="138" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D137" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="138" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B138" s="1" t="s">
         <v>137</v>
       </c>
       <c r="C138" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="139" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D138" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="139" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B139" s="1" t="s">
         <v>138</v>
       </c>
       <c r="C139" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="140" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D139" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="140" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B140" s="1" t="s">
         <v>139</v>
       </c>
       <c r="C140" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="141" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D140" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="141" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B141" s="1" t="s">
         <v>140</v>
       </c>
       <c r="C141" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="142" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D141" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="142" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B142" s="1" t="s">
         <v>141</v>
       </c>
       <c r="C142" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="143" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D142" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="143" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B143" s="1" t="s">
         <v>142</v>
       </c>
       <c r="C143" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="144" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D143" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="144" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B144" s="1" t="s">
         <v>143</v>
       </c>
       <c r="C144" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="145" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D144" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="145" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B145" s="1" t="s">
         <v>144</v>
       </c>
       <c r="C145" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="146" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D145" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="146" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B146" s="1" t="s">
         <v>145</v>
       </c>
       <c r="C146" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="147" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D146" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="147" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B147" s="1" t="s">
         <v>146</v>
       </c>
       <c r="C147" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="148" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D147" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="148" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B148" s="1" t="s">
         <v>147</v>
       </c>
       <c r="C148" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="149" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D148" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="149" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B149" s="1" t="s">
         <v>148</v>
       </c>
       <c r="C149" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="150" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D149" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="150" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B150" s="1" t="s">
         <v>149</v>
       </c>
       <c r="C150" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="151" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D150" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="151" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B151" s="1" t="s">
         <v>150</v>
       </c>
       <c r="C151" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="152" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D151" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="152" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B152" s="1" t="s">
         <v>151</v>
       </c>
       <c r="C152" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="153" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D152" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="153" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B153" s="1" t="s">
         <v>152</v>
       </c>
       <c r="C153" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="154" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D153" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="154" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B154" s="1" t="s">
         <v>153</v>
       </c>
       <c r="C154" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="155" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D154" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="155" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B155" s="1" t="s">
         <v>154</v>
       </c>
       <c r="C155" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="156" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D155" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="156" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B156" s="1" t="s">
         <v>155</v>
       </c>
       <c r="C156" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="157" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D156" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="157" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B157" s="1" t="s">
         <v>156</v>
       </c>
       <c r="C157" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="158" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D157" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="158" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B158" s="1" t="s">
         <v>157</v>
       </c>
       <c r="C158" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="159" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D158" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="159" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B159" s="1" t="s">
         <v>158</v>
       </c>
       <c r="C159" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="160" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D159" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="160" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B160" s="1" t="s">
         <v>159</v>
       </c>
       <c r="C160" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="161" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D160" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="161" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B161" s="1" t="s">
         <v>160</v>
       </c>
       <c r="C161" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="162" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D161" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="162" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B162" s="1" t="s">
         <v>161</v>
       </c>
       <c r="C162" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="163" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D162" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="163" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B163" s="1" t="s">
         <v>162</v>
       </c>
       <c r="C163" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="164" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D163" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="164" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B164" s="1" t="s">
         <v>163</v>
       </c>
       <c r="C164" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="165" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D164" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="165" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B165" s="1" t="s">
         <v>164</v>
       </c>
       <c r="C165" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="166" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D165" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="166" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B166" s="1" t="s">
         <v>165</v>
       </c>
       <c r="C166" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="167" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D166" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="167" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B167" s="1" t="s">
         <v>166</v>
       </c>
       <c r="C167" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="168" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D167" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="168" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B168" s="1" t="s">
         <v>167</v>
       </c>
       <c r="C168" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="169" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D168" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="169" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B169" s="1" t="s">
         <v>168</v>
       </c>
       <c r="C169" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="170" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D169" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="170" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B170" s="1" t="s">
         <v>169</v>
       </c>
       <c r="C170" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="171" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D170" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="171" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B171" s="1" t="s">
         <v>170</v>
       </c>
       <c r="C171" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="172" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D171" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="172" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B172" s="1" t="s">
         <v>171</v>
       </c>
       <c r="C172" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="173" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D172" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="173" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B173" s="1" t="s">
         <v>172</v>
       </c>
       <c r="C173" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="174" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D173" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="174" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B174" s="1" t="s">
         <v>173</v>
       </c>
       <c r="C174" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="175" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D174" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="175" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B175" s="1" t="s">
         <v>174</v>
       </c>
       <c r="C175" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="176" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D175" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="176" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B176" s="1" t="s">
         <v>175</v>
       </c>
       <c r="C176" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="177" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D176" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="177" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B177" s="1" t="s">
         <v>176</v>
       </c>
       <c r="C177" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="178" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D177" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="178" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B178" s="1" t="s">
         <v>177</v>
       </c>
       <c r="C178" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="179" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D178" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="179" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B179" s="1" t="s">
         <v>178</v>
       </c>
       <c r="C179" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="180" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D179" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="180" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B180" s="1" t="s">
         <v>179</v>
       </c>
       <c r="C180" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="181" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D180" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="181" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B181" s="1" t="s">
         <v>180</v>
       </c>
       <c r="C181" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="182" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D181" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="182" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B182" s="1" t="s">
         <v>181</v>
       </c>
       <c r="C182" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="183" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D182" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="183" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B183" s="1" t="s">
         <v>182</v>
       </c>
       <c r="C183" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="184" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D183" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="184" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B184" s="1" t="s">
         <v>183</v>
       </c>
       <c r="C184" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="185" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D184" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="185" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B185" s="1" t="s">
         <v>184</v>
       </c>
       <c r="C185" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="186" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D185" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="186" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B186" s="1" t="s">
         <v>185</v>
       </c>
       <c r="C186" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="187" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D186" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="187" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B187" s="1" t="s">
         <v>186</v>
       </c>
       <c r="C187" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="188" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D187" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="188" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B188" s="1" t="s">
         <v>187</v>
       </c>
       <c r="C188" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="189" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D188" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="189" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B189" s="1" t="s">
         <v>188</v>
       </c>
       <c r="C189" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="190" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D189" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="190" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B190" s="1" t="s">
         <v>189</v>
       </c>
       <c r="C190" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="191" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D190" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="191" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B191" s="1" t="s">
         <v>190</v>
       </c>
       <c r="C191" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="192" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D191" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="192" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B192" s="1" t="s">
         <v>191</v>
       </c>
       <c r="C192" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="193" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D192" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="193" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B193" s="1" t="s">
         <v>192</v>
       </c>
       <c r="C193" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="194" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D193" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="194" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B194" s="1" t="s">
         <v>193</v>
       </c>
       <c r="C194" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="195" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D194" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="195" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B195" s="1" t="s">
         <v>194</v>
       </c>
       <c r="C195" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="196" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D195" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="196" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B196" s="1" t="s">
         <v>195</v>
       </c>
       <c r="C196" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="197" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D196" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="197" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B197" s="1" t="s">
         <v>196</v>
       </c>
       <c r="C197" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="198" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D197" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="198" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B198" s="1" t="s">
         <v>197</v>
       </c>
       <c r="C198" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="199" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D198" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="199" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B199" s="1" t="s">
         <v>198</v>
       </c>
       <c r="C199" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="200" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D199" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="200" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B200" s="1" t="s">
         <v>199</v>
       </c>
       <c r="C200" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="201" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D200" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="201" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B201" s="1" t="s">
         <v>200</v>
       </c>
       <c r="C201" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="202" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D201" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="202" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B202" s="1" t="s">
         <v>201</v>
       </c>
       <c r="C202" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="203" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D202" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="203" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B203" s="1" t="s">
         <v>202</v>
       </c>
       <c r="C203" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="204" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D203" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="204" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B204" s="1" t="s">
         <v>203</v>
       </c>
       <c r="C204" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="205" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D204" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="205" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B205" s="1" t="s">
         <v>204</v>
       </c>
       <c r="C205" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="206" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D205" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="206" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B206" s="1" t="s">
         <v>205</v>
       </c>
       <c r="C206" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="207" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D206" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="207" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B207" s="1" t="s">
         <v>206</v>
       </c>
       <c r="C207" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="208" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D207" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="208" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B208" s="1" t="s">
         <v>207</v>
       </c>
       <c r="C208" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="209" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D208" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="209" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B209" s="1" t="s">
         <v>208</v>
       </c>
       <c r="C209" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="210" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D209" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="210" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B210" s="1" t="s">
         <v>209</v>
       </c>
       <c r="C210" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="211" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D210" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="211" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B211" s="1" t="s">
         <v>210</v>
       </c>
       <c r="C211" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="212" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D211" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="212" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B212" s="1" t="s">
         <v>211</v>
       </c>
       <c r="C212" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="213" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D212" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="213" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B213" s="1" t="s">
         <v>212</v>
       </c>
       <c r="C213" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="214" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D213" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="214" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B214" s="1" t="s">
         <v>213</v>
       </c>
       <c r="C214" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="215" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D214" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="215" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B215" s="1" t="s">
         <v>214</v>
       </c>
       <c r="C215" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="216" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D215" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="216" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B216" s="1" t="s">
         <v>215</v>
       </c>
       <c r="C216" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="217" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D216" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="217" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B217" s="1" t="s">
         <v>216</v>
       </c>
       <c r="C217" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="218" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D217" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="218" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B218" s="1" t="s">
         <v>217</v>
       </c>
       <c r="C218" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="219" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D218" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="219" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B219" s="1" t="s">
         <v>218</v>
       </c>
       <c r="C219" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="220" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D219" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="220" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B220" s="1" t="s">
         <v>219</v>
       </c>
       <c r="C220" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="221" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D220" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="221" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B221" s="1" t="s">
         <v>220</v>
       </c>
       <c r="C221" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="222" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D221" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="222" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B222" s="1" t="s">
         <v>221</v>
       </c>
       <c r="C222" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="223" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D222" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="223" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B223" s="1" t="s">
         <v>222</v>
       </c>
       <c r="C223" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="224" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D223" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="224" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B224" s="1" t="s">
         <v>223</v>
       </c>
       <c r="C224" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="225" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D224" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="225" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B225" s="1" t="s">
         <v>224</v>
       </c>
       <c r="C225" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="226" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D225" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="226" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B226" s="1" t="s">
         <v>225</v>
       </c>
@@ -4612,7 +5287,7 @@
         <v>783</v>
       </c>
     </row>
-    <row r="227" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="227" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B227" s="1" t="s">
         <v>226</v>
       </c>
@@ -4620,7 +5295,7 @@
         <v>783</v>
       </c>
     </row>
-    <row r="228" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="228" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B228" s="1" t="s">
         <v>227</v>
       </c>
@@ -4628,7 +5303,7 @@
         <v>783</v>
       </c>
     </row>
-    <row r="229" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="229" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B229" s="1" t="s">
         <v>228</v>
       </c>
@@ -4636,7 +5311,7 @@
         <v>783</v>
       </c>
     </row>
-    <row r="230" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="230" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B230" s="1" t="s">
         <v>229</v>
       </c>
@@ -4644,596 +5319,818 @@
         <v>783</v>
       </c>
     </row>
-    <row r="231" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="231" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B231" s="1" t="s">
         <v>230</v>
       </c>
       <c r="C231" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="232" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D231" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="232" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B232" s="1" t="s">
         <v>231</v>
       </c>
       <c r="C232" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="233" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D232" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="233" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B233" s="1" t="s">
         <v>232</v>
       </c>
       <c r="C233" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="234" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D233" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="234" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B234" s="1" t="s">
         <v>233</v>
       </c>
       <c r="C234" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="235" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D234" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="235" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B235" s="1" t="s">
         <v>234</v>
       </c>
       <c r="C235" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="236" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D235" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="236" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B236" s="1" t="s">
         <v>235</v>
       </c>
       <c r="C236" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="237" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D236" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="237" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B237" s="1" t="s">
         <v>236</v>
       </c>
       <c r="C237" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="238" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D237" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="238" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B238" s="1" t="s">
         <v>237</v>
       </c>
       <c r="C238" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="239" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D238" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="239" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B239" s="1" t="s">
         <v>238</v>
       </c>
       <c r="C239" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="240" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D239" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="240" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B240" s="1" t="s">
         <v>239</v>
       </c>
       <c r="C240" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="241" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D240" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="241" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B241" s="1" t="s">
         <v>240</v>
       </c>
       <c r="C241" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="242" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D241" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="242" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B242" s="1" t="s">
         <v>241</v>
       </c>
       <c r="C242" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="243" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D242" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="243" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B243" s="1" t="s">
         <v>242</v>
       </c>
       <c r="C243" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="244" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D243" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="244" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B244" s="1" t="s">
         <v>243</v>
       </c>
       <c r="C244" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="245" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D244" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="245" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B245" s="1" t="s">
         <v>244</v>
       </c>
       <c r="C245" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="246" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D245" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="246" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B246" s="1" t="s">
         <v>245</v>
       </c>
       <c r="C246" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="247" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D246" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="247" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B247" s="1" t="s">
         <v>246</v>
       </c>
       <c r="C247" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="248" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D247" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="248" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B248" s="1" t="s">
         <v>247</v>
       </c>
       <c r="C248" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="249" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D248" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="249" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B249" s="1" t="s">
         <v>248</v>
       </c>
       <c r="C249" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="250" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D249" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="250" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B250" s="1" t="s">
         <v>249</v>
       </c>
       <c r="C250" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="251" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D250" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="251" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B251" s="1" t="s">
         <v>250</v>
       </c>
       <c r="C251" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="252" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D251" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="252" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B252" s="1" t="s">
         <v>251</v>
       </c>
       <c r="C252" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="253" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D252" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="253" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B253" s="1" t="s">
         <v>252</v>
       </c>
       <c r="C253" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="254" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D253" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="254" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B254" s="1" t="s">
         <v>253</v>
       </c>
       <c r="C254" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="255" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D254" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="255" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B255" s="1" t="s">
         <v>254</v>
       </c>
       <c r="C255" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="256" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D255" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="256" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B256" s="1" t="s">
         <v>255</v>
       </c>
       <c r="C256" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="257" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D256" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="257" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B257" s="1" t="s">
         <v>256</v>
       </c>
       <c r="C257" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="258" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D257" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="258" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B258" s="1" t="s">
         <v>257</v>
       </c>
       <c r="C258" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="259" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D258" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="259" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B259" s="1" t="s">
         <v>258</v>
       </c>
       <c r="C259" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="260" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D259" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="260" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B260" s="1" t="s">
         <v>259</v>
       </c>
       <c r="C260" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="261" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D260" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="261" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B261" s="1" t="s">
         <v>260</v>
       </c>
       <c r="C261" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="262" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D261" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="262" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B262" s="1" t="s">
         <v>261</v>
       </c>
       <c r="C262" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="263" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D262" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="263" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B263" s="1" t="s">
         <v>262</v>
       </c>
       <c r="C263" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="264" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D263" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="264" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B264" s="1" t="s">
         <v>263</v>
       </c>
       <c r="C264" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="265" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D264" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="265" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B265" s="1" t="s">
         <v>264</v>
       </c>
       <c r="C265" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="266" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D265" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="266" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B266" s="1" t="s">
         <v>265</v>
       </c>
       <c r="C266" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="267" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D266" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="267" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B267" s="1" t="s">
         <v>266</v>
       </c>
       <c r="C267" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="268" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D267" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="268" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B268" s="1" t="s">
         <v>267</v>
       </c>
       <c r="C268" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="269" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D268" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="269" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B269" s="1" t="s">
         <v>268</v>
       </c>
       <c r="C269" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="270" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D269" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="270" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B270" s="1" t="s">
         <v>269</v>
       </c>
       <c r="C270" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="271" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D270" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="271" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B271" s="1" t="s">
         <v>270</v>
       </c>
       <c r="C271" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="272" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D271" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="272" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B272" s="1" t="s">
         <v>271</v>
       </c>
       <c r="C272" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="273" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D272" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="273" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B273" s="1" t="s">
         <v>272</v>
       </c>
       <c r="C273" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="274" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D273" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="274" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B274" s="1" t="s">
         <v>273</v>
       </c>
       <c r="C274" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="275" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D274" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="275" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B275" s="1" t="s">
         <v>274</v>
       </c>
       <c r="C275" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="276" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D275" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="276" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B276" s="1" t="s">
         <v>275</v>
       </c>
       <c r="C276" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="277" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D276" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="277" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B277" s="1" t="s">
         <v>276</v>
       </c>
       <c r="C277" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="278" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D277" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="278" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B278" s="1" t="s">
         <v>277</v>
       </c>
       <c r="C278" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="279" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D278" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="279" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B279" s="1" t="s">
         <v>278</v>
       </c>
       <c r="C279" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="280" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D279" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="280" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B280" s="1" t="s">
         <v>279</v>
       </c>
       <c r="C280" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="281" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D280" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="281" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B281" s="1" t="s">
         <v>280</v>
       </c>
       <c r="C281" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="282" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D281" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="282" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B282" s="1" t="s">
         <v>281</v>
       </c>
       <c r="C282" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="283" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D282" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="283" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B283" s="1" t="s">
         <v>282</v>
       </c>
       <c r="C283" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="284" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D283" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="284" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B284" s="1" t="s">
         <v>283</v>
       </c>
       <c r="C284" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="285" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D284" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="285" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B285" s="1" t="s">
         <v>284</v>
       </c>
       <c r="C285" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="286" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D285" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="286" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B286" s="1" t="s">
         <v>285</v>
       </c>
       <c r="C286" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="287" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D286" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="287" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B287" s="1" t="s">
         <v>286</v>
       </c>
       <c r="C287" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="288" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D287" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="288" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B288" s="1" t="s">
         <v>287</v>
       </c>
       <c r="C288" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="289" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D288" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="289" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B289" s="1" t="s">
         <v>288</v>
       </c>
       <c r="C289" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="290" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D289" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="290" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B290" s="1" t="s">
         <v>289</v>
       </c>
       <c r="C290" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="291" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D290" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="291" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B291" s="1" t="s">
         <v>290</v>
       </c>
       <c r="C291" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="292" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D291" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="292" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B292" s="1" t="s">
         <v>291</v>
       </c>
       <c r="C292" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="293" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D292" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="293" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B293" s="1" t="s">
         <v>292</v>
       </c>
       <c r="C293" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="294" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D293" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="294" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B294" s="1" t="s">
         <v>293</v>
       </c>
       <c r="C294" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="295" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D294" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="295" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B295" s="1" t="s">
         <v>294</v>
       </c>
       <c r="C295" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="296" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D295" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="296" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B296" s="1" t="s">
         <v>295</v>
       </c>
       <c r="C296" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="297" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D296" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="297" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B297" s="1" t="s">
         <v>296</v>
       </c>
       <c r="C297" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="298" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D297" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="298" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B298" s="1" t="s">
         <v>297</v>
       </c>
       <c r="C298" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="299" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D298" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="299" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B299" s="1" t="s">
         <v>298</v>
       </c>
       <c r="C299" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="300" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D299" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="300" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B300" s="1" t="s">
         <v>299</v>
       </c>
       <c r="C300" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="301" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D300" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="301" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B301" s="1" t="s">
         <v>300</v>
       </c>
       <c r="C301" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="302" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D301" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="302" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B302" s="1" t="s">
         <v>301</v>
       </c>
       <c r="C302" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="303" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D302" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="303" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B303" s="1" t="s">
         <v>302</v>
       </c>
       <c r="C303" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="304" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D303" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="304" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B304" s="1" t="s">
         <v>303</v>
       </c>
       <c r="C304" s="1" t="s">
         <v>783</v>
+      </c>
+      <c r="D304" s="1" t="s">
+        <v>789</v>
       </c>
     </row>
     <row r="305" spans="2:4" x14ac:dyDescent="0.25">
@@ -5243,6 +6140,9 @@
       <c r="C305" s="1" t="s">
         <v>783</v>
       </c>
+      <c r="D305" s="1" t="s">
+        <v>789</v>
+      </c>
     </row>
     <row r="306" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B306" s="1" t="s">
@@ -5251,6 +6151,9 @@
       <c r="C306" s="1" t="s">
         <v>783</v>
       </c>
+      <c r="D306" s="1" t="s">
+        <v>789</v>
+      </c>
     </row>
     <row r="307" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B307" s="1" t="s">
@@ -5259,6 +6162,9 @@
       <c r="C307" s="1" t="s">
         <v>783</v>
       </c>
+      <c r="D307" s="1" t="s">
+        <v>789</v>
+      </c>
     </row>
     <row r="308" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B308" s="1" t="s">
@@ -5267,6 +6173,9 @@
       <c r="C308" s="1" t="s">
         <v>783</v>
       </c>
+      <c r="D308" s="1" t="s">
+        <v>789</v>
+      </c>
     </row>
     <row r="309" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B309" s="1" t="s">
@@ -8978,7 +9887,7 @@
         <v>647</v>
       </c>
       <c r="C648" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D648" s="1" t="s">
         <v>789</v>
@@ -8989,7 +9898,7 @@
         <v>648</v>
       </c>
       <c r="C649" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D649" s="1" t="s">
         <v>789</v>
@@ -9000,7 +9909,7 @@
         <v>649</v>
       </c>
       <c r="C650" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D650" s="1" t="s">
         <v>789</v>
@@ -9011,7 +9920,7 @@
         <v>650</v>
       </c>
       <c r="C651" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D651" s="1" t="s">
         <v>789</v>
@@ -9022,7 +9931,7 @@
         <v>651</v>
       </c>
       <c r="C652" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D652" s="1" t="s">
         <v>789</v>
@@ -10404,7 +11313,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
       <formula>"SIM"</formula>
     </cfRule>
     <cfRule type="colorScale" priority="3">
@@ -10419,7 +11328,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="notContainsBlanks" dxfId="0" priority="4">
+    <cfRule type="notContainsBlanks" dxfId="3" priority="4">
       <formula>LEN(TRIM(D1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Traduzidos todos bg, bi e dg
</commit_message>
<xml_diff>
--- a/arquivos-tradutor.xlsx
+++ b/arquivos-tradutor.xlsx
@@ -2479,6 +2479,9 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
@@ -2486,6 +2489,9 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
@@ -2793,8 +2799,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:D781"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C663" sqref="C663"/>
+    <sheetView tabSelected="1" topLeftCell="A286" workbookViewId="0">
+      <selection activeCell="E306" sqref="E306"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2897,7 +2903,7 @@
         <v>8</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>789</v>
@@ -2908,7 +2914,7 @@
         <v>9</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>789</v>
@@ -2919,7 +2925,7 @@
         <v>10</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>789</v>
@@ -2930,7 +2936,7 @@
         <v>11</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>789</v>
@@ -2941,7 +2947,7 @@
         <v>12</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>789</v>
@@ -2952,7 +2958,7 @@
         <v>13</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>789</v>
@@ -2963,7 +2969,7 @@
         <v>14</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>789</v>
@@ -2974,7 +2980,7 @@
         <v>15</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>789</v>
@@ -2985,7 +2991,7 @@
         <v>16</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>789</v>
@@ -2996,7 +3002,7 @@
         <v>17</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>789</v>
@@ -3007,7 +3013,7 @@
         <v>18</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>789</v>
@@ -3018,7 +3024,7 @@
         <v>19</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>789</v>
@@ -3029,7 +3035,7 @@
         <v>20</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>789</v>
@@ -3040,7 +3046,7 @@
         <v>21</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>789</v>
@@ -3051,7 +3057,7 @@
         <v>22</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>789</v>
@@ -3062,7 +3068,7 @@
         <v>23</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>789</v>
@@ -3073,7 +3079,7 @@
         <v>24</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>789</v>
@@ -3084,7 +3090,7 @@
         <v>25</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>789</v>
@@ -3095,7 +3101,7 @@
         <v>26</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>789</v>
@@ -3106,7 +3112,7 @@
         <v>27</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>789</v>
@@ -3117,7 +3123,7 @@
         <v>28</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>789</v>
@@ -3128,7 +3134,7 @@
         <v>29</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>789</v>
@@ -3139,7 +3145,7 @@
         <v>30</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>789</v>
@@ -3150,7 +3156,7 @@
         <v>31</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>789</v>
@@ -3161,7 +3167,7 @@
         <v>32</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>789</v>
@@ -3172,7 +3178,7 @@
         <v>33</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>789</v>
@@ -3183,7 +3189,7 @@
         <v>34</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>789</v>
@@ -3194,7 +3200,7 @@
         <v>35</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>789</v>
@@ -3205,7 +3211,7 @@
         <v>36</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>789</v>
@@ -3216,7 +3222,7 @@
         <v>37</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>789</v>
@@ -3227,7 +3233,7 @@
         <v>38</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>789</v>
@@ -3238,7 +3244,7 @@
         <v>39</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>789</v>
@@ -3249,7 +3255,7 @@
         <v>40</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>789</v>
@@ -3260,7 +3266,7 @@
         <v>41</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>789</v>
@@ -3271,7 +3277,7 @@
         <v>42</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>789</v>
@@ -3282,7 +3288,7 @@
         <v>43</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>789</v>
@@ -3293,7 +3299,7 @@
         <v>44</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>789</v>
@@ -3304,7 +3310,7 @@
         <v>45</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>789</v>
@@ -3315,7 +3321,7 @@
         <v>46</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>789</v>
@@ -3326,7 +3332,7 @@
         <v>47</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>789</v>
@@ -3337,7 +3343,7 @@
         <v>48</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>789</v>
@@ -3348,7 +3354,7 @@
         <v>49</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>789</v>
@@ -3359,7 +3365,7 @@
         <v>50</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>789</v>
@@ -3370,7 +3376,7 @@
         <v>51</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>789</v>
@@ -3381,7 +3387,7 @@
         <v>52</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>789</v>
@@ -3392,7 +3398,7 @@
         <v>53</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>789</v>
@@ -3403,7 +3409,7 @@
         <v>54</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>789</v>
@@ -3414,7 +3420,7 @@
         <v>55</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>789</v>
@@ -3425,7 +3431,7 @@
         <v>56</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>789</v>
@@ -3436,7 +3442,7 @@
         <v>57</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>789</v>
@@ -3447,7 +3453,7 @@
         <v>58</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>789</v>
@@ -3458,7 +3464,7 @@
         <v>59</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>789</v>
@@ -3469,7 +3475,7 @@
         <v>60</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D61" s="1" t="s">
         <v>789</v>
@@ -3480,7 +3486,7 @@
         <v>61</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>789</v>
@@ -3491,7 +3497,7 @@
         <v>62</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D63" s="1" t="s">
         <v>789</v>
@@ -3502,7 +3508,7 @@
         <v>63</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D64" s="1" t="s">
         <v>789</v>
@@ -3513,7 +3519,7 @@
         <v>64</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>789</v>
@@ -3524,7 +3530,7 @@
         <v>65</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D66" s="1" t="s">
         <v>789</v>
@@ -3535,7 +3541,7 @@
         <v>66</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D67" s="1" t="s">
         <v>789</v>
@@ -3546,7 +3552,7 @@
         <v>67</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D68" s="1" t="s">
         <v>789</v>
@@ -3557,7 +3563,7 @@
         <v>68</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D69" s="1" t="s">
         <v>789</v>
@@ -3568,7 +3574,7 @@
         <v>69</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D70" s="1" t="s">
         <v>789</v>
@@ -3579,7 +3585,7 @@
         <v>70</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D71" s="1" t="s">
         <v>789</v>
@@ -3590,7 +3596,7 @@
         <v>71</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D72" s="1" t="s">
         <v>789</v>
@@ -3601,7 +3607,7 @@
         <v>72</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D73" s="1" t="s">
         <v>789</v>
@@ -3612,7 +3618,7 @@
         <v>73</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D74" s="1" t="s">
         <v>789</v>
@@ -3623,7 +3629,7 @@
         <v>74</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D75" s="1" t="s">
         <v>789</v>
@@ -3634,7 +3640,7 @@
         <v>75</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D76" s="1" t="s">
         <v>789</v>
@@ -3645,7 +3651,7 @@
         <v>76</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D77" s="1" t="s">
         <v>789</v>
@@ -3656,7 +3662,7 @@
         <v>77</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D78" s="1" t="s">
         <v>789</v>
@@ -3667,7 +3673,7 @@
         <v>78</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D79" s="1" t="s">
         <v>789</v>
@@ -3678,7 +3684,7 @@
         <v>79</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D80" s="1" t="s">
         <v>789</v>
@@ -3689,7 +3695,7 @@
         <v>80</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D81" s="1" t="s">
         <v>789</v>
@@ -3700,7 +3706,7 @@
         <v>81</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D82" s="1" t="s">
         <v>789</v>
@@ -3711,7 +3717,7 @@
         <v>82</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D83" s="1" t="s">
         <v>789</v>
@@ -3722,7 +3728,7 @@
         <v>83</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D84" s="1" t="s">
         <v>789</v>
@@ -3733,7 +3739,7 @@
         <v>84</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D85" s="1" t="s">
         <v>789</v>
@@ -3744,7 +3750,7 @@
         <v>85</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D86" s="1" t="s">
         <v>789</v>
@@ -3755,7 +3761,7 @@
         <v>86</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D87" s="1" t="s">
         <v>789</v>
@@ -3766,7 +3772,7 @@
         <v>87</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D88" s="1" t="s">
         <v>789</v>
@@ -3777,7 +3783,7 @@
         <v>88</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D89" s="1" t="s">
         <v>789</v>
@@ -3788,7 +3794,7 @@
         <v>89</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D90" s="1" t="s">
         <v>789</v>
@@ -3799,7 +3805,7 @@
         <v>90</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D91" s="1" t="s">
         <v>789</v>
@@ -3810,7 +3816,7 @@
         <v>91</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D92" s="1" t="s">
         <v>789</v>
@@ -3821,7 +3827,7 @@
         <v>92</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D93" s="1" t="s">
         <v>789</v>
@@ -3832,7 +3838,7 @@
         <v>93</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D94" s="1" t="s">
         <v>789</v>
@@ -3843,7 +3849,7 @@
         <v>94</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D95" s="1" t="s">
         <v>789</v>
@@ -3854,7 +3860,7 @@
         <v>95</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D96" s="1" t="s">
         <v>789</v>
@@ -3865,7 +3871,7 @@
         <v>96</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D97" s="1" t="s">
         <v>789</v>
@@ -3876,7 +3882,7 @@
         <v>97</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D98" s="1" t="s">
         <v>789</v>
@@ -3887,7 +3893,7 @@
         <v>98</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D99" s="1" t="s">
         <v>789</v>
@@ -3898,7 +3904,7 @@
         <v>99</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D100" s="1" t="s">
         <v>789</v>
@@ -3909,7 +3915,7 @@
         <v>100</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D101" s="1" t="s">
         <v>789</v>
@@ -3920,7 +3926,7 @@
         <v>101</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D102" s="1" t="s">
         <v>789</v>
@@ -3931,7 +3937,7 @@
         <v>102</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D103" s="1" t="s">
         <v>789</v>
@@ -3942,7 +3948,7 @@
         <v>103</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D104" s="1" t="s">
         <v>789</v>
@@ -3953,7 +3959,7 @@
         <v>104</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D105" s="1" t="s">
         <v>789</v>
@@ -3964,7 +3970,7 @@
         <v>105</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D106" s="1" t="s">
         <v>789</v>
@@ -3975,7 +3981,7 @@
         <v>106</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D107" s="1" t="s">
         <v>789</v>
@@ -3986,7 +3992,7 @@
         <v>107</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D108" s="1" t="s">
         <v>789</v>
@@ -3997,7 +4003,7 @@
         <v>108</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D109" s="1" t="s">
         <v>789</v>
@@ -4008,7 +4014,7 @@
         <v>109</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D110" s="1" t="s">
         <v>789</v>
@@ -4019,7 +4025,7 @@
         <v>110</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D111" s="1" t="s">
         <v>789</v>
@@ -4030,7 +4036,7 @@
         <v>111</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D112" s="1" t="s">
         <v>789</v>
@@ -4041,7 +4047,7 @@
         <v>112</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D113" s="1" t="s">
         <v>789</v>
@@ -4052,7 +4058,7 @@
         <v>113</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D114" s="1" t="s">
         <v>789</v>
@@ -4063,7 +4069,7 @@
         <v>114</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D115" s="1" t="s">
         <v>789</v>
@@ -4074,7 +4080,7 @@
         <v>115</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D116" s="1" t="s">
         <v>789</v>
@@ -4085,7 +4091,7 @@
         <v>116</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D117" s="1" t="s">
         <v>789</v>
@@ -4096,7 +4102,7 @@
         <v>117</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D118" s="1" t="s">
         <v>789</v>
@@ -4107,7 +4113,7 @@
         <v>118</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D119" s="1" t="s">
         <v>789</v>
@@ -4118,7 +4124,7 @@
         <v>119</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D120" s="1" t="s">
         <v>789</v>
@@ -4129,7 +4135,7 @@
         <v>120</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D121" s="1" t="s">
         <v>789</v>
@@ -4140,7 +4146,7 @@
         <v>121</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D122" s="1" t="s">
         <v>789</v>
@@ -4151,7 +4157,7 @@
         <v>122</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D123" s="1" t="s">
         <v>789</v>
@@ -4162,7 +4168,7 @@
         <v>123</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D124" s="1" t="s">
         <v>789</v>
@@ -4173,7 +4179,7 @@
         <v>124</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D125" s="1" t="s">
         <v>789</v>
@@ -4184,7 +4190,7 @@
         <v>125</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D126" s="1" t="s">
         <v>789</v>
@@ -4195,7 +4201,7 @@
         <v>126</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D127" s="1" t="s">
         <v>789</v>
@@ -4206,7 +4212,7 @@
         <v>127</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D128" s="1" t="s">
         <v>789</v>
@@ -4217,7 +4223,7 @@
         <v>128</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D129" s="1" t="s">
         <v>789</v>
@@ -4228,7 +4234,7 @@
         <v>129</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D130" s="1" t="s">
         <v>789</v>
@@ -4239,7 +4245,7 @@
         <v>130</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D131" s="1" t="s">
         <v>789</v>
@@ -4250,7 +4256,7 @@
         <v>131</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D132" s="1" t="s">
         <v>789</v>
@@ -4261,7 +4267,7 @@
         <v>132</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D133" s="1" t="s">
         <v>789</v>
@@ -4272,7 +4278,7 @@
         <v>133</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D134" s="1" t="s">
         <v>789</v>
@@ -4283,7 +4289,7 @@
         <v>134</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D135" s="1" t="s">
         <v>789</v>
@@ -4294,7 +4300,7 @@
         <v>135</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D136" s="1" t="s">
         <v>789</v>
@@ -4305,7 +4311,7 @@
         <v>136</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D137" s="1" t="s">
         <v>789</v>
@@ -4316,7 +4322,7 @@
         <v>137</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D138" s="1" t="s">
         <v>789</v>
@@ -4327,7 +4333,7 @@
         <v>138</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D139" s="1" t="s">
         <v>789</v>
@@ -4338,7 +4344,7 @@
         <v>139</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D140" s="1" t="s">
         <v>789</v>
@@ -4349,7 +4355,7 @@
         <v>140</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D141" s="1" t="s">
         <v>789</v>
@@ -4360,7 +4366,7 @@
         <v>141</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D142" s="1" t="s">
         <v>789</v>
@@ -4371,7 +4377,7 @@
         <v>142</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D143" s="1" t="s">
         <v>789</v>
@@ -4382,7 +4388,7 @@
         <v>143</v>
       </c>
       <c r="C144" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D144" s="1" t="s">
         <v>789</v>
@@ -4393,7 +4399,7 @@
         <v>144</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D145" s="1" t="s">
         <v>789</v>
@@ -4404,7 +4410,7 @@
         <v>145</v>
       </c>
       <c r="C146" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D146" s="1" t="s">
         <v>789</v>
@@ -4415,7 +4421,7 @@
         <v>146</v>
       </c>
       <c r="C147" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D147" s="1" t="s">
         <v>789</v>
@@ -4426,7 +4432,7 @@
         <v>147</v>
       </c>
       <c r="C148" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D148" s="1" t="s">
         <v>789</v>
@@ -4437,7 +4443,7 @@
         <v>148</v>
       </c>
       <c r="C149" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D149" s="1" t="s">
         <v>789</v>
@@ -4448,7 +4454,7 @@
         <v>149</v>
       </c>
       <c r="C150" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D150" s="1" t="s">
         <v>789</v>
@@ -4459,7 +4465,7 @@
         <v>150</v>
       </c>
       <c r="C151" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D151" s="1" t="s">
         <v>789</v>
@@ -4470,7 +4476,7 @@
         <v>151</v>
       </c>
       <c r="C152" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D152" s="1" t="s">
         <v>789</v>
@@ -4481,7 +4487,7 @@
         <v>152</v>
       </c>
       <c r="C153" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D153" s="1" t="s">
         <v>789</v>
@@ -4492,7 +4498,7 @@
         <v>153</v>
       </c>
       <c r="C154" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D154" s="1" t="s">
         <v>789</v>
@@ -4503,7 +4509,7 @@
         <v>154</v>
       </c>
       <c r="C155" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D155" s="1" t="s">
         <v>789</v>
@@ -4514,7 +4520,7 @@
         <v>155</v>
       </c>
       <c r="C156" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D156" s="1" t="s">
         <v>789</v>
@@ -4525,7 +4531,7 @@
         <v>156</v>
       </c>
       <c r="C157" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D157" s="1" t="s">
         <v>789</v>
@@ -4536,7 +4542,7 @@
         <v>157</v>
       </c>
       <c r="C158" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D158" s="1" t="s">
         <v>789</v>
@@ -4547,7 +4553,7 @@
         <v>158</v>
       </c>
       <c r="C159" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D159" s="1" t="s">
         <v>789</v>
@@ -4558,7 +4564,7 @@
         <v>159</v>
       </c>
       <c r="C160" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D160" s="1" t="s">
         <v>789</v>
@@ -4569,7 +4575,7 @@
         <v>160</v>
       </c>
       <c r="C161" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D161" s="1" t="s">
         <v>789</v>
@@ -4580,7 +4586,7 @@
         <v>161</v>
       </c>
       <c r="C162" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D162" s="1" t="s">
         <v>789</v>
@@ -4591,7 +4597,7 @@
         <v>162</v>
       </c>
       <c r="C163" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D163" s="1" t="s">
         <v>789</v>
@@ -4602,7 +4608,7 @@
         <v>163</v>
       </c>
       <c r="C164" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D164" s="1" t="s">
         <v>789</v>
@@ -4613,7 +4619,7 @@
         <v>164</v>
       </c>
       <c r="C165" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D165" s="1" t="s">
         <v>789</v>
@@ -4624,7 +4630,7 @@
         <v>165</v>
       </c>
       <c r="C166" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D166" s="1" t="s">
         <v>789</v>
@@ -4635,7 +4641,7 @@
         <v>166</v>
       </c>
       <c r="C167" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D167" s="1" t="s">
         <v>789</v>
@@ -4646,7 +4652,7 @@
         <v>167</v>
       </c>
       <c r="C168" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D168" s="1" t="s">
         <v>789</v>
@@ -4657,7 +4663,7 @@
         <v>168</v>
       </c>
       <c r="C169" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D169" s="1" t="s">
         <v>789</v>
@@ -4668,7 +4674,7 @@
         <v>169</v>
       </c>
       <c r="C170" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D170" s="1" t="s">
         <v>789</v>
@@ -4679,7 +4685,7 @@
         <v>170</v>
       </c>
       <c r="C171" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D171" s="1" t="s">
         <v>789</v>
@@ -4690,7 +4696,7 @@
         <v>171</v>
       </c>
       <c r="C172" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D172" s="1" t="s">
         <v>789</v>
@@ -4701,7 +4707,7 @@
         <v>172</v>
       </c>
       <c r="C173" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D173" s="1" t="s">
         <v>789</v>
@@ -4712,7 +4718,7 @@
         <v>173</v>
       </c>
       <c r="C174" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D174" s="1" t="s">
         <v>789</v>
@@ -4723,7 +4729,7 @@
         <v>174</v>
       </c>
       <c r="C175" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D175" s="1" t="s">
         <v>789</v>
@@ -4734,7 +4740,7 @@
         <v>175</v>
       </c>
       <c r="C176" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D176" s="1" t="s">
         <v>789</v>
@@ -4745,7 +4751,7 @@
         <v>176</v>
       </c>
       <c r="C177" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D177" s="1" t="s">
         <v>789</v>
@@ -4756,7 +4762,7 @@
         <v>177</v>
       </c>
       <c r="C178" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D178" s="1" t="s">
         <v>789</v>
@@ -4767,7 +4773,7 @@
         <v>178</v>
       </c>
       <c r="C179" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D179" s="1" t="s">
         <v>789</v>
@@ -4778,7 +4784,7 @@
         <v>179</v>
       </c>
       <c r="C180" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D180" s="1" t="s">
         <v>789</v>
@@ -4789,7 +4795,7 @@
         <v>180</v>
       </c>
       <c r="C181" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D181" s="1" t="s">
         <v>789</v>
@@ -4800,7 +4806,7 @@
         <v>181</v>
       </c>
       <c r="C182" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D182" s="1" t="s">
         <v>789</v>
@@ -4811,7 +4817,7 @@
         <v>182</v>
       </c>
       <c r="C183" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D183" s="1" t="s">
         <v>789</v>
@@ -4822,7 +4828,7 @@
         <v>183</v>
       </c>
       <c r="C184" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D184" s="1" t="s">
         <v>789</v>
@@ -4833,7 +4839,7 @@
         <v>184</v>
       </c>
       <c r="C185" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D185" s="1" t="s">
         <v>789</v>
@@ -4844,7 +4850,7 @@
         <v>185</v>
       </c>
       <c r="C186" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D186" s="1" t="s">
         <v>789</v>
@@ -4855,7 +4861,7 @@
         <v>186</v>
       </c>
       <c r="C187" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D187" s="1" t="s">
         <v>789</v>
@@ -4866,7 +4872,7 @@
         <v>187</v>
       </c>
       <c r="C188" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D188" s="1" t="s">
         <v>789</v>
@@ -4877,7 +4883,7 @@
         <v>188</v>
       </c>
       <c r="C189" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D189" s="1" t="s">
         <v>789</v>
@@ -4888,7 +4894,7 @@
         <v>189</v>
       </c>
       <c r="C190" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D190" s="1" t="s">
         <v>789</v>
@@ -4899,7 +4905,7 @@
         <v>190</v>
       </c>
       <c r="C191" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D191" s="1" t="s">
         <v>789</v>
@@ -4910,7 +4916,7 @@
         <v>191</v>
       </c>
       <c r="C192" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D192" s="1" t="s">
         <v>789</v>
@@ -4921,7 +4927,7 @@
         <v>192</v>
       </c>
       <c r="C193" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D193" s="1" t="s">
         <v>789</v>
@@ -4932,7 +4938,7 @@
         <v>193</v>
       </c>
       <c r="C194" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D194" s="1" t="s">
         <v>789</v>
@@ -4943,7 +4949,7 @@
         <v>194</v>
       </c>
       <c r="C195" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D195" s="1" t="s">
         <v>789</v>
@@ -4954,7 +4960,7 @@
         <v>195</v>
       </c>
       <c r="C196" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D196" s="1" t="s">
         <v>789</v>
@@ -4965,7 +4971,7 @@
         <v>196</v>
       </c>
       <c r="C197" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D197" s="1" t="s">
         <v>789</v>
@@ -4976,7 +4982,7 @@
         <v>197</v>
       </c>
       <c r="C198" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D198" s="1" t="s">
         <v>789</v>
@@ -4987,7 +4993,7 @@
         <v>198</v>
       </c>
       <c r="C199" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D199" s="1" t="s">
         <v>789</v>
@@ -4998,7 +5004,7 @@
         <v>199</v>
       </c>
       <c r="C200" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D200" s="1" t="s">
         <v>789</v>
@@ -5009,7 +5015,7 @@
         <v>200</v>
       </c>
       <c r="C201" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D201" s="1" t="s">
         <v>789</v>
@@ -5020,7 +5026,7 @@
         <v>201</v>
       </c>
       <c r="C202" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D202" s="1" t="s">
         <v>789</v>
@@ -5031,7 +5037,7 @@
         <v>202</v>
       </c>
       <c r="C203" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D203" s="1" t="s">
         <v>789</v>
@@ -5042,7 +5048,7 @@
         <v>203</v>
       </c>
       <c r="C204" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D204" s="1" t="s">
         <v>789</v>
@@ -5053,7 +5059,7 @@
         <v>204</v>
       </c>
       <c r="C205" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D205" s="1" t="s">
         <v>789</v>
@@ -5064,7 +5070,7 @@
         <v>205</v>
       </c>
       <c r="C206" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D206" s="1" t="s">
         <v>789</v>
@@ -5075,7 +5081,7 @@
         <v>206</v>
       </c>
       <c r="C207" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D207" s="1" t="s">
         <v>789</v>
@@ -5086,7 +5092,7 @@
         <v>207</v>
       </c>
       <c r="C208" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D208" s="1" t="s">
         <v>789</v>
@@ -5097,7 +5103,7 @@
         <v>208</v>
       </c>
       <c r="C209" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D209" s="1" t="s">
         <v>789</v>
@@ -5108,7 +5114,7 @@
         <v>209</v>
       </c>
       <c r="C210" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D210" s="1" t="s">
         <v>789</v>
@@ -5119,7 +5125,7 @@
         <v>210</v>
       </c>
       <c r="C211" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D211" s="1" t="s">
         <v>789</v>
@@ -5130,7 +5136,7 @@
         <v>211</v>
       </c>
       <c r="C212" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D212" s="1" t="s">
         <v>789</v>
@@ -5141,7 +5147,7 @@
         <v>212</v>
       </c>
       <c r="C213" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D213" s="1" t="s">
         <v>789</v>
@@ -5152,7 +5158,7 @@
         <v>213</v>
       </c>
       <c r="C214" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D214" s="1" t="s">
         <v>789</v>
@@ -5163,7 +5169,7 @@
         <v>214</v>
       </c>
       <c r="C215" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D215" s="1" t="s">
         <v>789</v>
@@ -5174,7 +5180,7 @@
         <v>215</v>
       </c>
       <c r="C216" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D216" s="1" t="s">
         <v>789</v>
@@ -5185,7 +5191,7 @@
         <v>216</v>
       </c>
       <c r="C217" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D217" s="1" t="s">
         <v>789</v>
@@ -5196,7 +5202,7 @@
         <v>217</v>
       </c>
       <c r="C218" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D218" s="1" t="s">
         <v>789</v>
@@ -5207,7 +5213,7 @@
         <v>218</v>
       </c>
       <c r="C219" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D219" s="1" t="s">
         <v>789</v>
@@ -5218,7 +5224,7 @@
         <v>219</v>
       </c>
       <c r="C220" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D220" s="1" t="s">
         <v>789</v>
@@ -5229,7 +5235,7 @@
         <v>220</v>
       </c>
       <c r="C221" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D221" s="1" t="s">
         <v>789</v>
@@ -5240,7 +5246,7 @@
         <v>221</v>
       </c>
       <c r="C222" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D222" s="1" t="s">
         <v>789</v>
@@ -5251,7 +5257,7 @@
         <v>222</v>
       </c>
       <c r="C223" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D223" s="1" t="s">
         <v>789</v>
@@ -5262,7 +5268,7 @@
         <v>223</v>
       </c>
       <c r="C224" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D224" s="1" t="s">
         <v>789</v>
@@ -5273,7 +5279,7 @@
         <v>224</v>
       </c>
       <c r="C225" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D225" s="1" t="s">
         <v>789</v>
@@ -5324,7 +5330,7 @@
         <v>230</v>
       </c>
       <c r="C231" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D231" s="1" t="s">
         <v>789</v>
@@ -5335,7 +5341,7 @@
         <v>231</v>
       </c>
       <c r="C232" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D232" s="1" t="s">
         <v>789</v>
@@ -5346,7 +5352,7 @@
         <v>232</v>
       </c>
       <c r="C233" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D233" s="1" t="s">
         <v>789</v>
@@ -5357,7 +5363,7 @@
         <v>233</v>
       </c>
       <c r="C234" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D234" s="1" t="s">
         <v>789</v>
@@ -5368,7 +5374,7 @@
         <v>234</v>
       </c>
       <c r="C235" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D235" s="1" t="s">
         <v>789</v>
@@ -5379,7 +5385,7 @@
         <v>235</v>
       </c>
       <c r="C236" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D236" s="1" t="s">
         <v>789</v>
@@ -5390,7 +5396,7 @@
         <v>236</v>
       </c>
       <c r="C237" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D237" s="1" t="s">
         <v>789</v>
@@ -5401,7 +5407,7 @@
         <v>237</v>
       </c>
       <c r="C238" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D238" s="1" t="s">
         <v>789</v>
@@ -5412,7 +5418,7 @@
         <v>238</v>
       </c>
       <c r="C239" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D239" s="1" t="s">
         <v>789</v>
@@ -5423,7 +5429,7 @@
         <v>239</v>
       </c>
       <c r="C240" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D240" s="1" t="s">
         <v>789</v>
@@ -5434,7 +5440,7 @@
         <v>240</v>
       </c>
       <c r="C241" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D241" s="1" t="s">
         <v>789</v>
@@ -5445,7 +5451,7 @@
         <v>241</v>
       </c>
       <c r="C242" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D242" s="1" t="s">
         <v>789</v>
@@ -5456,7 +5462,7 @@
         <v>242</v>
       </c>
       <c r="C243" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D243" s="1" t="s">
         <v>789</v>
@@ -5467,7 +5473,7 @@
         <v>243</v>
       </c>
       <c r="C244" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D244" s="1" t="s">
         <v>789</v>
@@ -5478,7 +5484,7 @@
         <v>244</v>
       </c>
       <c r="C245" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D245" s="1" t="s">
         <v>789</v>
@@ -5489,7 +5495,7 @@
         <v>245</v>
       </c>
       <c r="C246" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D246" s="1" t="s">
         <v>789</v>
@@ -5500,7 +5506,7 @@
         <v>246</v>
       </c>
       <c r="C247" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D247" s="1" t="s">
         <v>789</v>
@@ -5511,7 +5517,7 @@
         <v>247</v>
       </c>
       <c r="C248" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D248" s="1" t="s">
         <v>789</v>
@@ -5522,7 +5528,7 @@
         <v>248</v>
       </c>
       <c r="C249" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D249" s="1" t="s">
         <v>789</v>
@@ -5533,7 +5539,7 @@
         <v>249</v>
       </c>
       <c r="C250" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D250" s="1" t="s">
         <v>789</v>
@@ -5544,7 +5550,7 @@
         <v>250</v>
       </c>
       <c r="C251" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D251" s="1" t="s">
         <v>789</v>
@@ -5555,7 +5561,7 @@
         <v>251</v>
       </c>
       <c r="C252" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D252" s="1" t="s">
         <v>789</v>
@@ -5566,7 +5572,7 @@
         <v>252</v>
       </c>
       <c r="C253" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D253" s="1" t="s">
         <v>789</v>
@@ -5577,7 +5583,7 @@
         <v>253</v>
       </c>
       <c r="C254" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D254" s="1" t="s">
         <v>789</v>
@@ -5588,7 +5594,7 @@
         <v>254</v>
       </c>
       <c r="C255" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D255" s="1" t="s">
         <v>789</v>
@@ -5599,7 +5605,7 @@
         <v>255</v>
       </c>
       <c r="C256" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D256" s="1" t="s">
         <v>789</v>
@@ -5610,7 +5616,7 @@
         <v>256</v>
       </c>
       <c r="C257" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D257" s="1" t="s">
         <v>789</v>
@@ -5621,7 +5627,7 @@
         <v>257</v>
       </c>
       <c r="C258" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D258" s="1" t="s">
         <v>789</v>
@@ -5632,7 +5638,7 @@
         <v>258</v>
       </c>
       <c r="C259" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D259" s="1" t="s">
         <v>789</v>
@@ -5643,7 +5649,7 @@
         <v>259</v>
       </c>
       <c r="C260" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D260" s="1" t="s">
         <v>789</v>
@@ -5654,7 +5660,7 @@
         <v>260</v>
       </c>
       <c r="C261" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D261" s="1" t="s">
         <v>789</v>
@@ -5665,7 +5671,7 @@
         <v>261</v>
       </c>
       <c r="C262" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D262" s="1" t="s">
         <v>789</v>
@@ -5676,7 +5682,7 @@
         <v>262</v>
       </c>
       <c r="C263" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D263" s="1" t="s">
         <v>789</v>
@@ -5687,7 +5693,7 @@
         <v>263</v>
       </c>
       <c r="C264" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D264" s="1" t="s">
         <v>789</v>
@@ -5698,7 +5704,7 @@
         <v>264</v>
       </c>
       <c r="C265" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D265" s="1" t="s">
         <v>789</v>
@@ -5709,7 +5715,7 @@
         <v>265</v>
       </c>
       <c r="C266" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D266" s="1" t="s">
         <v>789</v>
@@ -5720,7 +5726,7 @@
         <v>266</v>
       </c>
       <c r="C267" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D267" s="1" t="s">
         <v>789</v>
@@ -5731,7 +5737,7 @@
         <v>267</v>
       </c>
       <c r="C268" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D268" s="1" t="s">
         <v>789</v>
@@ -5742,7 +5748,7 @@
         <v>268</v>
       </c>
       <c r="C269" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D269" s="1" t="s">
         <v>789</v>
@@ -5753,7 +5759,7 @@
         <v>269</v>
       </c>
       <c r="C270" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D270" s="1" t="s">
         <v>789</v>
@@ -5764,7 +5770,7 @@
         <v>270</v>
       </c>
       <c r="C271" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D271" s="1" t="s">
         <v>789</v>
@@ -5775,7 +5781,7 @@
         <v>271</v>
       </c>
       <c r="C272" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D272" s="1" t="s">
         <v>789</v>
@@ -5786,7 +5792,7 @@
         <v>272</v>
       </c>
       <c r="C273" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D273" s="1" t="s">
         <v>789</v>
@@ -5797,7 +5803,7 @@
         <v>273</v>
       </c>
       <c r="C274" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D274" s="1" t="s">
         <v>789</v>
@@ -5808,7 +5814,7 @@
         <v>274</v>
       </c>
       <c r="C275" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D275" s="1" t="s">
         <v>789</v>
@@ -5819,7 +5825,7 @@
         <v>275</v>
       </c>
       <c r="C276" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D276" s="1" t="s">
         <v>789</v>
@@ -5830,7 +5836,7 @@
         <v>276</v>
       </c>
       <c r="C277" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D277" s="1" t="s">
         <v>789</v>
@@ -5841,7 +5847,7 @@
         <v>277</v>
       </c>
       <c r="C278" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D278" s="1" t="s">
         <v>789</v>
@@ -5852,7 +5858,7 @@
         <v>278</v>
       </c>
       <c r="C279" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D279" s="1" t="s">
         <v>789</v>
@@ -5863,7 +5869,7 @@
         <v>279</v>
       </c>
       <c r="C280" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D280" s="1" t="s">
         <v>789</v>
@@ -5874,7 +5880,7 @@
         <v>280</v>
       </c>
       <c r="C281" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D281" s="1" t="s">
         <v>789</v>
@@ -5885,7 +5891,7 @@
         <v>281</v>
       </c>
       <c r="C282" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D282" s="1" t="s">
         <v>789</v>
@@ -5896,7 +5902,7 @@
         <v>282</v>
       </c>
       <c r="C283" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D283" s="1" t="s">
         <v>789</v>
@@ -5907,7 +5913,7 @@
         <v>283</v>
       </c>
       <c r="C284" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D284" s="1" t="s">
         <v>789</v>
@@ -5918,7 +5924,7 @@
         <v>284</v>
       </c>
       <c r="C285" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D285" s="1" t="s">
         <v>789</v>
@@ -5929,7 +5935,7 @@
         <v>285</v>
       </c>
       <c r="C286" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D286" s="1" t="s">
         <v>789</v>
@@ -5940,7 +5946,7 @@
         <v>286</v>
       </c>
       <c r="C287" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D287" s="1" t="s">
         <v>789</v>
@@ -5951,7 +5957,7 @@
         <v>287</v>
       </c>
       <c r="C288" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D288" s="1" t="s">
         <v>789</v>
@@ -5962,7 +5968,7 @@
         <v>288</v>
       </c>
       <c r="C289" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D289" s="1" t="s">
         <v>789</v>
@@ -5973,7 +5979,7 @@
         <v>289</v>
       </c>
       <c r="C290" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D290" s="1" t="s">
         <v>789</v>
@@ -5984,7 +5990,7 @@
         <v>290</v>
       </c>
       <c r="C291" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D291" s="1" t="s">
         <v>789</v>
@@ -5995,7 +6001,7 @@
         <v>291</v>
       </c>
       <c r="C292" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D292" s="1" t="s">
         <v>789</v>
@@ -6006,7 +6012,7 @@
         <v>292</v>
       </c>
       <c r="C293" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D293" s="1" t="s">
         <v>789</v>
@@ -6017,7 +6023,7 @@
         <v>293</v>
       </c>
       <c r="C294" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D294" s="1" t="s">
         <v>789</v>
@@ -6028,7 +6034,7 @@
         <v>294</v>
       </c>
       <c r="C295" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D295" s="1" t="s">
         <v>789</v>
@@ -6039,7 +6045,7 @@
         <v>295</v>
       </c>
       <c r="C296" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D296" s="1" t="s">
         <v>789</v>
@@ -6050,7 +6056,7 @@
         <v>296</v>
       </c>
       <c r="C297" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D297" s="1" t="s">
         <v>789</v>
@@ -6061,7 +6067,7 @@
         <v>297</v>
       </c>
       <c r="C298" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D298" s="1" t="s">
         <v>789</v>
@@ -6072,7 +6078,7 @@
         <v>298</v>
       </c>
       <c r="C299" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D299" s="1" t="s">
         <v>789</v>
@@ -6083,7 +6089,7 @@
         <v>299</v>
       </c>
       <c r="C300" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D300" s="1" t="s">
         <v>789</v>
@@ -6094,7 +6100,7 @@
         <v>300</v>
       </c>
       <c r="C301" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D301" s="1" t="s">
         <v>789</v>
@@ -6105,7 +6111,7 @@
         <v>301</v>
       </c>
       <c r="C302" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D302" s="1" t="s">
         <v>789</v>
@@ -6116,7 +6122,7 @@
         <v>302</v>
       </c>
       <c r="C303" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D303" s="1" t="s">
         <v>789</v>
@@ -6127,7 +6133,7 @@
         <v>303</v>
       </c>
       <c r="C304" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D304" s="1" t="s">
         <v>789</v>
@@ -6138,7 +6144,7 @@
         <v>304</v>
       </c>
       <c r="C305" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D305" s="1" t="s">
         <v>789</v>
@@ -6149,7 +6155,7 @@
         <v>305</v>
       </c>
       <c r="C306" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D306" s="1" t="s">
         <v>789</v>
@@ -6160,7 +6166,7 @@
         <v>306</v>
       </c>
       <c r="C307" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D307" s="1" t="s">
         <v>789</v>
@@ -6171,7 +6177,7 @@
         <v>307</v>
       </c>
       <c r="C308" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D308" s="1" t="s">
         <v>789</v>

</xml_diff>

<commit_message>
Revervado mais arquivos para luiz. Adicionada tool para extrair texto de outros arquivos.
</commit_message>
<xml_diff>
--- a/arquivos-tradutor.xlsx
+++ b/arquivos-tradutor.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2315" uniqueCount="793">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2330" uniqueCount="793">
   <si>
     <t>Arquivo</t>
   </si>
@@ -2467,11 +2467,8 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="14">
     <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
@@ -2479,9 +2476,6 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
@@ -2489,9 +2483,69 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
@@ -2799,8 +2853,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:D781"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A286" workbookViewId="0">
-      <selection activeCell="E306" sqref="E306"/>
+    <sheetView tabSelected="1" topLeftCell="A751" workbookViewId="0">
+      <selection activeCell="D774" sqref="D774"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5308,6 +5362,9 @@
       <c r="C228" s="1" t="s">
         <v>783</v>
       </c>
+      <c r="D228" s="1" t="s">
+        <v>789</v>
+      </c>
     </row>
     <row r="229" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B229" s="1" t="s">
@@ -5316,6 +5373,9 @@
       <c r="C229" s="1" t="s">
         <v>783</v>
       </c>
+      <c r="D229" s="1" t="s">
+        <v>789</v>
+      </c>
     </row>
     <row r="230" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B230" s="1" t="s">
@@ -5324,6 +5384,9 @@
       <c r="C230" s="1" t="s">
         <v>783</v>
       </c>
+      <c r="D230" s="1" t="s">
+        <v>789</v>
+      </c>
     </row>
     <row r="231" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B231" s="1" t="s">
@@ -6190,6 +6253,9 @@
       <c r="C309" s="1" t="s">
         <v>783</v>
       </c>
+      <c r="D309" s="1" t="s">
+        <v>789</v>
+      </c>
     </row>
     <row r="310" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B310" s="1" t="s">
@@ -6206,6 +6272,9 @@
       <c r="C311" s="1" t="s">
         <v>783</v>
       </c>
+      <c r="D311" s="1" t="s">
+        <v>789</v>
+      </c>
     </row>
     <row r="312" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B312" s="1" t="s">
@@ -11135,6 +11204,9 @@
       <c r="C761" s="1" t="s">
         <v>783</v>
       </c>
+      <c r="D761" s="1" t="s">
+        <v>789</v>
+      </c>
     </row>
     <row r="762" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B762" s="1" t="s">
@@ -11151,6 +11223,9 @@
       <c r="C763" s="1" t="s">
         <v>783</v>
       </c>
+      <c r="D763" s="1" t="s">
+        <v>789</v>
+      </c>
     </row>
     <row r="764" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B764" s="1" t="s">
@@ -11159,6 +11234,9 @@
       <c r="C764" s="1" t="s">
         <v>783</v>
       </c>
+      <c r="D764" s="1" t="s">
+        <v>789</v>
+      </c>
     </row>
     <row r="765" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B765" s="1" t="s">
@@ -11175,6 +11253,9 @@
       <c r="C766" s="1" t="s">
         <v>783</v>
       </c>
+      <c r="D766" s="1" t="s">
+        <v>789</v>
+      </c>
     </row>
     <row r="767" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B767" s="1" t="s">
@@ -11183,6 +11264,9 @@
       <c r="C767" s="1" t="s">
         <v>783</v>
       </c>
+      <c r="D767" s="1" t="s">
+        <v>789</v>
+      </c>
     </row>
     <row r="768" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B768" s="1" t="s">
@@ -11199,6 +11283,9 @@
       <c r="C769" s="1" t="s">
         <v>783</v>
       </c>
+      <c r="D769" s="1" t="s">
+        <v>789</v>
+      </c>
     </row>
     <row r="770" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B770" s="1" t="s">
@@ -11207,6 +11294,9 @@
       <c r="C770" s="1" t="s">
         <v>783</v>
       </c>
+      <c r="D770" s="1" t="s">
+        <v>789</v>
+      </c>
     </row>
     <row r="771" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B771" s="1" t="s">
@@ -11215,6 +11305,9 @@
       <c r="C771" s="1" t="s">
         <v>783</v>
       </c>
+      <c r="D771" s="1" t="s">
+        <v>789</v>
+      </c>
     </row>
     <row r="772" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B772" s="1" t="s">
@@ -11223,6 +11316,9 @@
       <c r="C772" s="1" t="s">
         <v>783</v>
       </c>
+      <c r="D772" s="1" t="s">
+        <v>789</v>
+      </c>
     </row>
     <row r="773" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B773" s="1" t="s">
@@ -11239,6 +11335,9 @@
       <c r="C774" s="1" t="s">
         <v>783</v>
       </c>
+      <c r="D774" s="1" t="s">
+        <v>789</v>
+      </c>
     </row>
     <row r="775" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B775" s="1" t="s">
@@ -11319,7 +11418,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="2" operator="equal">
       <formula>"SIM"</formula>
     </cfRule>
     <cfRule type="colorScale" priority="3">
@@ -11334,7 +11433,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="notContainsBlanks" dxfId="3" priority="4">
+    <cfRule type="notContainsBlanks" dxfId="12" priority="4">
       <formula>LEN(TRIM(D1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Finalizada traducao do mes_bg13_01_us.u16
</commit_message>
<xml_diff>
--- a/arquivos-tradutor.xlsx
+++ b/arquivos-tradutor.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Moacyr\Desktop\GITHUB-BD\traducao-blue-dragon-xbox360\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\danger\traducoes\traducao-blue-dragon-xbox360\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2330" uniqueCount="793">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2330" uniqueCount="794">
   <si>
     <t>Arquivo</t>
   </si>
@@ -2403,6 +2403,9 @@
   </si>
   <si>
     <t>*</t>
+  </si>
+  <si>
+    <t>UDS/cfarl</t>
   </si>
 </sst>
 </file>
@@ -2467,7 +2470,17 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -2769,8 +2782,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:D781"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A303" workbookViewId="0">
-      <selection activeCell="D311" sqref="D311"/>
+    <sheetView tabSelected="1" topLeftCell="A612" workbookViewId="0">
+      <selection activeCell="D630" sqref="D630"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9683,10 +9696,10 @@
         <v>629</v>
       </c>
       <c r="C630" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D630" s="1" t="s">
-        <v>784</v>
+        <v>793</v>
       </c>
     </row>
     <row r="631" spans="2:4" x14ac:dyDescent="0.25">
@@ -11334,7 +11347,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>"SIM"</formula>
     </cfRule>
     <cfRule type="colorScale" priority="3">
@@ -11349,7 +11362,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="notContainsBlanks" dxfId="0" priority="4">
+    <cfRule type="notContainsBlanks" dxfId="1" priority="4">
       <formula>LEN(TRIM(D1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Traduzidos cfarl mgml_strings_us.u16 shp_jwl_str_us.u16 wrp_pnt_list_us.u16
</commit_message>
<xml_diff>
--- a/arquivos-tradutor.xlsx
+++ b/arquivos-tradutor.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\danger\traducoes\traducao-blue-dragon-xbox360\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2330" uniqueCount="794">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2337" uniqueCount="795">
   <si>
     <t>Arquivo</t>
   </si>
@@ -2406,6 +2401,9 @@
   </si>
   <si>
     <t>UDS/cfarl</t>
+  </si>
+  <si>
+    <t>sem texto</t>
   </si>
 </sst>
 </file>
@@ -2470,11 +2468,18 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="4">
     <dxf>
       <font>
         <color rgb="FF006100"/>
       </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
@@ -2772,7 +2777,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2782,8 +2787,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:D781"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A612" workbookViewId="0">
-      <selection activeCell="D630" sqref="D630"/>
+    <sheetView tabSelected="1" topLeftCell="A604" workbookViewId="0">
+      <selection activeCell="C615" sqref="C615:C617"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9540,7 +9545,10 @@
         <v>614</v>
       </c>
       <c r="C615" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
+      </c>
+      <c r="D615" s="1" t="s">
+        <v>794</v>
       </c>
     </row>
     <row r="616" spans="2:4" x14ac:dyDescent="0.25">
@@ -9548,7 +9556,10 @@
         <v>615</v>
       </c>
       <c r="C616" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
+      </c>
+      <c r="D616" s="1" t="s">
+        <v>794</v>
       </c>
     </row>
     <row r="617" spans="2:4" x14ac:dyDescent="0.25">
@@ -9556,7 +9567,10 @@
         <v>616</v>
       </c>
       <c r="C617" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
+      </c>
+      <c r="D617" s="1" t="s">
+        <v>794</v>
       </c>
     </row>
     <row r="618" spans="2:4" x14ac:dyDescent="0.25">
@@ -11115,7 +11129,10 @@
         <v>758</v>
       </c>
       <c r="C759" s="1" t="s">
-        <v>783</v>
+        <v>790</v>
+      </c>
+      <c r="D759" s="1" t="s">
+        <v>794</v>
       </c>
     </row>
     <row r="760" spans="2:4" x14ac:dyDescent="0.25">
@@ -11175,7 +11192,10 @@
         <v>764</v>
       </c>
       <c r="C765" s="1" t="s">
-        <v>783</v>
+        <v>790</v>
+      </c>
+      <c r="D765" s="1" t="s">
+        <v>789</v>
       </c>
     </row>
     <row r="766" spans="2:4" x14ac:dyDescent="0.25">
@@ -11205,7 +11225,10 @@
         <v>767</v>
       </c>
       <c r="C768" s="1" t="s">
-        <v>783</v>
+        <v>790</v>
+      </c>
+      <c r="D768" s="1" t="s">
+        <v>789</v>
       </c>
     </row>
     <row r="769" spans="2:4" x14ac:dyDescent="0.25">
@@ -11331,7 +11354,10 @@
         <v>779</v>
       </c>
       <c r="C780" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
+      </c>
+      <c r="D780" s="1" t="s">
+        <v>789</v>
       </c>
     </row>
     <row r="781" spans="2:4" x14ac:dyDescent="0.25">
@@ -11347,7 +11373,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
       <formula>"SIM"</formula>
     </cfRule>
     <cfRule type="colorScale" priority="3">
@@ -11362,7 +11388,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="notContainsBlanks" dxfId="1" priority="4">
+    <cfRule type="notContainsBlanks" dxfId="2" priority="4">
       <formula>LEN(TRIM(D1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Traduzido mgc_dic_us.u16 Atualizado glossario.xlsx
</commit_message>
<xml_diff>
--- a/arquivos-tradutor.xlsx
+++ b/arquivos-tradutor.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2341" uniqueCount="795">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2342" uniqueCount="795">
   <si>
     <t>Arquivo</t>
   </si>
@@ -2473,11 +2473,18 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="4">
     <dxf>
       <font>
         <color rgb="FF006100"/>
       </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
@@ -2785,8 +2792,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:D781"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A216" workbookViewId="0">
-      <selection activeCell="G232" sqref="G232"/>
+    <sheetView tabSelected="1" topLeftCell="A757" workbookViewId="0">
+      <selection activeCell="C761" sqref="C761:C762"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11169,7 +11176,10 @@
         <v>761</v>
       </c>
       <c r="C762" s="1" t="s">
-        <v>783</v>
+        <v>790</v>
+      </c>
+      <c r="D762" s="1" t="s">
+        <v>789</v>
       </c>
     </row>
     <row r="763" spans="2:4" x14ac:dyDescent="0.25">
@@ -11383,7 +11393,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
       <formula>"SIM"</formula>
     </cfRule>
     <cfRule type="colorScale" priority="3">
@@ -11398,7 +11408,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="notContainsBlanks" dxfId="1" priority="4">
+    <cfRule type="notContainsBlanks" dxfId="2" priority="4">
       <formula>LEN(TRIM(D1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
arquivos traduzidos mes_bg03_01_us.u16 mes_bg17_01_us.u16 mes_bg22_01_us.u16
</commit_message>
<xml_diff>
--- a/arquivos-tradutor.xlsx
+++ b/arquivos-tradutor.xlsx
@@ -2772,8 +2772,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:D781"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A756" workbookViewId="0">
-      <selection activeCell="C760" sqref="C760"/>
+    <sheetView tabSelected="1" topLeftCell="A629" workbookViewId="0">
+      <selection activeCell="C642" sqref="C642"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9616,7 +9616,7 @@
         <v>621</v>
       </c>
       <c r="C622" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D622" s="1" t="s">
         <v>784</v>
@@ -9748,7 +9748,7 @@
         <v>633</v>
       </c>
       <c r="C634" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D634" s="1" t="s">
         <v>784</v>
@@ -9781,7 +9781,7 @@
         <v>636</v>
       </c>
       <c r="C637" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D637" s="1" t="s">
         <v>784</v>

</xml_diff>

<commit_message>
Concluída a traducao do SkWd_new_us.u16
</commit_message>
<xml_diff>
--- a/arquivos-tradutor.xlsx
+++ b/arquivos-tradutor.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Moacyr\Desktop\GITHUB-BLUE DRAGON\traducao-blue-dragon-xbox360\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\danger\traducoes\traducao-blue-dragon-xbox360\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -2470,7 +2470,17 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -2772,8 +2782,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:D781"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A592" workbookViewId="0">
-      <selection activeCell="D613" sqref="D613"/>
+    <sheetView tabSelected="1" topLeftCell="A559" workbookViewId="0">
+      <selection activeCell="C772" sqref="C772:C773"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11280,7 +11290,7 @@
         <v>772</v>
       </c>
       <c r="C773" s="1" t="s">
-        <v>783</v>
+        <v>789</v>
       </c>
       <c r="D773" s="1" t="s">
         <v>788</v>
@@ -11376,7 +11386,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>"SIM"</formula>
     </cfRule>
     <cfRule type="colorScale" priority="3">
@@ -11391,7 +11401,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="notContainsBlanks" dxfId="0" priority="4">
+    <cfRule type="notContainsBlanks" dxfId="1" priority="4">
       <formula>LEN(TRIM(D1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>